<commit_message>
medio dia 25 agosto
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01 DOCUEMENTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="JARCERIAS REMODELACION " sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="71">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -268,6 +268,9 @@
   <si>
     <t>CAMBIAR LAMINAS TRANSPARENTES</t>
   </si>
+  <si>
+    <t xml:space="preserve">Transferencia </t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +282,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +390,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF990000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -739,7 +750,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -986,6 +997,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,36 +1036,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1094,6 +1105,7 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1103,11 +1115,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF990000"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF00FF99"/>
-      <color rgb="FF990000"/>
       <color rgb="FFAC7300"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
@@ -2956,18 +2968,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="128"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="134"/>
+      <c r="D4" s="129"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2977,10 +2989,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="130"/>
+      <c r="C6" s="140"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -2997,10 +3009,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="132"/>
+      <c r="C8" s="137"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3017,10 +3029,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="132"/>
+      <c r="C10" s="137"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3037,10 +3049,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="132"/>
+      <c r="C12" s="137"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3057,10 +3069,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="132"/>
+      <c r="C14" s="137"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3077,10 +3089,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="135" t="s">
+      <c r="B16" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="136"/>
+      <c r="C16" s="131"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3097,14 +3109,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="135" t="s">
+      <c r="B18" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="136"/>
+      <c r="C18" s="131"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="137" t="s">
+      <c r="E18" s="132" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3114,7 +3126,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="138"/>
+      <c r="E19" s="133"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3125,10 +3137,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="136"/>
+      <c r="C21" s="131"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3145,10 +3157,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="140"/>
+      <c r="C23" s="135"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3165,10 +3177,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="133" t="s">
+      <c r="B25" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="133"/>
+      <c r="C25" s="128"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3219,6 +3231,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3227,11 +3244,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3450,7 +3462,7 @@
   </sheetPr>
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -4753,8 +4765,8 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5067,16 +5079,18 @@
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="75"/>
-      <c r="C34" s="76"/>
+      <c r="C34" s="76">
+        <v>44415</v>
+      </c>
       <c r="D34" s="77">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="E34" s="27"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="75"/>
       <c r="C35" s="76">
-        <v>44415</v>
+        <v>44422</v>
       </c>
       <c r="D35" s="77">
         <v>100000</v>
@@ -5086,12 +5100,14 @@
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="75"/>
       <c r="C36" s="76">
-        <v>44422</v>
+        <v>44428</v>
       </c>
       <c r="D36" s="77">
-        <v>100000</v>
-      </c>
-      <c r="E36" s="27"/>
+        <v>300000</v>
+      </c>
+      <c r="E36" s="164" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="75"/>
@@ -5143,7 +5159,7 @@
       </c>
       <c r="D44" s="99">
         <f>SUM(D5:D43)</f>
-        <v>2450000</v>
+        <v>2750000</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5222,7 +5238,7 @@
       </c>
       <c r="D50" s="116">
         <f>D47+D44+D45+D46+D48+D49</f>
-        <v>-5042427.9600000009</v>
+        <v>-4742427.9600000009</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5241,6 +5257,9 @@
       <c r="C54" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="C34:D36">
+    <sortCondition ref="C34:C36"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G47:I48"/>

</xml_diff>

<commit_message>
cierre del 30 OCT-21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1000,6 +1000,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1007,36 +1037,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2970,18 +2970,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="131"/>
+      <c r="D3" s="141"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="137" t="s">
+      <c r="C4" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="137"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2991,10 +2991,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="133"/>
+      <c r="C6" s="143"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3011,10 +3011,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="135"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3031,10 +3031,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="135"/>
+      <c r="C10" s="140"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3051,10 +3051,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="135"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3071,10 +3071,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="135"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3091,10 +3091,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3111,14 +3111,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="140" t="s">
+      <c r="E18" s="135" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3128,7 +3128,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="141"/>
+      <c r="E19" s="136"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3139,10 +3139,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3159,10 +3159,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="143"/>
+      <c r="C23" s="138"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3179,10 +3179,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="136" t="s">
+      <c r="B25" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="136"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3233,6 +3233,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3241,11 +3246,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4768,7 +4768,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5215,9 +5215,11 @@
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="126"/>
-      <c r="C47" s="76"/>
+      <c r="C47" s="76">
+        <v>44499</v>
+      </c>
       <c r="D47" s="77">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E47" s="127"/>
     </row>
@@ -5307,7 +5309,7 @@
       </c>
       <c r="D58" s="99">
         <f>SUM(D5:D57)</f>
-        <v>3650000</v>
+        <v>3700000</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5386,7 +5388,7 @@
       </c>
       <c r="D64" s="116">
         <f>D61+D58+D59+D60+D62+D63</f>
-        <v>-3842427.9600000004</v>
+        <v>-3792427.9600000004</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 30  NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="JARCERIAS REMODELACION " sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t xml:space="preserve">Transferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bolier solar y tanque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALVULAS </t>
   </si>
 </sst>
 </file>
@@ -1000,6 +1006,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1007,36 +1043,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2970,18 +2976,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="131"/>
+      <c r="D3" s="141"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="137" t="s">
+      <c r="C4" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="137"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2991,10 +2997,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="133"/>
+      <c r="C6" s="143"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3011,10 +3017,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="135"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3031,10 +3037,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="135"/>
+      <c r="C10" s="140"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3051,10 +3057,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="135"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3071,10 +3077,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="135"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3091,10 +3097,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3111,14 +3117,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="140" t="s">
+      <c r="E18" s="135" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3128,7 +3134,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="141"/>
+      <c r="E19" s="136"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3139,10 +3145,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3159,10 +3165,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="143"/>
+      <c r="C23" s="138"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3179,10 +3185,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="136" t="s">
+      <c r="B25" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="136"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3233,6 +3239,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3241,11 +3252,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3464,8 +3470,8 @@
   </sheetPr>
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,12 +3540,18 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="36">
+        <v>44527</v>
+      </c>
       <c r="D8" s="37">
-        <v>0</v>
-      </c>
-      <c r="E8" s="27"/>
+        <v>2800</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="31"/>
@@ -3547,7 +3559,9 @@
       <c r="D9" s="37">
         <v>0</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="27" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="31"/>
@@ -3587,7 +3601,7 @@
       </c>
       <c r="D14" s="25">
         <f>SUM(D5:D13)</f>
-        <v>57227</v>
+        <v>60027</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -3614,7 +3628,7 @@
       </c>
       <c r="D18" s="34">
         <f>D14+D15+D16</f>
-        <v>57227</v>
+        <v>60027</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -4767,8 +4781,8 @@
   </sheetPr>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5255,9 +5269,11 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="126"/>
-      <c r="C51" s="76"/>
+      <c r="C51" s="76">
+        <v>44527</v>
+      </c>
       <c r="D51" s="77">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E51" s="127"/>
     </row>
@@ -5315,7 +5331,7 @@
       </c>
       <c r="D58" s="99">
         <f>SUM(D5:D57)</f>
-        <v>3850000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5394,7 +5410,7 @@
       </c>
       <c r="D64" s="116">
         <f>D61+D58+D59+D60+D62+D63</f>
-        <v>-3642427.96</v>
+        <v>-3592427.96</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 4 DE DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="JARCERIAS REMODELACION " sheetId="1" r:id="rId1"/>
@@ -1006,6 +1006,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1028,21 +1043,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2976,18 +2976,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="141"/>
+      <c r="D3" s="131"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="132"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2997,10 +2997,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="143"/>
+      <c r="C6" s="133"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3017,10 +3017,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="139" t="s">
+      <c r="B8" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="140"/>
+      <c r="C8" s="135"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3037,10 +3037,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="140"/>
+      <c r="C10" s="135"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3057,10 +3057,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="140"/>
+      <c r="C12" s="135"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3077,10 +3077,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="139" t="s">
+      <c r="B14" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="140"/>
+      <c r="C14" s="135"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3097,10 +3097,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="133" t="s">
+      <c r="B16" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="134"/>
+      <c r="C16" s="139"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3117,14 +3117,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="133" t="s">
+      <c r="B18" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="134"/>
+      <c r="C18" s="139"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="135" t="s">
+      <c r="E18" s="140" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3134,7 +3134,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="136"/>
+      <c r="E19" s="141"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3145,10 +3145,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="133" t="s">
+      <c r="B21" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="134"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3165,10 +3165,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="137" t="s">
+      <c r="B23" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="138"/>
+      <c r="C23" s="143"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3185,10 +3185,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="131" t="s">
+      <c r="B25" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="131"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3239,11 +3239,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3252,6 +3247,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3470,7 +3470,7 @@
   </sheetPr>
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -4781,8 +4781,8 @@
   </sheetPr>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5279,9 +5279,11 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="126"/>
-      <c r="C52" s="76"/>
+      <c r="C52" s="76">
+        <v>44534</v>
+      </c>
       <c r="D52" s="77">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E52" s="127"/>
     </row>
@@ -5331,7 +5333,7 @@
       </c>
       <c r="D58" s="99">
         <f>SUM(D5:D57)</f>
-        <v>3900000</v>
+        <v>3950000</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5410,7 +5412,7 @@
       </c>
       <c r="D64" s="116">
         <f>D61+D58+D59+D60+D62+D63</f>
-        <v>-3592427.96</v>
+        <v>-3542427.96</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 2 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="74">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -277,6 +277,9 @@
   <si>
     <t xml:space="preserve">VALVULAS </t>
   </si>
+  <si>
+    <t>Transferencia   NLP  PANELES</t>
+  </si>
 </sst>
 </file>
 
@@ -409,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +446,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1006,6 +1015,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1015,36 +1054,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1114,6 +1123,11 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1123,8 +1137,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FF990000"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF00FF99"/>
@@ -2976,18 +2990,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="131"/>
+      <c r="D3" s="141"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="137" t="s">
+      <c r="C4" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="137"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2997,10 +3011,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="133"/>
+      <c r="C6" s="143"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3017,10 +3031,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="135"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3037,10 +3051,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="135"/>
+      <c r="C10" s="140"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3057,10 +3071,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="135"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3077,10 +3091,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="135"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3097,10 +3111,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3117,14 +3131,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="140" t="s">
+      <c r="E18" s="135" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3134,7 +3148,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="141"/>
+      <c r="E19" s="136"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3145,10 +3159,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3165,10 +3179,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="143"/>
+      <c r="C23" s="138"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3185,10 +3199,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="136" t="s">
+      <c r="B25" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="136"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3239,6 +3253,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3247,11 +3266,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4781,8 +4795,8 @@
   </sheetPr>
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5369,11 +5383,15 @@
     </row>
     <row r="61" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="126"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="77">
-        <v>0</v>
-      </c>
-      <c r="E61" s="127"/>
+      <c r="C61" s="167">
+        <v>44594</v>
+      </c>
+      <c r="D61" s="168">
+        <v>500000</v>
+      </c>
+      <c r="E61" s="169" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="62" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="126"/>
@@ -5413,7 +5431,7 @@
       </c>
       <c r="D66" s="99">
         <f>SUM(D5:D65)</f>
-        <v>4470000</v>
+        <v>4970000</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5492,7 +5510,7 @@
       </c>
       <c r="D72" s="116">
         <f>D69+D66+D67+D68+D70+D71</f>
-        <v>-3022427.96</v>
+        <v>-2522427.96</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE  14 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1020,6 +1020,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,36 +1057,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1595,13 +1595,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>428624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2990,18 +2990,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="134"/>
+      <c r="D3" s="144"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="140"/>
+      <c r="D4" s="135"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3011,10 +3011,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="136"/>
+      <c r="C6" s="146"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3031,10 +3031,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="138"/>
+      <c r="C8" s="143"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3051,10 +3051,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="138"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3071,10 +3071,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="137" t="s">
+      <c r="B12" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="138"/>
+      <c r="C12" s="143"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3091,10 +3091,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="138"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3111,10 +3111,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="142"/>
+      <c r="C16" s="137"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3131,14 +3131,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="141" t="s">
+      <c r="B18" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="142"/>
+      <c r="C18" s="137"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="143" t="s">
+      <c r="E18" s="138" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3148,7 +3148,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="144"/>
+      <c r="E19" s="139"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3159,10 +3159,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="142"/>
+      <c r="C21" s="137"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3179,10 +3179,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="146"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3199,10 +3199,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="139"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3253,6 +3253,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3261,11 +3266,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4793,10 +4793,10 @@
   <sheetPr>
     <tabColor rgb="FF00FF99"/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5405,130 +5405,194 @@
     </row>
     <row r="63" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="126"/>
-      <c r="C63" s="76"/>
+      <c r="C63" s="76">
+        <v>44604</v>
+      </c>
       <c r="D63" s="77">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="E63" s="127"/>
     </row>
     <row r="64" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="126"/>
       <c r="C64" s="76"/>
-      <c r="D64" s="77">
-        <v>0</v>
-      </c>
+      <c r="D64" s="77"/>
       <c r="E64" s="127"/>
     </row>
-    <row r="65" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="95"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="97">
-        <v>0</v>
-      </c>
-      <c r="E65" s="95"/>
-    </row>
-    <row r="66" spans="1:9" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="98" t="s">
+    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="126"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="127"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="126"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="127"/>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="126"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="127"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="126"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="77"/>
+      <c r="E68" s="127"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="126"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="77"/>
+      <c r="E69" s="127"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="126"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="77"/>
+      <c r="E70" s="127"/>
+    </row>
+    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="126"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="77"/>
+      <c r="E71" s="127"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="126"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="77"/>
+      <c r="E72" s="127"/>
+    </row>
+    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="126"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="77">
+        <v>0</v>
+      </c>
+      <c r="E73" s="127"/>
+    </row>
+    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="126"/>
+      <c r="C74" s="76"/>
+      <c r="D74" s="77">
+        <v>0</v>
+      </c>
+      <c r="E74" s="127"/>
+    </row>
+    <row r="75" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="95"/>
+      <c r="C75" s="96"/>
+      <c r="D75" s="97">
+        <v>0</v>
+      </c>
+      <c r="E75" s="95"/>
+    </row>
+    <row r="76" spans="1:9" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C76" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="99">
-        <f>SUM(D5:D65)</f>
-        <v>5070000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="106"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="108" t="s">
+      <c r="D76" s="99">
+        <f>SUM(D5:D75)</f>
+        <v>5170000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="106"/>
+      <c r="B77" s="107"/>
+      <c r="C77" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="109">
+      <c r="D77" s="109">
         <v>-3644591.85</v>
       </c>
-      <c r="E67" s="102">
+      <c r="E77" s="102">
         <v>44264</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="110"/>
-      <c r="B68" s="103"/>
-      <c r="C68" s="104" t="s">
+    <row r="78" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="110"/>
+      <c r="B78" s="103"/>
+      <c r="C78" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="D68" s="105">
+      <c r="D78" s="105">
         <v>-1303474.18</v>
       </c>
-      <c r="E68" s="100">
+      <c r="E78" s="100">
         <v>44264</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="110"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="104" t="s">
+    <row r="79" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="110"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="D69" s="105">
+      <c r="D79" s="105">
         <v>-937943.41</v>
       </c>
-      <c r="E69" s="100">
+      <c r="E79" s="100">
         <v>44264</v>
       </c>
-      <c r="G69" s="159">
-        <f>D67+D68+D69+D70</f>
+      <c r="G79" s="159">
+        <f>D77+D78+D79+D80</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H69" s="160"/>
-      <c r="I69" s="161"/>
-    </row>
-    <row r="70" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="110"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="104" t="s">
+      <c r="H79" s="160"/>
+      <c r="I79" s="161"/>
+    </row>
+    <row r="80" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="110"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="D70" s="105">
+      <c r="D80" s="105">
         <v>-1606418.52</v>
       </c>
-      <c r="E70" s="100">
+      <c r="E80" s="100">
         <v>44264</v>
       </c>
-      <c r="G70" s="162"/>
-      <c r="H70" s="163"/>
-      <c r="I70" s="164"/>
-    </row>
-    <row r="71" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="111"/>
-      <c r="B71" s="112"/>
-      <c r="C71" s="113"/>
-      <c r="D71" s="114">
-        <v>0</v>
-      </c>
-      <c r="E71" s="101"/>
-    </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="115" t="s">
+      <c r="G80" s="162"/>
+      <c r="H80" s="163"/>
+      <c r="I80" s="164"/>
+    </row>
+    <row r="81" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="111"/>
+      <c r="B81" s="112"/>
+      <c r="C81" s="113"/>
+      <c r="D81" s="114">
+        <v>0</v>
+      </c>
+      <c r="E81" s="101"/>
+    </row>
+    <row r="82" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="116">
-        <f>D69+D66+D67+D68+D70+D71</f>
-        <v>-2422427.96</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C73" s="1"/>
-      <c r="D73" s="2" t="s">
+      <c r="D82" s="116">
+        <f>D79+D76+D77+D78+D80+D81</f>
+        <v>-2322427.96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="1"/>
+      <c r="D83" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C76" s="1"/>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C86" s="1"/>
     </row>
   </sheetData>
   <sortState ref="C34:D36">
@@ -5536,7 +5600,7 @@
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G69:I70"/>
+    <mergeCell ref="G79:I80"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.13" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 8 ABR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="JARCERIAS REMODELACION " sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t xml:space="preserve">PAGOS  SOBRE </t>
+  </si>
+  <si>
+    <t>Transferencia PANELES</t>
   </si>
 </sst>
 </file>
@@ -1027,6 +1030,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1049,21 +1067,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1144,9 +1147,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF9933"/>
       <color rgb="FFAC7300"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF990000"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FF00FFFF"/>
@@ -3103,18 +3106,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="134"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="135"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3124,10 +3127,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="146"/>
+      <c r="C6" s="136"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3144,10 +3147,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="143"/>
+      <c r="C8" s="138"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3164,10 +3167,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="143"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3184,10 +3187,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="138"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3204,10 +3207,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="143"/>
+      <c r="C14" s="138"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3224,10 +3227,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="137"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3244,14 +3247,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="137"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="138" t="s">
+      <c r="E18" s="143" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3261,7 +3264,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="139"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3272,10 +3275,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="137"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3292,10 +3295,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="141"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3312,10 +3315,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="134" t="s">
+      <c r="B25" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="134"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3366,11 +3369,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3379,6 +3377,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4908,8 +4911,8 @@
   </sheetPr>
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5598,9 +5601,15 @@
     </row>
     <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="126"/>
-      <c r="C71" s="76"/>
-      <c r="D71" s="77"/>
-      <c r="E71" s="127"/>
+      <c r="C71" s="76">
+        <v>44659</v>
+      </c>
+      <c r="D71" s="77">
+        <v>350000</v>
+      </c>
+      <c r="E71" s="130" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="126"/>
@@ -5638,7 +5647,7 @@
       </c>
       <c r="D76" s="99">
         <f>SUM(D5:D75)</f>
-        <v>5870000</v>
+        <v>6220000</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5717,7 +5726,7 @@
       </c>
       <c r="D82" s="116">
         <f>D79+D76+D77+D78+D80+D81</f>
-        <v>-1622427.9600000002</v>
+        <v>-1272427.9600000002</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -6189,7 +6198,7 @@
   </sheetPr>
   <dimension ref="B1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 13 ABRIL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="78">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -290,6 +290,9 @@
   <si>
     <t>Transferencia PANELES</t>
   </si>
+  <si>
+    <t>DRENAJE</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +304,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +419,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF990000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color rgb="FF990000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -775,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1030,6 +1041,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,21 +1080,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1138,6 +1149,7 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1147,10 +1159,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF990000"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFFF9933"/>
       <color rgb="FFAC7300"/>
-      <color rgb="FF990000"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF00FF99"/>
@@ -3106,18 +3118,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="134"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="135"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3127,10 +3139,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="146"/>
+      <c r="C6" s="136"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3147,10 +3159,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="143"/>
+      <c r="C8" s="138"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3167,10 +3179,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="143"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3187,10 +3199,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="138"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3207,10 +3219,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="143"/>
+      <c r="C14" s="138"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3227,10 +3239,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="137"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3247,14 +3259,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="137"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="138" t="s">
+      <c r="E18" s="143" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3264,7 +3276,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="139"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3275,10 +3287,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="137"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3295,10 +3307,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="141"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3315,10 +3327,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="134" t="s">
+      <c r="B25" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="134"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3369,11 +3381,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3382,6 +3389,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4912,7 +4924,7 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5621,13 +5633,17 @@
       </c>
       <c r="E72" s="127"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B73" s="126"/>
-      <c r="C73" s="76"/>
+      <c r="C73" s="76">
+        <v>44663</v>
+      </c>
       <c r="D73" s="77">
-        <v>0</v>
-      </c>
-      <c r="E73" s="127"/>
+        <v>100000</v>
+      </c>
+      <c r="E73" s="170" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="126"/>
@@ -5651,7 +5667,7 @@
       </c>
       <c r="D76" s="99">
         <f>SUM(D5:D75)</f>
-        <v>6320000</v>
+        <v>6420000</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5730,7 +5746,7 @@
       </c>
       <c r="D82" s="116">
         <f>D79+D76+D77+D78+D80+D81</f>
-        <v>-1172427.9600000002</v>
+        <v>-1072427.9600000002</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cierre 7 may 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1042,6 +1042,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1049,36 +1079,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3118,18 +3118,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="135"/>
+      <c r="D3" s="145"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="141"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3139,10 +3139,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="137"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3159,10 +3159,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="138" t="s">
+      <c r="B8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="139"/>
+      <c r="C8" s="144"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3179,10 +3179,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="139"/>
+      <c r="C10" s="144"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3199,10 +3199,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="139"/>
+      <c r="C12" s="144"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3219,10 +3219,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="139"/>
+      <c r="C14" s="144"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3239,10 +3239,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="143"/>
+      <c r="C16" s="138"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3259,14 +3259,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="137" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="143"/>
+      <c r="C18" s="138"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="144" t="s">
+      <c r="E18" s="139" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3276,7 +3276,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="140"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3287,10 +3287,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="143"/>
+      <c r="C21" s="138"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3307,10 +3307,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="146" t="s">
+      <c r="B23" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="147"/>
+      <c r="C23" s="142"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3327,10 +3327,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="140" t="s">
+      <c r="B25" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="140"/>
+      <c r="C25" s="135"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3381,6 +3381,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3389,11 +3394,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4923,7 +4923,7 @@
   </sheetPr>
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
       <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 18 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="79">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>DRENAJE</t>
+  </si>
+  <si>
+    <t>TRANSFORMADOR</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1042,6 +1045,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1051,36 +1084,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1149,6 +1152,9 @@
     </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3118,18 +3124,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="135"/>
+      <c r="D3" s="145"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="141"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3139,10 +3145,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="137"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3159,10 +3165,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="138" t="s">
+      <c r="B8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="139"/>
+      <c r="C8" s="144"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3179,10 +3185,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="139"/>
+      <c r="C10" s="144"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3199,10 +3205,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="139"/>
+      <c r="C12" s="144"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3219,10 +3225,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="139"/>
+      <c r="C14" s="144"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3239,10 +3245,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="143"/>
+      <c r="C16" s="138"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3259,14 +3265,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="137" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="143"/>
+      <c r="C18" s="138"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="144" t="s">
+      <c r="E18" s="139" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3276,7 +3282,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="140"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3287,10 +3293,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="143"/>
+      <c r="C21" s="138"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3307,10 +3313,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="146" t="s">
+      <c r="B23" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="147"/>
+      <c r="C23" s="142"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3327,10 +3333,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="140" t="s">
+      <c r="B25" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="140"/>
+      <c r="C25" s="135"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3381,6 +3387,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3389,11 +3400,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4923,8 +4929,8 @@
   </sheetPr>
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5688,17 +5694,23 @@
     <row r="78" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="126"/>
       <c r="C78" s="76">
-        <v>44756</v>
+        <v>44690</v>
       </c>
       <c r="D78" s="77">
-        <v>100000</v>
-      </c>
-      <c r="E78" s="127"/>
+        <v>400000</v>
+      </c>
+      <c r="E78" s="171" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="79" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="126"/>
-      <c r="C79" s="76"/>
-      <c r="D79" s="77"/>
+      <c r="C79" s="76">
+        <v>44695</v>
+      </c>
+      <c r="D79" s="77">
+        <v>100000</v>
+      </c>
       <c r="E79" s="127"/>
     </row>
     <row r="80" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5721,7 +5733,7 @@
       </c>
       <c r="D82" s="99">
         <f>SUM(D5:D81)</f>
-        <v>6920000</v>
+        <v>7320000</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5800,7 +5812,7 @@
       </c>
       <c r="D88" s="116">
         <f>D85+D82+D83+D84+D86+D87</f>
-        <v>-572427.9600000002</v>
+        <v>-172427.9600000002</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 6 jUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18375" windowHeight="13620" firstSheet="18" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="JARCERIAS REMODELACION " sheetId="1" r:id="rId1"/>
@@ -1090,6 +1090,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1099,6 +1100,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1108,36 +1139,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1222,7 +1223,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2583,17 +2583,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="135" t="s">
+      <c r="I3" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="138"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3033,11 +3033,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3191,18 +3191,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="138"/>
+      <c r="D3" s="149"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="144"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3212,10 +3212,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="140"/>
+      <c r="C6" s="151"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3232,10 +3232,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="142"/>
+      <c r="C8" s="148"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3252,10 +3252,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="142"/>
+      <c r="C10" s="148"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3272,10 +3272,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="141" t="s">
+      <c r="B12" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="148"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3292,10 +3292,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="141" t="s">
+      <c r="B14" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="142"/>
+      <c r="C14" s="148"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3312,10 +3312,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="145" t="s">
+      <c r="B16" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="146"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3332,14 +3332,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="145" t="s">
+      <c r="B18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="146"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="147" t="s">
+      <c r="E18" s="143" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="148"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3360,10 +3360,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="146"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3380,10 +3380,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="150"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3400,10 +3400,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="143"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3454,6 +3454,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3462,11 +3467,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3505,11 +3505,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3710,11 +3710,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3899,11 +3899,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4107,9 +4107,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4340,9 +4340,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4700,36 +4700,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="152" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="152"/>
-      <c r="D57" s="152"/>
-      <c r="E57" s="153"/>
+      <c r="C57" s="153"/>
+      <c r="D57" s="153"/>
+      <c r="E57" s="154"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="154"/>
-      <c r="C58" s="155"/>
-      <c r="D58" s="155"/>
-      <c r="E58" s="156"/>
+      <c r="B58" s="155"/>
+      <c r="C58" s="156"/>
+      <c r="D58" s="156"/>
+      <c r="E58" s="157"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="154"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="155"/>
-      <c r="E59" s="156"/>
+      <c r="B59" s="155"/>
+      <c r="C59" s="156"/>
+      <c r="D59" s="156"/>
+      <c r="E59" s="157"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="154"/>
-      <c r="C60" s="155"/>
-      <c r="D60" s="155"/>
-      <c r="E60" s="156"/>
+      <c r="B60" s="155"/>
+      <c r="C60" s="156"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="157"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="157"/>
-      <c r="C61" s="158"/>
-      <c r="D61" s="158"/>
-      <c r="E61" s="159"/>
+      <c r="B61" s="158"/>
+      <c r="C61" s="159"/>
+      <c r="D61" s="159"/>
+      <c r="E61" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4774,9 +4774,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4996,7 +4996,7 @@
   </sheetPr>
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
@@ -5019,12 +5019,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="163"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
@@ -5808,7 +5808,7 @@
       <c r="D82" s="77">
         <v>300000</v>
       </c>
-      <c r="E82" s="179" t="s">
+      <c r="E82" s="135" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5893,12 +5893,12 @@
       <c r="E90" s="100">
         <v>44264</v>
       </c>
-      <c r="G90" s="163">
+      <c r="G90" s="164">
         <f>D88+D89+D90+D91</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H90" s="164"/>
-      <c r="I90" s="165"/>
+      <c r="H90" s="165"/>
+      <c r="I90" s="166"/>
     </row>
     <row r="91" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="110"/>
@@ -5912,9 +5912,9 @@
       <c r="E91" s="100">
         <v>44264</v>
       </c>
-      <c r="G91" s="166"/>
-      <c r="H91" s="167"/>
-      <c r="I91" s="168"/>
+      <c r="G91" s="167"/>
+      <c r="H91" s="168"/>
+      <c r="I91" s="169"/>
     </row>
     <row r="92" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="111"/>
@@ -6141,8 +6141,8 @@
   </sheetPr>
   <dimension ref="B1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6155,23 +6155,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="172" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="175"/>
+      <c r="D2" s="176"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="172"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="173"/>
+      <c r="B4" s="174"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6209,13 +6209,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6408,7 +6408,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="177" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6418,13 +6418,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="177"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="177"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6432,7 +6432,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="177"/>
+      <c r="B5" s="178"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6442,7 +6442,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="178"/>
+      <c r="B6" s="179"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6458,7 +6458,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169" t="s">
+      <c r="B8" s="170" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6470,7 +6470,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6670,7 +6670,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="177" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6680,13 +6680,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="177"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="177"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6694,7 +6694,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="177"/>
+      <c r="B5" s="178"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -6704,7 +6704,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="178"/>
+      <c r="B6" s="179"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -6720,7 +6720,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -6728,7 +6728,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>

</xml_diff>

<commit_message>
cierre 13 Jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1098,6 +1098,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1107,6 +1108,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1116,36 +1147,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1230,7 +1231,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2591,17 +2591,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="135" t="s">
+      <c r="I3" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="138"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3041,11 +3041,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3199,18 +3199,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="138"/>
+      <c r="D3" s="149"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="144"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3220,10 +3220,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="140"/>
+      <c r="C6" s="151"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3240,10 +3240,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="142"/>
+      <c r="C8" s="148"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3260,10 +3260,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="142"/>
+      <c r="C10" s="148"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3280,10 +3280,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="141" t="s">
+      <c r="B12" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="148"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3300,10 +3300,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="141" t="s">
+      <c r="B14" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="142"/>
+      <c r="C14" s="148"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3320,10 +3320,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="145" t="s">
+      <c r="B16" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="146"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3340,14 +3340,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="145" t="s">
+      <c r="B18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="146"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="147" t="s">
+      <c r="E18" s="143" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="148"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3368,10 +3368,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="146"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3388,10 +3388,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="150"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3408,10 +3408,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="143"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3462,6 +3462,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3470,11 +3475,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3513,11 +3513,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3718,11 +3718,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3907,11 +3907,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4115,9 +4115,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4348,9 +4348,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4708,36 +4708,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="152" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="152"/>
-      <c r="D57" s="152"/>
-      <c r="E57" s="153"/>
+      <c r="C57" s="153"/>
+      <c r="D57" s="153"/>
+      <c r="E57" s="154"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="154"/>
-      <c r="C58" s="155"/>
-      <c r="D58" s="155"/>
-      <c r="E58" s="156"/>
+      <c r="B58" s="155"/>
+      <c r="C58" s="156"/>
+      <c r="D58" s="156"/>
+      <c r="E58" s="157"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="154"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="155"/>
-      <c r="E59" s="156"/>
+      <c r="B59" s="155"/>
+      <c r="C59" s="156"/>
+      <c r="D59" s="156"/>
+      <c r="E59" s="157"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="154"/>
-      <c r="C60" s="155"/>
-      <c r="D60" s="155"/>
-      <c r="E60" s="156"/>
+      <c r="B60" s="155"/>
+      <c r="C60" s="156"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="157"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="157"/>
-      <c r="C61" s="158"/>
-      <c r="D61" s="158"/>
-      <c r="E61" s="159"/>
+      <c r="B61" s="158"/>
+      <c r="C61" s="159"/>
+      <c r="D61" s="159"/>
+      <c r="E61" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4782,9 +4782,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -5027,12 +5027,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="163"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
@@ -5816,7 +5816,7 @@
       <c r="D82" s="77">
         <v>300000</v>
       </c>
-      <c r="E82" s="179" t="s">
+      <c r="E82" s="135" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5933,12 +5933,12 @@
       <c r="E94" s="100">
         <v>44264</v>
       </c>
-      <c r="G94" s="163">
+      <c r="G94" s="164">
         <f>D92+D93+D94+D95</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H94" s="164"/>
-      <c r="I94" s="165"/>
+      <c r="H94" s="165"/>
+      <c r="I94" s="166"/>
     </row>
     <row r="95" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="110"/>
@@ -5952,9 +5952,9 @@
       <c r="E95" s="100">
         <v>44264</v>
       </c>
-      <c r="G95" s="166"/>
-      <c r="H95" s="167"/>
-      <c r="I95" s="168"/>
+      <c r="G95" s="167"/>
+      <c r="H95" s="168"/>
+      <c r="I95" s="169"/>
     </row>
     <row r="96" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="111"/>
@@ -6195,23 +6195,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="172" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="175"/>
+      <c r="D2" s="176"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="172"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="173"/>
+      <c r="B4" s="174"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6249,13 +6249,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6448,7 +6448,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="177" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6458,13 +6458,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="177"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="177"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6472,7 +6472,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="177"/>
+      <c r="B5" s="178"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6482,7 +6482,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="178"/>
+      <c r="B6" s="179"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6498,7 +6498,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169" t="s">
+      <c r="B8" s="170" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6510,7 +6510,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6710,7 +6710,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="177" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6720,13 +6720,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="177"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="177"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6734,7 +6734,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="177"/>
+      <c r="B5" s="178"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -6744,7 +6744,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="178"/>
+      <c r="B6" s="179"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -6760,7 +6760,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="169"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -6768,7 +6768,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>

</xml_diff>

<commit_message>
CIERRE 15 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="82">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t xml:space="preserve">PAGOS  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AISLANTE TERMICO PISOS </t>
   </si>
 </sst>
 </file>
@@ -1108,6 +1111,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1130,21 +1148,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3199,18 +3202,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="149"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="140"/>
+      <c r="D4" s="145"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3220,10 +3223,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="150" t="s">
+      <c r="B6" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="151"/>
+      <c r="C6" s="141"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3240,10 +3243,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="148"/>
+      <c r="C8" s="143"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3260,10 +3263,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="148"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3280,10 +3283,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="148"/>
+      <c r="C12" s="143"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3300,10 +3303,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="148"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3320,10 +3323,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="146" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="142"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3340,14 +3343,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="141" t="s">
+      <c r="B18" s="146" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="142"/>
+      <c r="C18" s="147"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="143" t="s">
+      <c r="E18" s="148" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3357,7 +3360,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="144"/>
+      <c r="E19" s="149"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3368,10 +3371,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="142"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3388,10 +3391,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="146"/>
+      <c r="C23" s="151"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3408,10 +3411,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="139"/>
+      <c r="C25" s="144"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3462,11 +3465,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3475,6 +3473,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5005,7 +5008,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5817,7 +5820,7 @@
         <v>300000</v>
       </c>
       <c r="E82" s="135" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cierre 20 jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1111,6 +1111,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1120,36 +1150,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1234,6 +1234,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3202,18 +3203,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="139" t="s">
+      <c r="C3" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="139"/>
+      <c r="D3" s="149"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="145"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3223,10 +3224,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="141"/>
+      <c r="C6" s="151"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3243,10 +3244,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="143"/>
+      <c r="C8" s="148"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3263,10 +3264,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="143"/>
+      <c r="C10" s="148"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3283,10 +3284,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="148"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3303,10 +3304,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="143"/>
+      <c r="C14" s="148"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3323,10 +3324,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="147"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3343,14 +3344,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="147"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="148" t="s">
+      <c r="E18" s="143" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3360,7 +3361,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="149"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3371,10 +3372,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="146" t="s">
+      <c r="B21" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="147"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3391,10 +3392,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="150" t="s">
+      <c r="B23" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="151"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3411,10 +3412,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="144" t="s">
+      <c r="B25" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="144"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3465,6 +3466,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3473,11 +3479,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5007,8 +5008,8 @@
   </sheetPr>
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5806,7 +5807,7 @@
       <c r="C81" s="76">
         <v>44709</v>
       </c>
-      <c r="D81" s="77">
+      <c r="D81" s="180">
         <v>200000</v>
       </c>
       <c r="E81" s="127"/>
@@ -5828,7 +5829,7 @@
       <c r="C83" s="76">
         <v>44716</v>
       </c>
-      <c r="D83" s="77">
+      <c r="D83" s="180">
         <v>150000</v>
       </c>
       <c r="E83" s="127"/>
@@ -5838,7 +5839,7 @@
       <c r="C84" s="76">
         <v>44716</v>
       </c>
-      <c r="D84" s="77">
+      <c r="D84" s="180">
         <v>50000</v>
       </c>
       <c r="E84" s="127"/>
@@ -5848,7 +5849,7 @@
       <c r="C85" s="76">
         <v>44723</v>
       </c>
-      <c r="D85" s="77">
+      <c r="D85" s="180">
         <v>150000</v>
       </c>
       <c r="E85" s="127"/>
@@ -5858,15 +5859,19 @@
       <c r="C86" s="76">
         <v>44723</v>
       </c>
-      <c r="D86" s="77">
+      <c r="D86" s="180">
         <v>50000</v>
       </c>
       <c r="E86" s="127"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B87" s="126"/>
-      <c r="C87" s="76"/>
-      <c r="D87" s="77"/>
+      <c r="C87" s="76">
+        <v>44730</v>
+      </c>
+      <c r="D87" s="77">
+        <v>100000</v>
+      </c>
       <c r="E87" s="127"/>
     </row>
     <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -5895,7 +5900,7 @@
       </c>
       <c r="D91" s="99">
         <f>SUM(D5:D90)</f>
-        <v>8320000</v>
+        <v>8420000</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5974,7 +5979,7 @@
       </c>
       <c r="D97" s="116">
         <f>D94+D91+D92+D93+D95+D96</f>
-        <v>827572.03999999957</v>
+        <v>927572.03999999957</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 24 JUN 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1102,6 +1102,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1111,6 +1112,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1135,21 +1151,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1234,7 +1235,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2595,17 +2595,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="136" t="s">
+      <c r="I3" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="137"/>
-      <c r="K3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3045,11 +3045,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3203,18 +3203,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="149"/>
+      <c r="D3" s="140"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="140"/>
+      <c r="D4" s="146"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3224,10 +3224,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="150" t="s">
+      <c r="B6" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="151"/>
+      <c r="C6" s="142"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3244,10 +3244,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="148"/>
+      <c r="C8" s="144"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3264,10 +3264,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="148"/>
+      <c r="C10" s="144"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3284,10 +3284,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="148"/>
+      <c r="C12" s="144"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3304,10 +3304,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="148"/>
+      <c r="C14" s="144"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3324,10 +3324,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="142"/>
+      <c r="C16" s="148"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3344,14 +3344,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="141" t="s">
+      <c r="B18" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="142"/>
+      <c r="C18" s="148"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="143" t="s">
+      <c r="E18" s="149" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3361,7 +3361,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="144"/>
+      <c r="E19" s="150"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3372,10 +3372,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="142"/>
+      <c r="C21" s="148"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3392,10 +3392,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="146"/>
+      <c r="C23" s="152"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3412,10 +3412,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="139"/>
+      <c r="C25" s="145"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3466,11 +3466,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3479,6 +3474,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3517,11 +3517,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3722,11 +3722,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3911,11 +3911,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4119,9 +4119,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4352,9 +4352,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4712,36 +4712,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="152" t="s">
+      <c r="B57" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="153"/>
-      <c r="D57" s="153"/>
-      <c r="E57" s="154"/>
+      <c r="C57" s="154"/>
+      <c r="D57" s="154"/>
+      <c r="E57" s="155"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="155"/>
-      <c r="C58" s="156"/>
-      <c r="D58" s="156"/>
-      <c r="E58" s="157"/>
+      <c r="B58" s="156"/>
+      <c r="C58" s="157"/>
+      <c r="D58" s="157"/>
+      <c r="E58" s="158"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="155"/>
-      <c r="C59" s="156"/>
-      <c r="D59" s="156"/>
-      <c r="E59" s="157"/>
+      <c r="B59" s="156"/>
+      <c r="C59" s="157"/>
+      <c r="D59" s="157"/>
+      <c r="E59" s="158"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="155"/>
-      <c r="C60" s="156"/>
-      <c r="D60" s="156"/>
-      <c r="E60" s="157"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="157"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="158"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="158"/>
-      <c r="C61" s="159"/>
-      <c r="D61" s="159"/>
-      <c r="E61" s="160"/>
+      <c r="B61" s="159"/>
+      <c r="C61" s="160"/>
+      <c r="D61" s="160"/>
+      <c r="E61" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4786,9 +4786,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -5009,7 +5009,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5031,12 +5031,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="164"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
@@ -5807,7 +5807,7 @@
       <c r="C81" s="76">
         <v>44709</v>
       </c>
-      <c r="D81" s="180">
+      <c r="D81" s="136">
         <v>200000</v>
       </c>
       <c r="E81" s="127"/>
@@ -5829,7 +5829,7 @@
       <c r="C83" s="76">
         <v>44716</v>
       </c>
-      <c r="D83" s="180">
+      <c r="D83" s="136">
         <v>150000</v>
       </c>
       <c r="E83" s="127"/>
@@ -5839,7 +5839,7 @@
       <c r="C84" s="76">
         <v>44716</v>
       </c>
-      <c r="D84" s="180">
+      <c r="D84" s="136">
         <v>50000</v>
       </c>
       <c r="E84" s="127"/>
@@ -5849,7 +5849,7 @@
       <c r="C85" s="76">
         <v>44723</v>
       </c>
-      <c r="D85" s="180">
+      <c r="D85" s="136">
         <v>150000</v>
       </c>
       <c r="E85" s="127"/>
@@ -5859,7 +5859,7 @@
       <c r="C86" s="76">
         <v>44723</v>
       </c>
-      <c r="D86" s="180">
+      <c r="D86" s="136">
         <v>50000</v>
       </c>
       <c r="E86" s="127"/>
@@ -5876,8 +5876,12 @@
     </row>
     <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B88" s="126"/>
-      <c r="C88" s="76"/>
-      <c r="D88" s="77"/>
+      <c r="C88" s="76">
+        <v>44736</v>
+      </c>
+      <c r="D88" s="77">
+        <v>100000</v>
+      </c>
       <c r="E88" s="127"/>
     </row>
     <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -5900,7 +5904,7 @@
       </c>
       <c r="D91" s="99">
         <f>SUM(D5:D90)</f>
-        <v>8420000</v>
+        <v>8520000</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5941,12 +5945,12 @@
       <c r="E94" s="100">
         <v>44264</v>
       </c>
-      <c r="G94" s="164">
+      <c r="G94" s="165">
         <f>D92+D93+D94+D95</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H94" s="165"/>
-      <c r="I94" s="166"/>
+      <c r="H94" s="166"/>
+      <c r="I94" s="167"/>
     </row>
     <row r="95" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="110"/>
@@ -5960,9 +5964,9 @@
       <c r="E95" s="100">
         <v>44264</v>
       </c>
-      <c r="G95" s="167"/>
-      <c r="H95" s="168"/>
-      <c r="I95" s="169"/>
+      <c r="G95" s="168"/>
+      <c r="H95" s="169"/>
+      <c r="I95" s="170"/>
     </row>
     <row r="96" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="111"/>
@@ -5979,7 +5983,7 @@
       </c>
       <c r="D97" s="116">
         <f>D94+D91+D92+D93+D95+D96</f>
-        <v>927572.03999999957</v>
+        <v>1027572.0399999996</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.25">
@@ -6203,23 +6207,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="173" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="176"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="173"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="174"/>
+      <c r="B4" s="175"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6257,13 +6261,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="170"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="171"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6456,7 +6460,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="178" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6466,13 +6470,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="178"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="178"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6480,7 +6484,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="178"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6490,7 +6494,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="179"/>
+      <c r="B6" s="180"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6506,7 +6510,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="170" t="s">
+      <c r="B8" s="171" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6518,7 +6522,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="171"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6718,7 +6722,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="178" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6728,13 +6732,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="178"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="178"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6742,7 +6746,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="178"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -6752,7 +6756,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="179"/>
+      <c r="B6" s="180"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -6768,7 +6772,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="170"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -6776,7 +6780,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="171"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>

</xml_diff>

<commit_message>
cierre 27 jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,6 +1112,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1121,36 +1151,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1235,6 +1235,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1702,15 +1703,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>428624</xdr:rowOff>
+      <xdr:rowOff>400049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1725,8 +1726,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4867275" y="5305424"/>
-          <a:ext cx="1581150" cy="1781175"/>
+          <a:off x="4857750" y="16697324"/>
+          <a:ext cx="1581150" cy="2286000"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst/>
@@ -3203,18 +3204,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="140" t="s">
+      <c r="C3" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="140"/>
+      <c r="D3" s="150"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="146"/>
+      <c r="D4" s="141"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3224,10 +3225,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="142"/>
+      <c r="C6" s="152"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3244,10 +3245,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="144"/>
+      <c r="C8" s="149"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3264,10 +3265,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="143" t="s">
+      <c r="B10" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="144"/>
+      <c r="C10" s="149"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3284,10 +3285,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="144"/>
+      <c r="C12" s="149"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3304,10 +3305,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="144"/>
+      <c r="C14" s="149"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3324,10 +3325,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="148"/>
+      <c r="C16" s="143"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3344,14 +3345,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="147" t="s">
+      <c r="B18" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="148"/>
+      <c r="C18" s="143"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="149" t="s">
+      <c r="E18" s="144" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3361,7 +3362,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="150"/>
+      <c r="E19" s="145"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3372,10 +3373,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="147" t="s">
+      <c r="B21" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="148"/>
+      <c r="C21" s="143"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3392,10 +3393,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="146" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="152"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3412,10 +3413,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="145"/>
+      <c r="C25" s="140"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3466,6 +3467,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3474,11 +3480,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5006,10 +5007,10 @@
   <sheetPr>
     <tabColor rgb="FF00FF99"/>
   </sheetPr>
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5887,7 +5888,9 @@
     <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89" s="126"/>
       <c r="C89" s="76"/>
-      <c r="D89" s="77"/>
+      <c r="D89" s="77">
+        <v>0</v>
+      </c>
       <c r="E89" s="127"/>
     </row>
     <row r="90" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5898,7 +5901,7 @@
       </c>
       <c r="E90" s="95"/>
     </row>
-    <row r="91" spans="1:9" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C91" s="98" t="s">
         <v>3</v>
       </c>
@@ -5907,99 +5910,103 @@
         <v>8520000</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="106"/>
-      <c r="B92" s="107"/>
-      <c r="C92" s="108" t="s">
+    <row r="92" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C92" s="48"/>
+      <c r="D92" s="181"/>
+    </row>
+    <row r="93" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="106"/>
+      <c r="B93" s="107"/>
+      <c r="C93" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="D92" s="109">
+      <c r="D93" s="109">
         <v>-3644591.85</v>
       </c>
-      <c r="E92" s="102">
+      <c r="E93" s="102">
         <v>44264</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="110"/>
-      <c r="B93" s="103"/>
-      <c r="C93" s="104" t="s">
+    <row r="94" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="110"/>
+      <c r="B94" s="103"/>
+      <c r="C94" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="D93" s="105">
+      <c r="D94" s="105">
         <v>-1303474.18</v>
-      </c>
-      <c r="E93" s="100">
-        <v>44264</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="110"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D94" s="105">
-        <v>-937943.41</v>
       </c>
       <c r="E94" s="100">
         <v>44264</v>
       </c>
-      <c r="G94" s="165">
-        <f>D92+D93+D94+D95</f>
-        <v>-7492427.9600000009</v>
-      </c>
-      <c r="H94" s="166"/>
-      <c r="I94" s="167"/>
-    </row>
-    <row r="95" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="110"/>
       <c r="B95" s="3"/>
       <c r="C95" s="104" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D95" s="105">
-        <v>-1606418.52</v>
+        <v>-937943.41</v>
       </c>
       <c r="E95" s="100">
         <v>44264</v>
       </c>
-      <c r="G95" s="168"/>
-      <c r="H95" s="169"/>
-      <c r="I95" s="170"/>
+      <c r="G95" s="165">
+        <f>D93+D94+D95+D96</f>
+        <v>-7492427.9600000009</v>
+      </c>
+      <c r="H95" s="166"/>
+      <c r="I95" s="167"/>
     </row>
     <row r="96" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="111"/>
-      <c r="B96" s="112"/>
-      <c r="C96" s="113"/>
-      <c r="D96" s="114">
-        <v>0</v>
-      </c>
-      <c r="E96" s="101"/>
-    </row>
-    <row r="97" spans="3:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C97" s="115" t="s">
+      <c r="A96" s="110"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="D96" s="105">
+        <v>-1606418.52</v>
+      </c>
+      <c r="E96" s="100">
+        <v>44264</v>
+      </c>
+      <c r="G96" s="168"/>
+      <c r="H96" s="169"/>
+      <c r="I96" s="170"/>
+    </row>
+    <row r="97" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="111"/>
+      <c r="B97" s="112"/>
+      <c r="C97" s="113"/>
+      <c r="D97" s="114">
+        <v>0</v>
+      </c>
+      <c r="E97" s="101"/>
+    </row>
+    <row r="98" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="D97" s="116">
-        <f>D94+D91+D92+D93+D95+D96</f>
+      <c r="D98" s="116">
+        <f>D95+D91+D93+D94+D96+D97</f>
         <v>1027572.0399999996</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-      <c r="D98" s="2" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+      <c r="D99" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="1"/>
     </row>
   </sheetData>
   <sortState ref="C34:D36">
@@ -6007,7 +6014,7 @@
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G94:I95"/>
+    <mergeCell ref="G95:I96"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.13" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 13 jUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="83">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve">AISLANTE TERMICO PISOS </t>
+  </si>
+  <si>
+    <t>PISO CONCRETO</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1104,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1113,6 +1115,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,21 +1154,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1235,6 +1237,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2596,17 +2601,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="138" t="s">
+      <c r="I3" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="139"/>
-      <c r="K3" s="140"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3046,11 +3051,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3204,18 +3209,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="151"/>
+      <c r="D3" s="140"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="142"/>
+      <c r="D4" s="146"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3225,10 +3230,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="153"/>
+      <c r="C6" s="142"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3245,10 +3250,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="150"/>
+      <c r="C8" s="144"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3265,10 +3270,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="150"/>
+      <c r="C10" s="144"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3285,10 +3290,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="149" t="s">
+      <c r="B12" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="150"/>
+      <c r="C12" s="144"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3305,10 +3310,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="149" t="s">
+      <c r="B14" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="150"/>
+      <c r="C14" s="144"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3325,10 +3330,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="144"/>
+      <c r="C16" s="148"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3345,14 +3350,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="144"/>
+      <c r="C18" s="148"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="145" t="s">
+      <c r="E18" s="149" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3362,7 +3367,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="146"/>
+      <c r="E19" s="150"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3373,10 +3378,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="144"/>
+      <c r="C21" s="148"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3393,10 +3398,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="148"/>
+      <c r="C23" s="152"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3413,10 +3418,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="141"/>
+      <c r="C25" s="145"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3467,11 +3472,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3480,6 +3480,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3518,11 +3523,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3723,11 +3728,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3912,11 +3917,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4120,9 +4125,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4353,9 +4358,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4713,36 +4718,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="154" t="s">
+      <c r="B57" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="155"/>
-      <c r="D57" s="155"/>
-      <c r="E57" s="156"/>
+      <c r="C57" s="154"/>
+      <c r="D57" s="154"/>
+      <c r="E57" s="155"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="157"/>
-      <c r="C58" s="158"/>
-      <c r="D58" s="158"/>
-      <c r="E58" s="159"/>
+      <c r="B58" s="156"/>
+      <c r="C58" s="157"/>
+      <c r="D58" s="157"/>
+      <c r="E58" s="158"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="157"/>
-      <c r="C59" s="158"/>
-      <c r="D59" s="158"/>
-      <c r="E59" s="159"/>
+      <c r="B59" s="156"/>
+      <c r="C59" s="157"/>
+      <c r="D59" s="157"/>
+      <c r="E59" s="158"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="157"/>
-      <c r="C60" s="158"/>
-      <c r="D60" s="158"/>
-      <c r="E60" s="159"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="157"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="158"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="160"/>
-      <c r="C61" s="161"/>
-      <c r="D61" s="161"/>
-      <c r="E61" s="162"/>
+      <c r="B61" s="159"/>
+      <c r="C61" s="160"/>
+      <c r="D61" s="160"/>
+      <c r="E61" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4787,9 +4792,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -5009,8 +5014,8 @@
   </sheetPr>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5032,12 +5037,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="164"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="165"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="164"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
@@ -5803,17 +5808,17 @@
       </c>
       <c r="E80" s="127"/>
     </row>
-    <row r="81" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="126"/>
       <c r="C81" s="76">
         <v>44709</v>
       </c>
-      <c r="D81" s="136">
+      <c r="D81" s="135">
         <v>200000</v>
       </c>
       <c r="E81" s="127"/>
     </row>
-    <row r="82" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="126"/>
       <c r="C82" s="76">
         <v>44713</v>
@@ -5821,51 +5826,54 @@
       <c r="D82" s="77">
         <v>300000</v>
       </c>
-      <c r="E82" s="135" t="s">
+      <c r="E82" s="181" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F82" s="85" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="126"/>
       <c r="C83" s="76">
         <v>44716</v>
       </c>
-      <c r="D83" s="136">
+      <c r="D83" s="135">
         <v>150000</v>
       </c>
       <c r="E83" s="127"/>
     </row>
-    <row r="84" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="126"/>
       <c r="C84" s="76">
         <v>44716</v>
       </c>
-      <c r="D84" s="136">
+      <c r="D84" s="135">
         <v>50000</v>
       </c>
       <c r="E84" s="127"/>
     </row>
-    <row r="85" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B85" s="126"/>
       <c r="C85" s="76">
         <v>44723</v>
       </c>
-      <c r="D85" s="136">
+      <c r="D85" s="135">
         <v>150000</v>
       </c>
       <c r="E85" s="127"/>
     </row>
-    <row r="86" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="126"/>
       <c r="C86" s="76">
         <v>44723</v>
       </c>
-      <c r="D86" s="136">
+      <c r="D86" s="135">
         <v>50000</v>
       </c>
       <c r="E86" s="127"/>
     </row>
-    <row r="87" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B87" s="126"/>
       <c r="C87" s="76">
         <v>44730</v>
@@ -5875,7 +5883,7 @@
       </c>
       <c r="E87" s="127"/>
     </row>
-    <row r="88" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B88" s="126"/>
       <c r="C88" s="76">
         <v>44736</v>
@@ -5885,7 +5893,7 @@
       </c>
       <c r="E88" s="127"/>
     </row>
-    <row r="89" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89" s="126"/>
       <c r="C89" s="76">
         <v>44744</v>
@@ -5895,7 +5903,7 @@
       </c>
       <c r="E89" s="127"/>
     </row>
-    <row r="90" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B90" s="126"/>
       <c r="C90" s="76">
         <v>44751</v>
@@ -5905,37 +5913,46 @@
       </c>
       <c r="E90" s="127"/>
     </row>
-    <row r="91" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="126"/>
-      <c r="C91" s="76"/>
-      <c r="D91" s="77"/>
-      <c r="E91" s="127"/>
-    </row>
-    <row r="92" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C91" s="76">
+        <v>44746</v>
+      </c>
+      <c r="D91" s="77">
+        <v>500000</v>
+      </c>
+      <c r="E91" s="130" t="s">
+        <v>82</v>
+      </c>
+      <c r="F91" s="85" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B92" s="126"/>
       <c r="C92" s="76"/>
       <c r="D92" s="77"/>
       <c r="E92" s="127"/>
     </row>
-    <row r="93" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="126"/>
       <c r="C93" s="76"/>
       <c r="D93" s="77"/>
       <c r="E93" s="127"/>
     </row>
-    <row r="94" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B94" s="126"/>
       <c r="C94" s="76"/>
       <c r="D94" s="77"/>
       <c r="E94" s="127"/>
     </row>
-    <row r="95" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B95" s="126"/>
       <c r="C95" s="76"/>
       <c r="D95" s="77"/>
       <c r="E95" s="127"/>
     </row>
-    <row r="96" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B96" s="126"/>
       <c r="C96" s="76"/>
       <c r="D96" s="77"/>
@@ -5965,12 +5982,12 @@
       </c>
       <c r="D100" s="99">
         <f>SUM(D5:D99)</f>
-        <v>8720000</v>
+        <v>9220000</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C101" s="48"/>
-      <c r="D101" s="137"/>
+      <c r="D101" s="136"/>
     </row>
     <row r="102" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="106"/>
@@ -6010,12 +6027,12 @@
       <c r="E104" s="100">
         <v>44264</v>
       </c>
-      <c r="G104" s="166">
+      <c r="G104" s="165">
         <f>D102+D103+D104+D105</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H104" s="167"/>
-      <c r="I104" s="168"/>
+      <c r="H104" s="166"/>
+      <c r="I104" s="167"/>
     </row>
     <row r="105" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="110"/>
@@ -6029,9 +6046,9 @@
       <c r="E105" s="100">
         <v>44264</v>
       </c>
-      <c r="G105" s="169"/>
-      <c r="H105" s="170"/>
-      <c r="I105" s="171"/>
+      <c r="G105" s="168"/>
+      <c r="H105" s="169"/>
+      <c r="I105" s="170"/>
     </row>
     <row r="106" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="111"/>
@@ -6048,7 +6065,7 @@
       </c>
       <c r="D107" s="116">
         <f>D104+D100+D102+D103+D105+D106</f>
-        <v>1227572.0399999996</v>
+        <v>1727572.0400000005</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -6272,23 +6289,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="178"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="175"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="176"/>
+      <c r="B4" s="175"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6326,13 +6343,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="173"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6525,7 +6542,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="178" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6535,13 +6552,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="180"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="180"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6549,7 +6566,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="180"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6559,7 +6576,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="181"/>
+      <c r="B6" s="180"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6575,7 +6592,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="172" t="s">
+      <c r="B8" s="171" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6587,7 +6604,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="173"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6787,7 +6804,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="178" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6797,13 +6814,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="180"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="180"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6811,7 +6828,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="180"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -6821,7 +6838,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="181"/>
+      <c r="B6" s="180"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -6837,7 +6854,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -6845,7 +6862,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="173"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>

</xml_diff>

<commit_message>
cierre 23 julio 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1118,6 +1118,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1140,21 +1155,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3209,18 +3209,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="151"/>
+      <c r="D3" s="141"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="142"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3230,10 +3230,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="153"/>
+      <c r="C6" s="143"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3250,10 +3250,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="150"/>
+      <c r="C8" s="145"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3270,10 +3270,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="150"/>
+      <c r="C10" s="145"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3290,10 +3290,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="149" t="s">
+      <c r="B12" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="150"/>
+      <c r="C12" s="145"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3310,10 +3310,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="149" t="s">
+      <c r="B14" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="150"/>
+      <c r="C14" s="145"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3330,10 +3330,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="144"/>
+      <c r="C16" s="149"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3350,14 +3350,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="144"/>
+      <c r="C18" s="149"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="145" t="s">
+      <c r="E18" s="150" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="146"/>
+      <c r="E19" s="151"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3378,10 +3378,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="144"/>
+      <c r="C21" s="149"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3398,10 +3398,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="148"/>
+      <c r="C23" s="153"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3418,10 +3418,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="141"/>
+      <c r="C25" s="146"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3472,11 +3472,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3485,6 +3480,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5015,7 +5015,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5941,8 +5941,12 @@
     </row>
     <row r="93" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="126"/>
-      <c r="C93" s="76"/>
-      <c r="D93" s="77"/>
+      <c r="C93" s="76">
+        <v>44765</v>
+      </c>
+      <c r="D93" s="77">
+        <v>100000</v>
+      </c>
       <c r="E93" s="127"/>
     </row>
     <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5987,7 +5991,7 @@
       </c>
       <c r="D100" s="99">
         <f>SUM(D5:D99)</f>
-        <v>9320000</v>
+        <v>9420000</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6070,7 +6074,7 @@
       </c>
       <c r="D107" s="116">
         <f>D104+D100+D102+D103+D105+D106</f>
-        <v>1827572.0400000005</v>
+        <v>1927572.0400000005</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cierre 30 julio 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1118,6 +1118,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1125,36 +1155,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3209,18 +3209,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="141"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="147"/>
+      <c r="D4" s="142"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3230,10 +3230,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="143"/>
+      <c r="C6" s="153"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3250,10 +3250,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="145"/>
+      <c r="C8" s="150"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3270,10 +3270,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="145"/>
+      <c r="C10" s="150"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3290,10 +3290,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="149" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="145"/>
+      <c r="C12" s="150"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3310,10 +3310,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="149" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="145"/>
+      <c r="C14" s="150"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3330,10 +3330,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="143" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="149"/>
+      <c r="C16" s="144"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3350,14 +3350,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="149"/>
+      <c r="C18" s="144"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="150" t="s">
+      <c r="E18" s="145" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="151"/>
+      <c r="E19" s="146"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3378,10 +3378,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="148" t="s">
+      <c r="B21" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="149"/>
+      <c r="C21" s="144"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3398,10 +3398,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="153"/>
+      <c r="C23" s="148"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3418,10 +3418,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="146" t="s">
+      <c r="B25" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="146"/>
+      <c r="C25" s="141"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3472,6 +3472,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3480,11 +3485,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5015,7 +5015,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5951,14 +5951,22 @@
     </row>
     <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B94" s="126"/>
-      <c r="C94" s="76"/>
-      <c r="D94" s="77"/>
+      <c r="C94" s="76">
+        <v>44772</v>
+      </c>
+      <c r="D94" s="77">
+        <v>100000</v>
+      </c>
       <c r="E94" s="127"/>
     </row>
     <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B95" s="126"/>
-      <c r="C95" s="76"/>
-      <c r="D95" s="77"/>
+      <c r="C95" s="76">
+        <v>44771</v>
+      </c>
+      <c r="D95" s="77">
+        <v>100000</v>
+      </c>
       <c r="E95" s="127"/>
     </row>
     <row r="96" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5991,7 +5999,7 @@
       </c>
       <c r="D100" s="99">
         <f>SUM(D5:D99)</f>
-        <v>9420000</v>
+        <v>9620000</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6074,7 +6082,7 @@
       </c>
       <c r="D107" s="116">
         <f>D104+D100+D102+D103+D105+D106</f>
-        <v>1927572.0400000005</v>
+        <v>2127572.0400000005</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 27 AGO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -1144,6 +1144,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1153,6 +1154,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1162,36 +1193,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1270,7 +1271,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2694,17 +2694,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="144"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3144,11 +3144,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3302,18 +3302,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="155" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="155"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="150"/>
+      <c r="D4" s="146"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3323,10 +3323,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="146"/>
+      <c r="C6" s="157"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3343,10 +3343,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="148"/>
+      <c r="C8" s="154"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3363,10 +3363,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="153" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="148"/>
+      <c r="C10" s="154"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3383,10 +3383,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="148"/>
+      <c r="C12" s="154"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3403,10 +3403,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="153" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="148"/>
+      <c r="C14" s="154"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3423,10 +3423,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="152"/>
+      <c r="C16" s="148"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3443,14 +3443,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="152"/>
+      <c r="C18" s="148"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="153" t="s">
+      <c r="E18" s="149" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3460,7 +3460,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="154"/>
+      <c r="E19" s="150"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3471,10 +3471,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="152"/>
+      <c r="C21" s="148"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3491,10 +3491,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="156"/>
+      <c r="C23" s="152"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3511,10 +3511,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="149" t="s">
+      <c r="B25" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="149"/>
+      <c r="C25" s="145"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3565,6 +3565,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3573,11 +3578,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3616,11 +3616,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3821,11 +3821,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4010,11 +4010,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4218,9 +4218,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4451,9 +4451,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4811,36 +4811,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="157" t="s">
+      <c r="B57" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="158"/>
-      <c r="D57" s="158"/>
-      <c r="E57" s="159"/>
+      <c r="C57" s="159"/>
+      <c r="D57" s="159"/>
+      <c r="E57" s="160"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="160"/>
-      <c r="C58" s="161"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="162"/>
+      <c r="B58" s="161"/>
+      <c r="C58" s="162"/>
+      <c r="D58" s="162"/>
+      <c r="E58" s="163"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="160"/>
-      <c r="C59" s="161"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="162"/>
+      <c r="B59" s="161"/>
+      <c r="C59" s="162"/>
+      <c r="D59" s="162"/>
+      <c r="E59" s="163"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="160"/>
-      <c r="C60" s="161"/>
-      <c r="D60" s="161"/>
-      <c r="E60" s="162"/>
+      <c r="B60" s="161"/>
+      <c r="C60" s="162"/>
+      <c r="D60" s="162"/>
+      <c r="E60" s="163"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="163"/>
-      <c r="C61" s="164"/>
-      <c r="D61" s="164"/>
-      <c r="E61" s="165"/>
+      <c r="B61" s="164"/>
+      <c r="C61" s="165"/>
+      <c r="D61" s="165"/>
+      <c r="E61" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4885,9 +4885,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -5107,8 +5107,8 @@
   </sheetPr>
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5132,12 +5132,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="168"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="169"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
     </row>
@@ -6132,8 +6132,12 @@
     </row>
     <row r="102" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B102" s="126"/>
-      <c r="C102" s="76"/>
-      <c r="D102" s="77"/>
+      <c r="C102" s="76">
+        <v>44800</v>
+      </c>
+      <c r="D102" s="77">
+        <v>100000</v>
+      </c>
       <c r="E102" s="139"/>
       <c r="F102" s="85"/>
     </row>
@@ -6211,7 +6215,7 @@
       </c>
       <c r="D113" s="99">
         <f>SUM(D5:D112)</f>
-        <v>10169786.73</v>
+        <v>10269786.73</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6250,11 +6254,11 @@
         <v>-659691.4</v>
       </c>
       <c r="E117" s="100"/>
-      <c r="G117" s="169">
+      <c r="G117" s="170">
         <f>D115+D116+D117+D118</f>
         <v>-8718896</v>
       </c>
-      <c r="H117" s="170"/>
+      <c r="H117" s="171"/>
     </row>
     <row r="118" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="110"/>
@@ -6266,8 +6270,8 @@
         <v>-1241668.1599999999</v>
       </c>
       <c r="E118" s="100"/>
-      <c r="G118" s="171"/>
-      <c r="H118" s="172"/>
+      <c r="G118" s="172"/>
+      <c r="H118" s="173"/>
     </row>
     <row r="119" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="111"/>
@@ -6275,7 +6279,7 @@
       <c r="C119" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="D119" s="183">
+      <c r="D119" s="141">
         <v>-2122661.75</v>
       </c>
       <c r="E119" s="101"/>
@@ -6286,7 +6290,7 @@
       </c>
       <c r="D120" s="116">
         <f>D117+D113+D115+D116+D118+D119</f>
-        <v>-671771.01999999979</v>
+        <v>-571771.01999999979</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -6510,23 +6514,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="179" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="179"/>
+      <c r="D2" s="180"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="176"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="177"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6564,13 +6568,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="173"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="174"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6763,7 +6767,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="180" t="s">
+      <c r="B2" s="181" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6773,13 +6777,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="181"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="181"/>
+      <c r="B4" s="182"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6787,7 +6791,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="181"/>
+      <c r="B5" s="182"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6797,7 +6801,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="182"/>
+      <c r="B6" s="183"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6813,7 +6817,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="173" t="s">
+      <c r="B8" s="174" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6825,7 +6829,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="174"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -7025,7 +7029,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="180" t="s">
+      <c r="B2" s="181" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -7035,13 +7039,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="181"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="181"/>
+      <c r="B4" s="182"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -7049,7 +7053,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="181"/>
+      <c r="B5" s="182"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -7059,7 +7063,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="182"/>
+      <c r="B6" s="183"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -7075,7 +7079,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="173"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -7083,7 +7087,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="174"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -7300,12 +7304,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="168"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="169"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
     </row>
@@ -8424,11 +8428,11 @@
       <c r="E117" s="100">
         <v>44264</v>
       </c>
-      <c r="G117" s="169">
+      <c r="G117" s="170">
         <f>D115+D116+D117+D118</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H117" s="170"/>
+      <c r="H117" s="171"/>
     </row>
     <row r="118" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="110"/>
@@ -8442,8 +8446,8 @@
       <c r="E118" s="100">
         <v>44264</v>
       </c>
-      <c r="G118" s="171"/>
-      <c r="H118" s="172"/>
+      <c r="G118" s="172"/>
+      <c r="H118" s="173"/>
     </row>
     <row r="119" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="111"/>

</xml_diff>

<commit_message>
cierre del sabado 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -891,7 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1177,6 +1177,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2726,17 +2729,17 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
       <c r="H3" s="50"/>
-      <c r="I3" s="151" t="s">
+      <c r="I3" s="152" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="152"/>
-      <c r="K3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="154"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3176,11 +3179,11 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -3334,18 +3337,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="154" t="s">
+      <c r="C3" s="155" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="154"/>
+      <c r="D3" s="155"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="160"/>
+      <c r="D4" s="161"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3355,10 +3358,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="155" t="s">
+      <c r="B6" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="156"/>
+      <c r="C6" s="157"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3375,10 +3378,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="157" t="s">
+      <c r="B8" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="158"/>
+      <c r="C8" s="159"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3395,10 +3398,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="158"/>
+      <c r="C10" s="159"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3415,10 +3418,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="157" t="s">
+      <c r="B12" s="158" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="158"/>
+      <c r="C12" s="159"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3435,10 +3438,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="158"/>
+      <c r="C14" s="159"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3455,10 +3458,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="161" t="s">
+      <c r="B16" s="162" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="162"/>
+      <c r="C16" s="163"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3475,14 +3478,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="162"/>
+      <c r="C18" s="163"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="163" t="s">
+      <c r="E18" s="164" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3492,7 +3495,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="164"/>
+      <c r="E19" s="165"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3503,10 +3506,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="161" t="s">
+      <c r="B21" s="162" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="162"/>
+      <c r="C21" s="163"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3523,10 +3526,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="165" t="s">
+      <c r="B23" s="166" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="166"/>
+      <c r="C23" s="167"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3543,10 +3546,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="159" t="s">
+      <c r="B25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="159"/>
+      <c r="C25" s="160"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3648,11 +3651,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -3853,11 +3856,11 @@
       <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4042,11 +4045,11 @@
     </row>
     <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="50"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="152" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="83" t="s">
@@ -4250,9 +4253,9 @@
       <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4483,9 +4486,9 @@
       <c r="B3" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -4843,36 +4846,36 @@
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="167" t="s">
+      <c r="B57" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="168"/>
-      <c r="D57" s="168"/>
-      <c r="E57" s="169"/>
+      <c r="C57" s="169"/>
+      <c r="D57" s="169"/>
+      <c r="E57" s="170"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="170"/>
-      <c r="C58" s="171"/>
-      <c r="D58" s="171"/>
-      <c r="E58" s="172"/>
+      <c r="B58" s="171"/>
+      <c r="C58" s="172"/>
+      <c r="D58" s="172"/>
+      <c r="E58" s="173"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="170"/>
-      <c r="C59" s="171"/>
-      <c r="D59" s="171"/>
-      <c r="E59" s="172"/>
+      <c r="B59" s="171"/>
+      <c r="C59" s="172"/>
+      <c r="D59" s="172"/>
+      <c r="E59" s="173"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="170"/>
-      <c r="C60" s="171"/>
-      <c r="D60" s="171"/>
-      <c r="E60" s="172"/>
+      <c r="B60" s="171"/>
+      <c r="C60" s="172"/>
+      <c r="D60" s="172"/>
+      <c r="E60" s="173"/>
     </row>
     <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="173"/>
-      <c r="C61" s="174"/>
-      <c r="D61" s="174"/>
-      <c r="E61" s="175"/>
+      <c r="B61" s="174"/>
+      <c r="C61" s="175"/>
+      <c r="D61" s="175"/>
+      <c r="E61" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4917,9 +4920,9 @@
       <c r="B3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
@@ -5140,7 +5143,7 @@
   <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B106" sqref="B105:B106"/>
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5164,12 +5167,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
     </row>
@@ -6260,11 +6263,11 @@
       <c r="E111" s="139"/>
       <c r="F111" s="85"/>
     </row>
-    <row r="112" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B112" s="149">
         <v>44891</v>
       </c>
-      <c r="C112" s="76" t="s">
+      <c r="C112" s="151" t="s">
         <v>91</v>
       </c>
       <c r="D112" s="150">
@@ -6297,9 +6300,11 @@
     </row>
     <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B115" s="126"/>
-      <c r="C115" s="76"/>
+      <c r="C115" s="76">
+        <v>44919</v>
+      </c>
       <c r="D115" s="77">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="E115" s="127"/>
     </row>
@@ -6320,7 +6325,7 @@
       </c>
       <c r="D117" s="25">
         <f>SUM(D5:D116)</f>
-        <v>10640428.73</v>
+        <v>10710428.73</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6359,11 +6364,11 @@
         <v>-659691.4</v>
       </c>
       <c r="E121" s="100"/>
-      <c r="G121" s="179">
+      <c r="G121" s="180">
         <f>D119+D120+D121+D122</f>
         <v>-8718896</v>
       </c>
-      <c r="H121" s="180"/>
+      <c r="H121" s="181"/>
     </row>
     <row r="122" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="110"/>
@@ -6375,8 +6380,8 @@
         <v>-1241668.1599999999</v>
       </c>
       <c r="E122" s="100"/>
-      <c r="G122" s="181"/>
-      <c r="H122" s="182"/>
+      <c r="G122" s="182"/>
+      <c r="H122" s="183"/>
     </row>
     <row r="123" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="111"/>
@@ -6404,7 +6409,7 @@
       </c>
       <c r="D125" s="116">
         <f>D121+D117+D119+D120+D122+D123+D124</f>
-        <v>-201129.01999999979</v>
+        <v>-131129.01999999979</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -6628,23 +6633,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="186" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="188" t="s">
+      <c r="C2" s="189" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="189"/>
+      <c r="D2" s="190"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="186"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="187"/>
+      <c r="B4" s="188"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6682,13 +6687,13 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="183"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="184"/>
+      <c r="B9" s="185"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -6881,7 +6886,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="191" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6891,13 +6896,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="191"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="191"/>
+      <c r="B4" s="192"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6905,7 +6910,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="191"/>
+      <c r="B5" s="192"/>
       <c r="C5" s="47">
         <v>44380</v>
       </c>
@@ -6915,7 +6920,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="192"/>
+      <c r="B6" s="193"/>
       <c r="C6" s="36">
         <v>44396</v>
       </c>
@@ -6931,7 +6936,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="183" t="s">
+      <c r="B8" s="184" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="36">
@@ -6943,7 +6948,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="184"/>
+      <c r="B9" s="185"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -7143,7 +7148,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="191" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -7153,13 +7158,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="191"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="153"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="191"/>
+      <c r="B4" s="192"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
@@ -7167,7 +7172,7 @@
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="191"/>
+      <c r="B5" s="192"/>
       <c r="C5" s="47">
         <v>44621</v>
       </c>
@@ -7177,7 +7182,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="192"/>
+      <c r="B6" s="193"/>
       <c r="C6" s="36">
         <v>44656</v>
       </c>
@@ -7193,7 +7198,7 @@
       <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="183"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37">
         <v>0</v>
@@ -7201,7 +7206,7 @@
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="184"/>
+      <c r="B9" s="185"/>
       <c r="C9" s="93"/>
       <c r="D9" s="77"/>
       <c r="E9" s="27"/>
@@ -7418,12 +7423,12 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
     </row>
@@ -8542,11 +8547,11 @@
       <c r="E117" s="100">
         <v>44264</v>
       </c>
-      <c r="G117" s="179">
+      <c r="G117" s="180">
         <f>D115+D116+D117+D118</f>
         <v>-7492427.9600000009</v>
       </c>
-      <c r="H117" s="180"/>
+      <c r="H117" s="181"/>
     </row>
     <row r="118" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="110"/>
@@ -8560,8 +8565,8 @@
       <c r="E118" s="100">
         <v>44264</v>
       </c>
-      <c r="G118" s="181"/>
-      <c r="H118" s="182"/>
+      <c r="G118" s="182"/>
+      <c r="H118" s="183"/>
     </row>
     <row r="119" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="111"/>

</xml_diff>

<commit_message>
cierre 12 Jul 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -373,9 +373,6 @@
     <t xml:space="preserve">MUNICIPIO DE PUEBLA </t>
   </si>
   <si>
-    <t>LAVAMANOS Y COLADERAS</t>
-  </si>
-  <si>
     <t>TUBERIAS DE ORIENTE</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t xml:space="preserve">BOMBA, HIDRO, </t>
+  </si>
+  <si>
+    <t>LAVAMANOS Y COLADERAS, CABINA BOTAS</t>
   </si>
 </sst>
 </file>
@@ -1370,6 +1370,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1379,36 +1409,6 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1436,53 +1436,53 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="19" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3651,18 +3651,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="192" t="s">
+      <c r="C3" s="202" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="192"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="198" t="s">
+      <c r="C4" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="198"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3672,10 +3672,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="193" t="s">
+      <c r="B6" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="194"/>
+      <c r="C6" s="204"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -3692,10 +3692,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="200" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="196"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -3712,10 +3712,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="195" t="s">
+      <c r="B10" s="200" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="196"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -3732,10 +3732,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="195" t="s">
+      <c r="B12" s="200" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="196"/>
+      <c r="C12" s="201"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -3752,10 +3752,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="195" t="s">
+      <c r="B14" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="196"/>
+      <c r="C14" s="201"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -3772,10 +3772,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="199" t="s">
+      <c r="B16" s="194" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="200"/>
+      <c r="C16" s="195"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -3792,14 +3792,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="199" t="s">
+      <c r="B18" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="200"/>
+      <c r="C18" s="195"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="201" t="s">
+      <c r="E18" s="196" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3809,7 +3809,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="202"/>
+      <c r="E19" s="197"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -3820,10 +3820,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="199" t="s">
+      <c r="B21" s="194" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="200"/>
+      <c r="C21" s="195"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -3840,10 +3840,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="203" t="s">
+      <c r="B23" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="204"/>
+      <c r="C23" s="199"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -3860,10 +3860,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="197" t="s">
+      <c r="B25" s="192" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="197"/>
+      <c r="C25" s="192"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -3914,6 +3914,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -3922,11 +3927,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5457,7 +5457,7 @@
   <dimension ref="B1:Y66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5487,80 +5487,80 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="219" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="218" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="219"/>
+      <c r="D2" s="218"/>
       <c r="E2" s="17"/>
-      <c r="I2" s="216" t="s">
+      <c r="I2" s="219" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="219" t="s">
+      <c r="J2" s="218" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="219"/>
+      <c r="K2" s="218"/>
       <c r="L2" s="17"/>
       <c r="M2" s="166"/>
-      <c r="P2" s="224" t="s">
+      <c r="P2" s="222" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="219" t="s">
+      <c r="Q2" s="218" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="219"/>
+      <c r="R2" s="218"/>
       <c r="S2" s="17"/>
-      <c r="V2" s="227" t="s">
+      <c r="V2" s="225" t="s">
         <v>94</v>
       </c>
-      <c r="W2" s="219" t="s">
+      <c r="W2" s="218" t="s">
         <v>80</v>
       </c>
-      <c r="X2" s="219"/>
+      <c r="X2" s="218"/>
       <c r="Y2" s="17"/>
     </row>
     <row r="3" spans="2:25" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="217"/>
+      <c r="B3" s="220"/>
       <c r="C3" s="190"/>
       <c r="D3" s="190"/>
       <c r="E3" s="191"/>
-      <c r="I3" s="217"/>
+      <c r="I3" s="220"/>
       <c r="J3" s="190"/>
       <c r="K3" s="190"/>
       <c r="L3" s="191"/>
       <c r="M3" s="166"/>
-      <c r="P3" s="225"/>
+      <c r="P3" s="223"/>
       <c r="Q3" s="190"/>
       <c r="R3" s="190"/>
       <c r="S3" s="191"/>
-      <c r="V3" s="228"/>
+      <c r="V3" s="226"/>
       <c r="W3" s="190"/>
       <c r="X3" s="190"/>
       <c r="Y3" s="191"/>
     </row>
     <row r="4" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="217"/>
+      <c r="B4" s="220"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="217"/>
+      <c r="I4" s="220"/>
       <c r="J4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="23"/>
       <c r="M4" s="166"/>
-      <c r="P4" s="225"/>
+      <c r="P4" s="223"/>
       <c r="Q4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="R4" s="22"/>
       <c r="S4" s="23"/>
-      <c r="V4" s="228"/>
+      <c r="V4" s="226"/>
       <c r="W4" s="21" t="s">
         <v>2</v>
       </c>
@@ -5568,7 +5568,7 @@
       <c r="Y4" s="23"/>
     </row>
     <row r="5" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="217"/>
+      <c r="B5" s="220"/>
       <c r="C5" s="155" t="s">
         <v>80</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>563480</v>
       </c>
       <c r="E5" s="28"/>
-      <c r="I5" s="217"/>
+      <c r="I5" s="220"/>
       <c r="J5" s="155">
         <v>45010</v>
       </c>
@@ -5585,7 +5585,7 @@
       </c>
       <c r="L5" s="28"/>
       <c r="M5" s="166"/>
-      <c r="P5" s="225"/>
+      <c r="P5" s="223"/>
       <c r="Q5" s="155">
         <v>44947</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>50000</v>
       </c>
       <c r="S5" s="28"/>
-      <c r="V5" s="228"/>
+      <c r="V5" s="226"/>
       <c r="W5" s="155">
         <v>44873</v>
       </c>
@@ -5603,7 +5603,7 @@
       <c r="Y5" s="28"/>
     </row>
     <row r="6" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="217"/>
+      <c r="B6" s="220"/>
       <c r="C6" s="155">
         <v>45010</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>50000</v>
       </c>
       <c r="E6" s="27"/>
-      <c r="I6" s="217"/>
+      <c r="I6" s="220"/>
       <c r="J6" s="154">
         <v>45017</v>
       </c>
@@ -5620,7 +5620,7 @@
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="166"/>
-      <c r="P6" s="225"/>
+      <c r="P6" s="223"/>
       <c r="Q6" s="176">
         <v>44954</v>
       </c>
@@ -5628,13 +5628,13 @@
         <v>50000</v>
       </c>
       <c r="S6" s="27"/>
-      <c r="V6" s="228"/>
+      <c r="V6" s="226"/>
       <c r="W6" s="176"/>
       <c r="X6" s="37"/>
       <c r="Y6" s="27"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="217"/>
+      <c r="B7" s="220"/>
       <c r="C7" s="165">
         <v>45017</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>100000</v>
       </c>
       <c r="E7" s="41"/>
-      <c r="I7" s="217"/>
+      <c r="I7" s="220"/>
       <c r="J7" s="154">
         <v>45021</v>
       </c>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="L7" s="41"/>
       <c r="M7" s="166"/>
-      <c r="P7" s="225"/>
+      <c r="P7" s="223"/>
       <c r="Q7" s="176">
         <v>44961</v>
       </c>
@@ -5659,13 +5659,13 @@
         <v>50000</v>
       </c>
       <c r="S7" s="41"/>
-      <c r="V7" s="228"/>
+      <c r="V7" s="226"/>
       <c r="W7" s="176"/>
       <c r="X7" s="37"/>
       <c r="Y7" s="41"/>
     </row>
     <row r="8" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="217"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="165">
         <v>45021</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>50000</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="I8" s="217"/>
+      <c r="I8" s="220"/>
       <c r="J8" s="154">
         <v>45031</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="166"/>
-      <c r="P8" s="225"/>
+      <c r="P8" s="223"/>
       <c r="Q8" s="176">
         <v>44968</v>
       </c>
@@ -5690,13 +5690,13 @@
         <v>50000</v>
       </c>
       <c r="S8" s="27"/>
-      <c r="V8" s="228"/>
+      <c r="V8" s="226"/>
       <c r="W8" s="176"/>
       <c r="X8" s="37"/>
       <c r="Y8" s="27"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="217"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="165">
         <v>45031</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>100000</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="I9" s="217"/>
+      <c r="I9" s="220"/>
       <c r="J9" s="156">
         <v>45038</v>
       </c>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="L9" s="27"/>
       <c r="M9" s="166"/>
-      <c r="P9" s="225"/>
+      <c r="P9" s="223"/>
       <c r="Q9" s="156">
         <v>44975</v>
       </c>
@@ -5721,15 +5721,15 @@
         <v>50000</v>
       </c>
       <c r="S9" s="27"/>
-      <c r="V9" s="228"/>
-      <c r="W9" s="220" t="s">
+      <c r="V9" s="226"/>
+      <c r="W9" s="214" t="s">
         <v>95</v>
       </c>
-      <c r="X9" s="220"/>
-      <c r="Y9" s="221"/>
+      <c r="X9" s="214"/>
+      <c r="Y9" s="215"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="217"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="156">
         <v>45038</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>50000</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="I10" s="217"/>
+      <c r="I10" s="220"/>
       <c r="J10" s="156">
         <v>45045</v>
       </c>
@@ -5746,7 +5746,7 @@
       </c>
       <c r="L10" s="27"/>
       <c r="M10" s="166"/>
-      <c r="P10" s="225"/>
+      <c r="P10" s="223"/>
       <c r="Q10" s="156">
         <v>44982</v>
       </c>
@@ -5754,13 +5754,13 @@
         <v>50000</v>
       </c>
       <c r="S10" s="27"/>
-      <c r="V10" s="228"/>
-      <c r="W10" s="222"/>
-      <c r="X10" s="222"/>
-      <c r="Y10" s="223"/>
+      <c r="V10" s="226"/>
+      <c r="W10" s="216"/>
+      <c r="X10" s="216"/>
+      <c r="Y10" s="217"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="217"/>
+      <c r="B11" s="220"/>
       <c r="C11" s="156">
         <v>45045</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="I11" s="217"/>
+      <c r="I11" s="220"/>
       <c r="J11" s="156">
         <v>45052</v>
       </c>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="166"/>
-      <c r="P11" s="225"/>
+      <c r="P11" s="223"/>
       <c r="Q11" s="156">
         <v>44989</v>
       </c>
@@ -5785,13 +5785,13 @@
         <v>50000</v>
       </c>
       <c r="S11" s="27"/>
-      <c r="V11" s="228"/>
+      <c r="V11" s="226"/>
       <c r="W11" s="156"/>
       <c r="X11" s="77"/>
       <c r="Y11" s="27"/>
     </row>
     <row r="12" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="217"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="156">
         <v>45052</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>100000</v>
       </c>
       <c r="E12" s="146"/>
-      <c r="I12" s="217"/>
+      <c r="I12" s="220"/>
       <c r="J12" s="157">
         <v>45059</v>
       </c>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="L12" s="146"/>
       <c r="M12" s="166"/>
-      <c r="P12" s="225"/>
+      <c r="P12" s="223"/>
       <c r="Q12" s="157">
         <v>44989</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>50000</v>
       </c>
       <c r="S12" s="146"/>
-      <c r="V12" s="228"/>
+      <c r="V12" s="226"/>
       <c r="W12" s="176"/>
       <c r="X12" s="37">
         <v>0</v>
@@ -5824,7 +5824,7 @@
       <c r="Y12" s="3"/>
     </row>
     <row r="13" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="217"/>
+      <c r="B13" s="220"/>
       <c r="C13" s="157">
         <v>45059</v>
       </c>
@@ -5832,12 +5832,12 @@
         <v>100000</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="I13" s="217"/>
+      <c r="I13" s="220"/>
       <c r="J13" s="154"/>
       <c r="K13" s="37"/>
       <c r="L13" s="3"/>
       <c r="M13" s="166"/>
-      <c r="P13" s="225"/>
+      <c r="P13" s="223"/>
       <c r="Q13" s="176">
         <v>44996</v>
       </c>
@@ -5845,13 +5845,13 @@
         <v>50000</v>
       </c>
       <c r="S13" s="3"/>
-      <c r="V13" s="228"/>
+      <c r="V13" s="226"/>
       <c r="W13" s="176"/>
       <c r="X13" s="37"/>
       <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="217"/>
+      <c r="B14" s="220"/>
       <c r="C14" s="165">
         <v>45066</v>
       </c>
@@ -5859,12 +5859,12 @@
         <v>100000</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="I14" s="217"/>
+      <c r="I14" s="220"/>
       <c r="J14" s="154"/>
       <c r="K14" s="37"/>
       <c r="L14" s="3"/>
       <c r="M14" s="166"/>
-      <c r="P14" s="225"/>
+      <c r="P14" s="223"/>
       <c r="Q14" s="176">
         <v>45003</v>
       </c>
@@ -5872,13 +5872,13 @@
         <v>113480</v>
       </c>
       <c r="S14" s="3"/>
-      <c r="V14" s="228"/>
+      <c r="V14" s="226"/>
       <c r="W14" s="176"/>
       <c r="X14" s="37"/>
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="217"/>
+      <c r="B15" s="220"/>
       <c r="C15" s="165">
         <v>45073</v>
       </c>
@@ -5886,18 +5886,18 @@
         <v>100000</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="I15" s="217"/>
+      <c r="I15" s="220"/>
       <c r="J15" s="154"/>
       <c r="K15" s="37"/>
       <c r="L15" s="3"/>
       <c r="M15" s="166"/>
-      <c r="P15" s="225"/>
+      <c r="P15" s="223"/>
       <c r="Q15" s="176"/>
       <c r="R15" s="37">
         <v>0</v>
       </c>
       <c r="S15" s="3"/>
-      <c r="V15" s="228"/>
+      <c r="V15" s="226"/>
       <c r="W15" s="158" t="s">
         <v>3</v>
       </c>
@@ -5907,7 +5907,7 @@
       </c>
     </row>
     <row r="16" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="217"/>
+      <c r="B16" s="220"/>
       <c r="C16" s="165">
         <v>45079</v>
       </c>
@@ -5915,18 +5915,18 @@
         <v>100000</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="I16" s="217"/>
+      <c r="I16" s="220"/>
       <c r="J16" s="154"/>
       <c r="K16" s="37"/>
       <c r="L16" s="3"/>
       <c r="M16" s="166"/>
-      <c r="P16" s="225"/>
+      <c r="P16" s="223"/>
       <c r="Q16" s="176"/>
       <c r="R16" s="37">
         <v>0</v>
       </c>
       <c r="S16" s="3"/>
-      <c r="V16" s="228"/>
+      <c r="V16" s="226"/>
       <c r="W16" s="121"/>
       <c r="X16" s="49">
         <v>67769</v>
@@ -5936,7 +5936,7 @@
       </c>
     </row>
     <row r="17" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="217"/>
+      <c r="B17" s="220"/>
       <c r="C17" s="165">
         <v>45086</v>
       </c>
@@ -5946,12 +5946,12 @@
       <c r="E17" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="217"/>
+      <c r="I17" s="220"/>
       <c r="J17" s="154"/>
       <c r="K17" s="37"/>
       <c r="L17" s="3"/>
       <c r="M17" s="166"/>
-      <c r="P17" s="225"/>
+      <c r="P17" s="223"/>
       <c r="Q17" s="184" t="s">
         <v>3</v>
       </c>
@@ -5959,7 +5959,7 @@
         <f>SUM(R5:R16)</f>
         <v>563480</v>
       </c>
-      <c r="V17" s="228"/>
+      <c r="V17" s="226"/>
       <c r="W17" s="65"/>
       <c r="X17" s="49">
         <v>0</v>
@@ -5967,7 +5967,7 @@
       <c r="Y17" s="124"/>
     </row>
     <row r="18" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="217"/>
+      <c r="B18" s="220"/>
       <c r="C18" s="167">
         <v>45090</v>
       </c>
@@ -5977,12 +5977,12 @@
       <c r="E18" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="I18" s="217"/>
+      <c r="I18" s="220"/>
       <c r="J18" s="154"/>
       <c r="K18" s="37"/>
       <c r="L18" s="3"/>
       <c r="M18" s="166"/>
-      <c r="P18" s="225"/>
+      <c r="P18" s="223"/>
       <c r="Q18" s="160"/>
       <c r="R18" s="161">
         <v>-563480</v>
@@ -5990,14 +5990,14 @@
       <c r="S18" s="152">
         <v>44947</v>
       </c>
-      <c r="V18" s="228"/>
+      <c r="V18" s="226"/>
       <c r="W18" s="84"/>
       <c r="X18" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="217"/>
+      <c r="B19" s="220"/>
       <c r="C19" s="167">
         <v>45091</v>
       </c>
@@ -6007,18 +6007,18 @@
       <c r="E19" s="169" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="217"/>
+      <c r="I19" s="220"/>
       <c r="J19" s="154"/>
       <c r="K19" s="37"/>
       <c r="L19" s="3"/>
       <c r="M19" s="166"/>
-      <c r="P19" s="225"/>
+      <c r="P19" s="223"/>
       <c r="Q19" s="162"/>
       <c r="R19" s="161">
         <v>0</v>
       </c>
       <c r="S19" s="124"/>
-      <c r="V19" s="229"/>
+      <c r="V19" s="227"/>
       <c r="W19" s="185" t="s">
         <v>4</v>
       </c>
@@ -6028,7 +6028,7 @@
       </c>
     </row>
     <row r="20" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="217"/>
+      <c r="B20" s="220"/>
       <c r="C20" s="167">
         <v>45091</v>
       </c>
@@ -6038,12 +6038,12 @@
       <c r="E20" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="217"/>
+      <c r="I20" s="220"/>
       <c r="J20" s="154"/>
       <c r="K20" s="37"/>
       <c r="L20" s="3"/>
       <c r="M20" s="166"/>
-      <c r="P20" s="225"/>
+      <c r="P20" s="223"/>
       <c r="Q20" s="163"/>
       <c r="R20" s="164">
         <v>0</v>
@@ -6054,7 +6054,7 @@
       <c r="Y20" s="118"/>
     </row>
     <row r="21" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="217"/>
+      <c r="B21" s="220"/>
       <c r="C21" s="165">
         <v>45092</v>
       </c>
@@ -6063,12 +6063,12 @@
       </c>
       <c r="E21" s="168"/>
       <c r="F21" s="187"/>
-      <c r="I21" s="217"/>
+      <c r="I21" s="220"/>
       <c r="J21" s="154"/>
       <c r="K21" s="37"/>
       <c r="L21" s="3"/>
       <c r="M21" s="166"/>
-      <c r="P21" s="225"/>
+      <c r="P21" s="223"/>
       <c r="Q21" s="33" t="s">
         <v>4</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="Y21" s="118"/>
     </row>
     <row r="22" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="217"/>
+      <c r="B22" s="220"/>
       <c r="C22" s="165">
         <v>45101</v>
       </c>
@@ -6091,12 +6091,12 @@
       </c>
       <c r="E22" s="168"/>
       <c r="F22" s="187"/>
-      <c r="I22" s="217"/>
+      <c r="I22" s="220"/>
       <c r="J22" s="154"/>
       <c r="K22" s="37"/>
       <c r="L22" s="3"/>
       <c r="M22" s="166"/>
-      <c r="P22" s="226"/>
+      <c r="P22" s="224"/>
       <c r="Q22" s="182"/>
       <c r="R22" s="183"/>
       <c r="S22" s="118"/>
@@ -6106,7 +6106,7 @@
       <c r="Y22" s="118"/>
     </row>
     <row r="23" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="217"/>
+      <c r="B23" s="220"/>
       <c r="C23" s="165">
         <v>45108</v>
       </c>
@@ -6115,7 +6115,7 @@
       </c>
       <c r="E23" s="168"/>
       <c r="F23" s="187"/>
-      <c r="I23" s="217"/>
+      <c r="I23" s="220"/>
       <c r="J23" s="154"/>
       <c r="K23" s="37"/>
       <c r="L23" s="3"/>
@@ -6130,7 +6130,7 @@
       <c r="Y23" s="118"/>
     </row>
     <row r="24" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="217"/>
+      <c r="B24" s="220"/>
       <c r="C24" s="165">
         <v>45106</v>
       </c>
@@ -6138,10 +6138,10 @@
         <v>59417.41</v>
       </c>
       <c r="E24" s="168" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F24" s="187"/>
-      <c r="I24" s="217"/>
+      <c r="I24" s="220"/>
       <c r="J24" s="154"/>
       <c r="K24" s="37"/>
       <c r="L24" s="3"/>
@@ -6156,7 +6156,7 @@
       <c r="Y24" s="118"/>
     </row>
     <row r="25" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="217"/>
+      <c r="B25" s="220"/>
       <c r="C25" s="165">
         <v>45111</v>
       </c>
@@ -6164,10 +6164,10 @@
         <v>14034.04</v>
       </c>
       <c r="E25" s="168" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F25" s="187"/>
-      <c r="I25" s="217"/>
+      <c r="I25" s="220"/>
       <c r="J25" s="154"/>
       <c r="K25" s="37"/>
       <c r="L25" s="3"/>
@@ -6182,7 +6182,7 @@
       <c r="Y25" s="118"/>
     </row>
     <row r="26" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="217"/>
+      <c r="B26" s="220"/>
       <c r="C26" s="176">
         <v>45111</v>
       </c>
@@ -6190,10 +6190,10 @@
         <v>11732.11</v>
       </c>
       <c r="E26" s="168" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F26" s="187"/>
-      <c r="I26" s="217"/>
+      <c r="I26" s="220"/>
       <c r="J26" s="176"/>
       <c r="K26" s="37"/>
       <c r="L26" s="3"/>
@@ -6208,7 +6208,7 @@
       <c r="Y26" s="118"/>
     </row>
     <row r="27" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="217"/>
+      <c r="B27" s="220"/>
       <c r="C27" s="176">
         <v>45111</v>
       </c>
@@ -6216,10 +6216,10 @@
         <v>33455</v>
       </c>
       <c r="E27" s="168" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F27" s="187"/>
-      <c r="I27" s="217"/>
+      <c r="I27" s="220"/>
       <c r="J27" s="176"/>
       <c r="K27" s="37"/>
       <c r="L27" s="3"/>
@@ -6234,7 +6234,7 @@
       <c r="Y27" s="118"/>
     </row>
     <row r="28" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="217"/>
+      <c r="B28" s="220"/>
       <c r="C28" s="176">
         <v>45111</v>
       </c>
@@ -6242,10 +6242,10 @@
         <v>177734.22</v>
       </c>
       <c r="E28" s="168" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="187"/>
-      <c r="I28" s="217"/>
+      <c r="I28" s="220"/>
       <c r="J28" s="176"/>
       <c r="K28" s="37"/>
       <c r="L28" s="3"/>
@@ -6260,7 +6260,7 @@
       <c r="Y28" s="118"/>
     </row>
     <row r="29" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="217"/>
+      <c r="B29" s="220"/>
       <c r="C29" s="188">
         <v>45115</v>
       </c>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="E29" s="168"/>
       <c r="F29" s="187"/>
-      <c r="I29" s="217"/>
+      <c r="I29" s="220"/>
       <c r="J29" s="176"/>
       <c r="K29" s="37"/>
       <c r="L29" s="3"/>
@@ -6284,12 +6284,12 @@
       <c r="Y29" s="118"/>
     </row>
     <row r="30" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="217"/>
+      <c r="B30" s="220"/>
       <c r="C30" s="176"/>
       <c r="D30" s="37"/>
       <c r="E30" s="168"/>
       <c r="F30" s="187"/>
-      <c r="I30" s="217"/>
+      <c r="I30" s="220"/>
       <c r="J30" s="176"/>
       <c r="K30" s="37"/>
       <c r="L30" s="3"/>
@@ -6304,12 +6304,12 @@
       <c r="Y30" s="118"/>
     </row>
     <row r="31" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="217"/>
+      <c r="B31" s="220"/>
       <c r="C31" s="176"/>
       <c r="D31" s="37"/>
       <c r="E31" s="168"/>
       <c r="F31" s="187"/>
-      <c r="I31" s="217"/>
+      <c r="I31" s="220"/>
       <c r="J31" s="176"/>
       <c r="K31" s="37"/>
       <c r="L31" s="3"/>
@@ -6324,12 +6324,12 @@
       <c r="Y31" s="118"/>
     </row>
     <row r="32" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="217"/>
+      <c r="B32" s="220"/>
       <c r="C32" s="176"/>
       <c r="D32" s="37"/>
       <c r="E32" s="168"/>
       <c r="F32" s="187"/>
-      <c r="I32" s="217"/>
+      <c r="I32" s="220"/>
       <c r="J32" s="176"/>
       <c r="K32" s="37"/>
       <c r="L32" s="3"/>
@@ -6344,12 +6344,12 @@
       <c r="Y32" s="118"/>
     </row>
     <row r="33" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="217"/>
+      <c r="B33" s="220"/>
       <c r="C33" s="176"/>
       <c r="D33" s="37"/>
       <c r="E33" s="168"/>
       <c r="F33" s="187"/>
-      <c r="I33" s="217"/>
+      <c r="I33" s="220"/>
       <c r="J33" s="176"/>
       <c r="K33" s="37"/>
       <c r="L33" s="3"/>
@@ -6364,12 +6364,12 @@
       <c r="Y33" s="118"/>
     </row>
     <row r="34" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="217"/>
+      <c r="B34" s="220"/>
       <c r="C34" s="176"/>
       <c r="D34" s="37"/>
       <c r="E34" s="168"/>
       <c r="F34" s="187"/>
-      <c r="I34" s="217"/>
+      <c r="I34" s="220"/>
       <c r="J34" s="176"/>
       <c r="K34" s="37"/>
       <c r="L34" s="3"/>
@@ -6384,12 +6384,12 @@
       <c r="Y34" s="118"/>
     </row>
     <row r="35" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="217"/>
+      <c r="B35" s="220"/>
       <c r="C35" s="176"/>
       <c r="D35" s="37"/>
       <c r="E35" s="168"/>
       <c r="F35" s="187"/>
-      <c r="I35" s="217"/>
+      <c r="I35" s="220"/>
       <c r="J35" s="176"/>
       <c r="K35" s="37"/>
       <c r="L35" s="3"/>
@@ -6404,12 +6404,12 @@
       <c r="Y35" s="118"/>
     </row>
     <row r="36" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="217"/>
+      <c r="B36" s="220"/>
       <c r="C36" s="176"/>
       <c r="D36" s="37"/>
       <c r="E36" s="168"/>
       <c r="F36" s="187"/>
-      <c r="I36" s="217"/>
+      <c r="I36" s="220"/>
       <c r="J36" s="176"/>
       <c r="K36" s="37"/>
       <c r="L36" s="3"/>
@@ -6424,12 +6424,12 @@
       <c r="Y36" s="118"/>
     </row>
     <row r="37" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="217"/>
+      <c r="B37" s="220"/>
       <c r="C37" s="165"/>
       <c r="D37" s="37"/>
       <c r="E37" s="168"/>
       <c r="F37" s="187"/>
-      <c r="I37" s="217"/>
+      <c r="I37" s="220"/>
       <c r="J37" s="154"/>
       <c r="K37" s="37"/>
       <c r="L37" s="3"/>
@@ -6444,7 +6444,7 @@
       <c r="Y37" s="118"/>
     </row>
     <row r="38" spans="2:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="218"/>
+      <c r="B38" s="221"/>
       <c r="C38" s="158" t="s">
         <v>3</v>
       </c>
@@ -6452,7 +6452,7 @@
         <f>SUM(D5:D37)</f>
         <v>2637197.3400000003</v>
       </c>
-      <c r="I38" s="218"/>
+      <c r="I38" s="221"/>
       <c r="J38" s="158" t="s">
         <v>3</v>
       </c>
@@ -6614,20 +6614,20 @@
       <c r="D48" s="171">
         <v>29450</v>
       </c>
-      <c r="E48" s="214" t="s">
+      <c r="E48" s="228" t="s">
         <v>100</v>
       </c>
-      <c r="F48" s="214"/>
-      <c r="G48" s="214"/>
-      <c r="H48" s="214"/>
-      <c r="I48" s="214"/>
-      <c r="J48" s="214"/>
-      <c r="K48" s="214"/>
-      <c r="L48" s="214"/>
-      <c r="M48" s="214"/>
-      <c r="N48" s="214"/>
-      <c r="O48" s="214"/>
-      <c r="P48" s="214"/>
+      <c r="F48" s="228"/>
+      <c r="G48" s="228"/>
+      <c r="H48" s="228"/>
+      <c r="I48" s="228"/>
+      <c r="J48" s="228"/>
+      <c r="K48" s="228"/>
+      <c r="L48" s="228"/>
+      <c r="M48" s="228"/>
+      <c r="N48" s="228"/>
+      <c r="O48" s="228"/>
+      <c r="P48" s="228"/>
     </row>
     <row r="49" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="175" t="s">
@@ -6635,54 +6635,54 @@
       </c>
       <c r="C49" s="172"/>
       <c r="D49" s="173"/>
-      <c r="E49" s="214"/>
-      <c r="F49" s="214"/>
-      <c r="G49" s="214"/>
-      <c r="H49" s="214"/>
-      <c r="I49" s="214"/>
-      <c r="J49" s="214"/>
-      <c r="K49" s="214"/>
-      <c r="L49" s="214"/>
-      <c r="M49" s="214"/>
-      <c r="N49" s="214"/>
-      <c r="O49" s="214"/>
-      <c r="P49" s="214"/>
+      <c r="E49" s="228"/>
+      <c r="F49" s="228"/>
+      <c r="G49" s="228"/>
+      <c r="H49" s="228"/>
+      <c r="I49" s="228"/>
+      <c r="J49" s="228"/>
+      <c r="K49" s="228"/>
+      <c r="L49" s="228"/>
+      <c r="M49" s="228"/>
+      <c r="N49" s="228"/>
+      <c r="O49" s="228"/>
+      <c r="P49" s="228"/>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="172"/>
       <c r="C50" s="172"/>
       <c r="D50" s="173"/>
-      <c r="E50" s="214"/>
-      <c r="F50" s="214"/>
-      <c r="G50" s="214"/>
-      <c r="H50" s="214"/>
-      <c r="I50" s="214"/>
-      <c r="J50" s="214"/>
-      <c r="K50" s="214"/>
-      <c r="L50" s="214"/>
-      <c r="M50" s="214"/>
-      <c r="N50" s="214"/>
-      <c r="O50" s="214"/>
-      <c r="P50" s="214"/>
+      <c r="E50" s="228"/>
+      <c r="F50" s="228"/>
+      <c r="G50" s="228"/>
+      <c r="H50" s="228"/>
+      <c r="I50" s="228"/>
+      <c r="J50" s="228"/>
+      <c r="K50" s="228"/>
+      <c r="L50" s="228"/>
+      <c r="M50" s="228"/>
+      <c r="N50" s="228"/>
+      <c r="O50" s="228"/>
+      <c r="P50" s="228"/>
     </row>
     <row r="51" spans="2:25" ht="21" x14ac:dyDescent="0.35">
       <c r="B51" s="172"/>
       <c r="C51" s="172"/>
       <c r="D51" s="173"/>
-      <c r="E51" s="215" t="s">
+      <c r="E51" s="229" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="215"/>
-      <c r="G51" s="215"/>
-      <c r="H51" s="215"/>
-      <c r="I51" s="215"/>
-      <c r="J51" s="215"/>
-      <c r="K51" s="215"/>
-      <c r="L51" s="215"/>
-      <c r="M51" s="215"/>
-      <c r="N51" s="215"/>
-      <c r="O51" s="215"/>
-      <c r="P51" s="215"/>
+      <c r="F51" s="229"/>
+      <c r="G51" s="229"/>
+      <c r="H51" s="229"/>
+      <c r="I51" s="229"/>
+      <c r="J51" s="229"/>
+      <c r="K51" s="229"/>
+      <c r="L51" s="229"/>
+      <c r="M51" s="229"/>
+      <c r="N51" s="229"/>
+      <c r="O51" s="229"/>
+      <c r="P51" s="229"/>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B54" s="118"/>
@@ -6920,6 +6920,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E48:P50"/>
+    <mergeCell ref="E51:P51"/>
+    <mergeCell ref="B2:B38"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:E3"/>
     <mergeCell ref="W9:Y10"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="W3:Y3"/>
@@ -6930,11 +6935,6 @@
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="P2:P22"/>
     <mergeCell ref="V2:V19"/>
-    <mergeCell ref="E48:P50"/>
-    <mergeCell ref="E51:P51"/>
-    <mergeCell ref="B2:B38"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8470,7 +8470,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="222" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="239" t="s">
@@ -8480,13 +8480,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="225"/>
+      <c r="B3" s="223"/>
       <c r="C3" s="190"/>
       <c r="D3" s="190"/>
       <c r="E3" s="191"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="226"/>
+      <c r="B4" s="224"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
CIERRE 1 SEPT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
+++ b/01 DOCUEMENTOS/ARQUITECTO RODOLFO ---2021--2018.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="139">
   <si>
     <t xml:space="preserve">PAGOS  SOBRE REMODELACION </t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>AZULEJOS BAÑOS EXTERIOR  HOMBRES OBRADOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOME DEPOT </t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1688,6 +1694,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1712,21 +1733,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1754,6 +1760,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1763,9 +1787,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="19" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1778,15 +1799,6 @@
     <xf numFmtId="15" fontId="19" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1796,11 +1808,23 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1811,24 +1835,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1870,6 +1876,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4090,18 +4099,18 @@
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
-      <c r="C3" s="244" t="s">
+      <c r="C3" s="234" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="244"/>
+      <c r="D3" s="234"/>
       <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-      <c r="C4" s="235" t="s">
+      <c r="C4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="235"/>
+      <c r="D4" s="240"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4111,10 +4120,10 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="245" t="s">
+      <c r="B6" s="235" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="246"/>
+      <c r="C6" s="236"/>
       <c r="D6" s="37">
         <v>1064853</v>
       </c>
@@ -4131,10 +4140,10 @@
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="242" t="s">
+      <c r="B8" s="237" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="243"/>
+      <c r="C8" s="238"/>
       <c r="D8" s="37">
         <v>382873</v>
       </c>
@@ -4151,10 +4160,10 @@
       <c r="E9" s="51"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="242" t="s">
+      <c r="B10" s="237" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="243"/>
+      <c r="C10" s="238"/>
       <c r="D10" s="37">
         <v>554226</v>
       </c>
@@ -4171,10 +4180,10 @@
       <c r="E11" s="51"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="242" t="s">
+      <c r="B12" s="237" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="243"/>
+      <c r="C12" s="238"/>
       <c r="D12" s="37">
         <v>873457</v>
       </c>
@@ -4191,10 +4200,10 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="242" t="s">
+      <c r="B14" s="237" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="243"/>
+      <c r="C14" s="238"/>
       <c r="D14" s="37">
         <v>108040</v>
       </c>
@@ -4211,10 +4220,10 @@
       <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="236" t="s">
+      <c r="B16" s="241" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="237"/>
+      <c r="C16" s="242"/>
       <c r="D16" s="37">
         <v>451709</v>
       </c>
@@ -4231,14 +4240,14 @@
       <c r="E17" s="27"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="236" t="s">
+      <c r="B18" s="241" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="237"/>
+      <c r="C18" s="242"/>
       <c r="D18" s="39">
         <v>828541</v>
       </c>
-      <c r="E18" s="238" t="s">
+      <c r="E18" s="243" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4248,7 +4257,7 @@
       <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="239"/>
+      <c r="E19" s="244"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -4259,10 +4268,10 @@
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="236" t="s">
+      <c r="B21" s="241" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="237"/>
+      <c r="C21" s="242"/>
       <c r="D21" s="39">
         <v>70000</v>
       </c>
@@ -4279,10 +4288,10 @@
       <c r="E22" s="52"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="240" t="s">
+      <c r="B23" s="245" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="241"/>
+      <c r="C23" s="246"/>
       <c r="D23" s="39">
         <v>748884</v>
       </c>
@@ -4299,10 +4308,10 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="234" t="s">
+      <c r="B25" s="239" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="234"/>
+      <c r="C25" s="239"/>
       <c r="D25" s="37">
         <v>99356</v>
       </c>
@@ -4353,11 +4362,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B16:C16"/>
@@ -4366,6 +4370,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5931,98 +5940,98 @@
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:33" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="264" t="s">
+      <c r="B2" s="258" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="259" t="s">
+      <c r="C2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="259"/>
+      <c r="D2" s="261"/>
       <c r="E2" s="17"/>
-      <c r="I2" s="264" t="s">
+      <c r="I2" s="258" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="259" t="s">
+      <c r="J2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="259"/>
+      <c r="K2" s="261"/>
       <c r="L2" s="17"/>
-      <c r="P2" s="264" t="s">
+      <c r="P2" s="258" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="259" t="s">
+      <c r="Q2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="259"/>
+      <c r="R2" s="261"/>
       <c r="S2" s="17"/>
       <c r="T2" s="166"/>
-      <c r="X2" s="267" t="s">
+      <c r="X2" s="269" t="s">
         <v>92</v>
       </c>
-      <c r="Y2" s="259" t="s">
+      <c r="Y2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="259"/>
+      <c r="Z2" s="261"/>
       <c r="AA2" s="17"/>
-      <c r="AD2" s="256" t="s">
+      <c r="AD2" s="262" t="s">
         <v>94</v>
       </c>
-      <c r="AE2" s="259" t="s">
+      <c r="AE2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" s="259"/>
+      <c r="AF2" s="261"/>
       <c r="AG2" s="17"/>
     </row>
     <row r="3" spans="2:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="265"/>
+      <c r="B3" s="259"/>
       <c r="C3" s="232"/>
       <c r="D3" s="232"/>
       <c r="E3" s="233"/>
-      <c r="I3" s="265"/>
+      <c r="I3" s="259"/>
       <c r="J3" s="232"/>
       <c r="K3" s="232"/>
       <c r="L3" s="233"/>
-      <c r="P3" s="265"/>
+      <c r="P3" s="259"/>
       <c r="Q3" s="232"/>
       <c r="R3" s="232"/>
       <c r="S3" s="233"/>
       <c r="T3" s="166"/>
-      <c r="X3" s="268"/>
+      <c r="X3" s="270"/>
       <c r="Y3" s="232"/>
       <c r="Z3" s="232"/>
       <c r="AA3" s="233"/>
-      <c r="AD3" s="257"/>
+      <c r="AD3" s="263"/>
       <c r="AE3" s="232"/>
       <c r="AF3" s="232"/>
       <c r="AG3" s="233"/>
     </row>
     <row r="4" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="265"/>
+      <c r="B4" s="259"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="265"/>
+      <c r="I4" s="259"/>
       <c r="J4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="23"/>
-      <c r="P4" s="265"/>
+      <c r="P4" s="259"/>
       <c r="Q4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="R4" s="22"/>
       <c r="S4" s="23"/>
       <c r="T4" s="166"/>
-      <c r="X4" s="268"/>
+      <c r="X4" s="270"/>
       <c r="Y4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="Z4" s="22"/>
       <c r="AA4" s="23"/>
-      <c r="AD4" s="257"/>
+      <c r="AD4" s="263"/>
       <c r="AE4" s="21" t="s">
         <v>2</v>
       </c>
@@ -6030,7 +6039,7 @@
       <c r="AG4" s="23"/>
     </row>
     <row r="5" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="265"/>
+      <c r="B5" s="259"/>
       <c r="C5" s="203" t="s">
         <v>80</v>
       </c>
@@ -6038,7 +6047,7 @@
         <v>563480</v>
       </c>
       <c r="E5" s="28"/>
-      <c r="I5" s="265"/>
+      <c r="I5" s="259"/>
       <c r="J5" s="155" t="s">
         <v>80</v>
       </c>
@@ -6046,7 +6055,7 @@
         <v>563480</v>
       </c>
       <c r="L5" s="28"/>
-      <c r="P5" s="265"/>
+      <c r="P5" s="259"/>
       <c r="Q5" s="155">
         <v>45010</v>
       </c>
@@ -6055,7 +6064,7 @@
       </c>
       <c r="S5" s="28"/>
       <c r="T5" s="166"/>
-      <c r="X5" s="268"/>
+      <c r="X5" s="270"/>
       <c r="Y5" s="155">
         <v>44947</v>
       </c>
@@ -6063,7 +6072,7 @@
         <v>50000</v>
       </c>
       <c r="AA5" s="28"/>
-      <c r="AD5" s="257"/>
+      <c r="AD5" s="263"/>
       <c r="AE5" s="155">
         <v>44873</v>
       </c>
@@ -6073,7 +6082,7 @@
       <c r="AG5" s="28"/>
     </row>
     <row r="6" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="265"/>
+      <c r="B6" s="259"/>
       <c r="C6" s="155">
         <v>45010</v>
       </c>
@@ -6081,7 +6090,7 @@
         <v>50000</v>
       </c>
       <c r="E6" s="27"/>
-      <c r="I6" s="265"/>
+      <c r="I6" s="259"/>
       <c r="J6" s="155">
         <v>45010</v>
       </c>
@@ -6089,7 +6098,7 @@
         <v>50000</v>
       </c>
       <c r="L6" s="27"/>
-      <c r="P6" s="265"/>
+      <c r="P6" s="259"/>
       <c r="Q6" s="197">
         <v>45017</v>
       </c>
@@ -6098,7 +6107,7 @@
       </c>
       <c r="S6" s="27"/>
       <c r="T6" s="166"/>
-      <c r="X6" s="268"/>
+      <c r="X6" s="270"/>
       <c r="Y6" s="197">
         <v>44954</v>
       </c>
@@ -6106,13 +6115,13 @@
         <v>50000</v>
       </c>
       <c r="AA6" s="27"/>
-      <c r="AD6" s="257"/>
+      <c r="AD6" s="263"/>
       <c r="AE6" s="197"/>
       <c r="AF6" s="37"/>
       <c r="AG6" s="27"/>
     </row>
     <row r="7" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="265"/>
+      <c r="B7" s="259"/>
       <c r="C7" s="225">
         <v>45017</v>
       </c>
@@ -6120,7 +6129,7 @@
         <v>100000</v>
       </c>
       <c r="E7" s="41"/>
-      <c r="I7" s="265"/>
+      <c r="I7" s="259"/>
       <c r="J7" s="197">
         <v>45017</v>
       </c>
@@ -6128,7 +6137,7 @@
         <v>100000</v>
       </c>
       <c r="L7" s="41"/>
-      <c r="P7" s="265"/>
+      <c r="P7" s="259"/>
       <c r="Q7" s="197">
         <v>45021</v>
       </c>
@@ -6137,7 +6146,7 @@
       </c>
       <c r="S7" s="41"/>
       <c r="T7" s="166"/>
-      <c r="X7" s="268"/>
+      <c r="X7" s="270"/>
       <c r="Y7" s="197">
         <v>44961</v>
       </c>
@@ -6145,13 +6154,13 @@
         <v>50000</v>
       </c>
       <c r="AA7" s="41"/>
-      <c r="AD7" s="257"/>
+      <c r="AD7" s="263"/>
       <c r="AE7" s="197"/>
       <c r="AF7" s="37"/>
       <c r="AG7" s="41"/>
     </row>
     <row r="8" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="265"/>
+      <c r="B8" s="259"/>
       <c r="C8" s="225">
         <v>45021</v>
       </c>
@@ -6159,7 +6168,7 @@
         <v>50000</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="I8" s="265"/>
+      <c r="I8" s="259"/>
       <c r="J8" s="197">
         <v>45021</v>
       </c>
@@ -6167,7 +6176,7 @@
         <v>50000</v>
       </c>
       <c r="L8" s="27"/>
-      <c r="P8" s="265"/>
+      <c r="P8" s="259"/>
       <c r="Q8" s="197">
         <v>45031</v>
       </c>
@@ -6176,7 +6185,7 @@
       </c>
       <c r="S8" s="27"/>
       <c r="T8" s="166"/>
-      <c r="X8" s="268"/>
+      <c r="X8" s="270"/>
       <c r="Y8" s="197">
         <v>44968</v>
       </c>
@@ -6184,13 +6193,13 @@
         <v>50000</v>
       </c>
       <c r="AA8" s="27"/>
-      <c r="AD8" s="257"/>
+      <c r="AD8" s="263"/>
       <c r="AE8" s="197"/>
       <c r="AF8" s="37"/>
       <c r="AG8" s="27"/>
     </row>
     <row r="9" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="265"/>
+      <c r="B9" s="259"/>
       <c r="C9" s="225">
         <v>45031</v>
       </c>
@@ -6198,7 +6207,7 @@
         <v>100000</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="I9" s="265"/>
+      <c r="I9" s="259"/>
       <c r="J9" s="197">
         <v>45031</v>
       </c>
@@ -6206,7 +6215,7 @@
         <v>100000</v>
       </c>
       <c r="L9" s="27"/>
-      <c r="P9" s="265"/>
+      <c r="P9" s="259"/>
       <c r="Q9" s="156">
         <v>45038</v>
       </c>
@@ -6215,7 +6224,7 @@
       </c>
       <c r="S9" s="27"/>
       <c r="T9" s="166"/>
-      <c r="X9" s="268"/>
+      <c r="X9" s="270"/>
       <c r="Y9" s="156">
         <v>44975</v>
       </c>
@@ -6223,15 +6232,15 @@
         <v>50000</v>
       </c>
       <c r="AA9" s="27"/>
-      <c r="AD9" s="257"/>
-      <c r="AE9" s="260" t="s">
+      <c r="AD9" s="263"/>
+      <c r="AE9" s="265" t="s">
         <v>95</v>
       </c>
-      <c r="AF9" s="260"/>
-      <c r="AG9" s="261"/>
+      <c r="AF9" s="265"/>
+      <c r="AG9" s="266"/>
     </row>
     <row r="10" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="265"/>
+      <c r="B10" s="259"/>
       <c r="C10" s="156">
         <v>45038</v>
       </c>
@@ -6239,7 +6248,7 @@
         <v>50000</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="I10" s="265"/>
+      <c r="I10" s="259"/>
       <c r="J10" s="156">
         <v>45038</v>
       </c>
@@ -6247,7 +6256,7 @@
         <v>50000</v>
       </c>
       <c r="L10" s="27"/>
-      <c r="P10" s="265"/>
+      <c r="P10" s="259"/>
       <c r="Q10" s="156">
         <v>45045</v>
       </c>
@@ -6256,7 +6265,7 @@
       </c>
       <c r="S10" s="27"/>
       <c r="T10" s="166"/>
-      <c r="X10" s="268"/>
+      <c r="X10" s="270"/>
       <c r="Y10" s="156">
         <v>44982</v>
       </c>
@@ -6264,13 +6273,13 @@
         <v>50000</v>
       </c>
       <c r="AA10" s="27"/>
-      <c r="AD10" s="257"/>
-      <c r="AE10" s="262"/>
-      <c r="AF10" s="262"/>
-      <c r="AG10" s="263"/>
+      <c r="AD10" s="263"/>
+      <c r="AE10" s="267"/>
+      <c r="AF10" s="267"/>
+      <c r="AG10" s="268"/>
     </row>
     <row r="11" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="265"/>
+      <c r="B11" s="259"/>
       <c r="C11" s="156">
         <v>45045</v>
       </c>
@@ -6278,7 +6287,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="I11" s="265"/>
+      <c r="I11" s="259"/>
       <c r="J11" s="156">
         <v>45045</v>
       </c>
@@ -6286,7 +6295,7 @@
         <v>100000</v>
       </c>
       <c r="L11" s="27"/>
-      <c r="P11" s="265"/>
+      <c r="P11" s="259"/>
       <c r="Q11" s="156">
         <v>45052</v>
       </c>
@@ -6295,7 +6304,7 @@
       </c>
       <c r="S11" s="27"/>
       <c r="T11" s="166"/>
-      <c r="X11" s="268"/>
+      <c r="X11" s="270"/>
       <c r="Y11" s="156">
         <v>44989</v>
       </c>
@@ -6303,13 +6312,13 @@
         <v>50000</v>
       </c>
       <c r="AA11" s="27"/>
-      <c r="AD11" s="257"/>
+      <c r="AD11" s="263"/>
       <c r="AE11" s="156"/>
       <c r="AF11" s="77"/>
       <c r="AG11" s="27"/>
     </row>
     <row r="12" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="265"/>
+      <c r="B12" s="259"/>
       <c r="C12" s="156">
         <v>45052</v>
       </c>
@@ -6317,7 +6326,7 @@
         <v>100000</v>
       </c>
       <c r="E12" s="146"/>
-      <c r="I12" s="265"/>
+      <c r="I12" s="259"/>
       <c r="J12" s="156">
         <v>45052</v>
       </c>
@@ -6325,7 +6334,7 @@
         <v>100000</v>
       </c>
       <c r="L12" s="146"/>
-      <c r="P12" s="265"/>
+      <c r="P12" s="259"/>
       <c r="Q12" s="157">
         <v>45059</v>
       </c>
@@ -6334,7 +6343,7 @@
       </c>
       <c r="S12" s="146"/>
       <c r="T12" s="166"/>
-      <c r="X12" s="268"/>
+      <c r="X12" s="270"/>
       <c r="Y12" s="157">
         <v>44989</v>
       </c>
@@ -6342,7 +6351,7 @@
         <v>50000</v>
       </c>
       <c r="AA12" s="146"/>
-      <c r="AD12" s="257"/>
+      <c r="AD12" s="263"/>
       <c r="AE12" s="197"/>
       <c r="AF12" s="37">
         <v>0</v>
@@ -6350,7 +6359,7 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="265"/>
+      <c r="B13" s="259"/>
       <c r="C13" s="157">
         <v>45059</v>
       </c>
@@ -6358,7 +6367,7 @@
         <v>100000</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="I13" s="265"/>
+      <c r="I13" s="259"/>
       <c r="J13" s="157">
         <v>45059</v>
       </c>
@@ -6366,12 +6375,12 @@
         <v>100000</v>
       </c>
       <c r="L13" s="3"/>
-      <c r="P13" s="265"/>
+      <c r="P13" s="259"/>
       <c r="Q13" s="197"/>
       <c r="R13" s="37"/>
       <c r="S13" s="3"/>
       <c r="T13" s="166"/>
-      <c r="X13" s="268"/>
+      <c r="X13" s="270"/>
       <c r="Y13" s="197">
         <v>44996</v>
       </c>
@@ -6379,13 +6388,13 @@
         <v>50000</v>
       </c>
       <c r="AA13" s="3"/>
-      <c r="AD13" s="257"/>
+      <c r="AD13" s="263"/>
       <c r="AE13" s="197"/>
       <c r="AF13" s="37"/>
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="265"/>
+      <c r="B14" s="259"/>
       <c r="C14" s="225">
         <v>45066</v>
       </c>
@@ -6393,7 +6402,7 @@
         <v>100000</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="I14" s="265"/>
+      <c r="I14" s="259"/>
       <c r="J14" s="197">
         <v>45066</v>
       </c>
@@ -6401,12 +6410,12 @@
         <v>100000</v>
       </c>
       <c r="L14" s="3"/>
-      <c r="P14" s="265"/>
+      <c r="P14" s="259"/>
       <c r="Q14" s="197"/>
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="166"/>
-      <c r="X14" s="268"/>
+      <c r="X14" s="270"/>
       <c r="Y14" s="197">
         <v>45003</v>
       </c>
@@ -6414,13 +6423,13 @@
         <v>113480</v>
       </c>
       <c r="AA14" s="3"/>
-      <c r="AD14" s="257"/>
+      <c r="AD14" s="263"/>
       <c r="AE14" s="197"/>
       <c r="AF14" s="37"/>
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="265"/>
+      <c r="B15" s="259"/>
       <c r="C15" s="225">
         <v>45073</v>
       </c>
@@ -6428,7 +6437,7 @@
         <v>100000</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="I15" s="265"/>
+      <c r="I15" s="259"/>
       <c r="J15" s="197">
         <v>45073</v>
       </c>
@@ -6436,18 +6445,18 @@
         <v>100000</v>
       </c>
       <c r="L15" s="3"/>
-      <c r="P15" s="265"/>
+      <c r="P15" s="259"/>
       <c r="Q15" s="197"/>
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="166"/>
-      <c r="X15" s="268"/>
+      <c r="X15" s="270"/>
       <c r="Y15" s="197"/>
       <c r="Z15" s="37">
         <v>0</v>
       </c>
       <c r="AA15" s="3"/>
-      <c r="AD15" s="257"/>
+      <c r="AD15" s="263"/>
       <c r="AE15" s="158" t="s">
         <v>3</v>
       </c>
@@ -6457,7 +6466,7 @@
       </c>
     </row>
     <row r="16" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="265"/>
+      <c r="B16" s="259"/>
       <c r="C16" s="225">
         <v>45079</v>
       </c>
@@ -6465,7 +6474,7 @@
         <v>100000</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="I16" s="265"/>
+      <c r="I16" s="259"/>
       <c r="J16" s="197">
         <v>45079</v>
       </c>
@@ -6473,18 +6482,18 @@
         <v>100000</v>
       </c>
       <c r="L16" s="3"/>
-      <c r="P16" s="265"/>
+      <c r="P16" s="259"/>
       <c r="Q16" s="197"/>
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="166"/>
-      <c r="X16" s="268"/>
+      <c r="X16" s="270"/>
       <c r="Y16" s="197"/>
       <c r="Z16" s="37">
         <v>0</v>
       </c>
       <c r="AA16" s="3"/>
-      <c r="AD16" s="257"/>
+      <c r="AD16" s="263"/>
       <c r="AE16" s="121"/>
       <c r="AF16" s="49">
         <v>67769</v>
@@ -6494,7 +6503,7 @@
       </c>
     </row>
     <row r="17" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="265"/>
+      <c r="B17" s="259"/>
       <c r="C17" s="225">
         <v>45092</v>
       </c>
@@ -6502,7 +6511,7 @@
         <v>100000</v>
       </c>
       <c r="E17" s="168"/>
-      <c r="I17" s="265"/>
+      <c r="I17" s="259"/>
       <c r="J17" s="197">
         <v>45086</v>
       </c>
@@ -6512,12 +6521,12 @@
       <c r="L17" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="P17" s="265"/>
+      <c r="P17" s="259"/>
       <c r="Q17" s="197"/>
       <c r="R17" s="37"/>
       <c r="S17" s="3"/>
       <c r="T17" s="166"/>
-      <c r="X17" s="268"/>
+      <c r="X17" s="270"/>
       <c r="Y17" s="184" t="s">
         <v>3</v>
       </c>
@@ -6525,7 +6534,7 @@
         <f>SUM(Z5:Z16)</f>
         <v>563480</v>
       </c>
-      <c r="AD17" s="257"/>
+      <c r="AD17" s="263"/>
       <c r="AE17" s="65"/>
       <c r="AF17" s="49">
         <v>0</v>
@@ -6533,7 +6542,7 @@
       <c r="AG17" s="124"/>
     </row>
     <row r="18" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="265"/>
+      <c r="B18" s="259"/>
       <c r="C18" s="225">
         <v>45101</v>
       </c>
@@ -6541,7 +6550,7 @@
         <v>100000</v>
       </c>
       <c r="E18" s="168"/>
-      <c r="I18" s="265"/>
+      <c r="I18" s="259"/>
       <c r="J18" s="197">
         <v>45090</v>
       </c>
@@ -6551,12 +6560,12 @@
       <c r="L18" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="P18" s="265"/>
+      <c r="P18" s="259"/>
       <c r="Q18" s="197"/>
       <c r="R18" s="37"/>
       <c r="S18" s="3"/>
       <c r="T18" s="166"/>
-      <c r="X18" s="268"/>
+      <c r="X18" s="270"/>
       <c r="Y18" s="160"/>
       <c r="Z18" s="161">
         <v>-563480</v>
@@ -6564,14 +6573,14 @@
       <c r="AA18" s="152">
         <v>44947</v>
       </c>
-      <c r="AD18" s="257"/>
+      <c r="AD18" s="263"/>
       <c r="AE18" s="84"/>
       <c r="AF18" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="265"/>
+      <c r="B19" s="259"/>
       <c r="C19" s="225">
         <v>45108</v>
       </c>
@@ -6579,7 +6588,7 @@
         <v>100000</v>
       </c>
       <c r="E19" s="168"/>
-      <c r="I19" s="265"/>
+      <c r="I19" s="259"/>
       <c r="J19" s="197">
         <v>45091</v>
       </c>
@@ -6589,18 +6598,18 @@
       <c r="L19" s="169" t="s">
         <v>98</v>
       </c>
-      <c r="P19" s="265"/>
+      <c r="P19" s="259"/>
       <c r="Q19" s="197"/>
       <c r="R19" s="37"/>
       <c r="S19" s="3"/>
       <c r="T19" s="166"/>
-      <c r="X19" s="268"/>
+      <c r="X19" s="270"/>
       <c r="Y19" s="162"/>
       <c r="Z19" s="161">
         <v>0</v>
       </c>
       <c r="AA19" s="124"/>
-      <c r="AD19" s="258"/>
+      <c r="AD19" s="264"/>
       <c r="AE19" s="185" t="s">
         <v>4</v>
       </c>
@@ -6610,7 +6619,7 @@
       </c>
     </row>
     <row r="20" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="265"/>
+      <c r="B20" s="259"/>
       <c r="C20" s="225">
         <v>45115</v>
       </c>
@@ -6618,7 +6627,7 @@
         <v>100000</v>
       </c>
       <c r="E20" s="168"/>
-      <c r="I20" s="265"/>
+      <c r="I20" s="259"/>
       <c r="J20" s="197">
         <v>45091</v>
       </c>
@@ -6628,12 +6637,12 @@
       <c r="L20" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="P20" s="265"/>
+      <c r="P20" s="259"/>
       <c r="Q20" s="197"/>
       <c r="R20" s="37"/>
       <c r="S20" s="3"/>
       <c r="T20" s="166"/>
-      <c r="X20" s="268"/>
+      <c r="X20" s="270"/>
       <c r="Y20" s="163"/>
       <c r="Z20" s="164">
         <v>0</v>
@@ -6644,7 +6653,7 @@
       <c r="AG20" s="118"/>
     </row>
     <row r="21" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="265"/>
+      <c r="B21" s="259"/>
       <c r="C21" s="225">
         <v>45122</v>
       </c>
@@ -6653,7 +6662,7 @@
       </c>
       <c r="E21" s="168"/>
       <c r="F21" s="187"/>
-      <c r="I21" s="265"/>
+      <c r="I21" s="259"/>
       <c r="J21" s="197">
         <v>45092</v>
       </c>
@@ -6662,12 +6671,12 @@
       </c>
       <c r="L21" s="168"/>
       <c r="M21" s="187"/>
-      <c r="P21" s="265"/>
+      <c r="P21" s="259"/>
       <c r="Q21" s="197"/>
       <c r="R21" s="37"/>
       <c r="S21" s="3"/>
       <c r="T21" s="166"/>
-      <c r="X21" s="268"/>
+      <c r="X21" s="270"/>
       <c r="Y21" s="33" t="s">
         <v>4</v>
       </c>
@@ -6681,7 +6690,7 @@
       <c r="AG21" s="118"/>
     </row>
     <row r="22" spans="2:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="265"/>
+      <c r="B22" s="259"/>
       <c r="C22" s="225">
         <v>45129</v>
       </c>
@@ -6690,7 +6699,7 @@
       </c>
       <c r="E22" s="168"/>
       <c r="F22" s="187"/>
-      <c r="I22" s="265"/>
+      <c r="I22" s="259"/>
       <c r="J22" s="197">
         <v>45101</v>
       </c>
@@ -6699,12 +6708,12 @@
       </c>
       <c r="L22" s="168"/>
       <c r="M22" s="187"/>
-      <c r="P22" s="265"/>
+      <c r="P22" s="259"/>
       <c r="Q22" s="197"/>
       <c r="R22" s="37"/>
       <c r="S22" s="3"/>
       <c r="T22" s="166"/>
-      <c r="X22" s="269"/>
+      <c r="X22" s="271"/>
       <c r="Y22" s="182"/>
       <c r="Z22" s="183"/>
       <c r="AA22" s="118"/>
@@ -6714,7 +6723,7 @@
       <c r="AG22" s="118"/>
     </row>
     <row r="23" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="265"/>
+      <c r="B23" s="259"/>
       <c r="C23" s="226">
         <v>45134</v>
       </c>
@@ -6725,7 +6734,7 @@
         <v>109</v>
       </c>
       <c r="F23" s="187"/>
-      <c r="I23" s="265"/>
+      <c r="I23" s="259"/>
       <c r="J23" s="197">
         <v>45108</v>
       </c>
@@ -6734,7 +6743,7 @@
       </c>
       <c r="L23" s="168"/>
       <c r="M23" s="187"/>
-      <c r="P23" s="265"/>
+      <c r="P23" s="259"/>
       <c r="Q23" s="197"/>
       <c r="R23" s="37"/>
       <c r="S23" s="3"/>
@@ -6749,7 +6758,7 @@
       <c r="AG23" s="118"/>
     </row>
     <row r="24" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="265"/>
+      <c r="B24" s="259"/>
       <c r="C24" s="226">
         <v>45138</v>
       </c>
@@ -6760,7 +6769,7 @@
         <v>111</v>
       </c>
       <c r="F24" s="187"/>
-      <c r="I24" s="265"/>
+      <c r="I24" s="259"/>
       <c r="J24" s="197">
         <v>45106</v>
       </c>
@@ -6771,7 +6780,7 @@
         <v>104</v>
       </c>
       <c r="M24" s="187"/>
-      <c r="P24" s="265"/>
+      <c r="P24" s="259"/>
       <c r="Q24" s="197"/>
       <c r="R24" s="37"/>
       <c r="S24" s="3"/>
@@ -6786,7 +6795,7 @@
       <c r="AG24" s="118"/>
     </row>
     <row r="25" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="265"/>
+      <c r="B25" s="259"/>
       <c r="C25" s="226">
         <v>45138</v>
       </c>
@@ -6797,7 +6806,7 @@
         <v>112</v>
       </c>
       <c r="F25" s="187"/>
-      <c r="I25" s="265"/>
+      <c r="I25" s="259"/>
       <c r="J25" s="197">
         <v>45111</v>
       </c>
@@ -6808,7 +6817,7 @@
         <v>107</v>
       </c>
       <c r="M25" s="187"/>
-      <c r="P25" s="265"/>
+      <c r="P25" s="259"/>
       <c r="Q25" s="197"/>
       <c r="R25" s="37"/>
       <c r="S25" s="3"/>
@@ -6823,7 +6832,7 @@
       <c r="AG25" s="118"/>
     </row>
     <row r="26" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="265"/>
+      <c r="B26" s="259"/>
       <c r="C26" s="226">
         <v>45138</v>
       </c>
@@ -6834,7 +6843,7 @@
         <v>113</v>
       </c>
       <c r="F26" s="187"/>
-      <c r="I26" s="265"/>
+      <c r="I26" s="259"/>
       <c r="J26" s="197">
         <v>45111</v>
       </c>
@@ -6845,7 +6854,7 @@
         <v>105</v>
       </c>
       <c r="M26" s="187"/>
-      <c r="P26" s="265"/>
+      <c r="P26" s="259"/>
       <c r="Q26" s="197"/>
       <c r="R26" s="37"/>
       <c r="S26" s="3"/>
@@ -6860,7 +6869,7 @@
       <c r="AG26" s="118"/>
     </row>
     <row r="27" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="265"/>
+      <c r="B27" s="259"/>
       <c r="C27" s="226">
         <v>45138</v>
       </c>
@@ -6871,7 +6880,7 @@
         <v>114</v>
       </c>
       <c r="F27" s="187"/>
-      <c r="I27" s="265"/>
+      <c r="I27" s="259"/>
       <c r="J27" s="197">
         <v>45111</v>
       </c>
@@ -6882,7 +6891,7 @@
         <v>103</v>
       </c>
       <c r="M27" s="187"/>
-      <c r="P27" s="265"/>
+      <c r="P27" s="259"/>
       <c r="Q27" s="197"/>
       <c r="R27" s="37"/>
       <c r="S27" s="3"/>
@@ -6897,7 +6906,7 @@
       <c r="AG27" s="118"/>
     </row>
     <row r="28" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="265"/>
+      <c r="B28" s="259"/>
       <c r="C28" s="226">
         <v>45139</v>
       </c>
@@ -6908,7 +6917,7 @@
         <v>115</v>
       </c>
       <c r="F28" s="187"/>
-      <c r="I28" s="265"/>
+      <c r="I28" s="259"/>
       <c r="J28" s="197">
         <v>45111</v>
       </c>
@@ -6919,7 +6928,7 @@
         <v>106</v>
       </c>
       <c r="M28" s="187"/>
-      <c r="P28" s="265"/>
+      <c r="P28" s="259"/>
       <c r="Q28" s="197"/>
       <c r="R28" s="37"/>
       <c r="S28" s="3"/>
@@ -6934,7 +6943,7 @@
       <c r="AG28" s="118"/>
     </row>
     <row r="29" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="265"/>
+      <c r="B29" s="259"/>
       <c r="C29" s="207">
         <v>45150</v>
       </c>
@@ -6945,7 +6954,7 @@
         <v>129</v>
       </c>
       <c r="F29" s="187"/>
-      <c r="I29" s="265"/>
+      <c r="I29" s="259"/>
       <c r="J29" s="197">
         <v>45115</v>
       </c>
@@ -6954,7 +6963,7 @@
       </c>
       <c r="L29" s="168"/>
       <c r="M29" s="187"/>
-      <c r="P29" s="265"/>
+      <c r="P29" s="259"/>
       <c r="Q29" s="197"/>
       <c r="R29" s="37"/>
       <c r="S29" s="3"/>
@@ -6969,12 +6978,12 @@
       <c r="AG29" s="118"/>
     </row>
     <row r="30" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="265"/>
+      <c r="B30" s="259"/>
       <c r="C30" s="225"/>
       <c r="D30" s="37"/>
       <c r="E30" s="168"/>
       <c r="F30" s="187"/>
-      <c r="I30" s="265"/>
+      <c r="I30" s="259"/>
       <c r="J30" s="197">
         <v>45120</v>
       </c>
@@ -6985,7 +6994,7 @@
         <v>108</v>
       </c>
       <c r="M30" s="187"/>
-      <c r="P30" s="265"/>
+      <c r="P30" s="259"/>
       <c r="Q30" s="197"/>
       <c r="R30" s="37"/>
       <c r="S30" s="3"/>
@@ -7000,12 +7009,12 @@
       <c r="AG30" s="118"/>
     </row>
     <row r="31" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="265"/>
+      <c r="B31" s="259"/>
       <c r="C31" s="225"/>
       <c r="D31" s="37"/>
       <c r="E31" s="168"/>
       <c r="F31" s="187"/>
-      <c r="I31" s="265"/>
+      <c r="I31" s="259"/>
       <c r="J31" s="197">
         <v>45122</v>
       </c>
@@ -7014,7 +7023,7 @@
       </c>
       <c r="L31" s="168"/>
       <c r="M31" s="187"/>
-      <c r="P31" s="265"/>
+      <c r="P31" s="259"/>
       <c r="Q31" s="197"/>
       <c r="R31" s="37"/>
       <c r="S31" s="3"/>
@@ -7029,12 +7038,12 @@
       <c r="AG31" s="118"/>
     </row>
     <row r="32" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="265"/>
+      <c r="B32" s="259"/>
       <c r="C32" s="225"/>
       <c r="D32" s="37"/>
       <c r="E32" s="168"/>
       <c r="F32" s="187"/>
-      <c r="I32" s="265"/>
+      <c r="I32" s="259"/>
       <c r="J32" s="197">
         <v>45129</v>
       </c>
@@ -7043,7 +7052,7 @@
       </c>
       <c r="L32" s="168"/>
       <c r="M32" s="187"/>
-      <c r="P32" s="265"/>
+      <c r="P32" s="259"/>
       <c r="Q32" s="197"/>
       <c r="R32" s="37"/>
       <c r="S32" s="3"/>
@@ -7058,12 +7067,12 @@
       <c r="AG32" s="118"/>
     </row>
     <row r="33" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="265"/>
+      <c r="B33" s="259"/>
       <c r="C33" s="225"/>
       <c r="D33" s="37"/>
       <c r="E33" s="168"/>
       <c r="F33" s="187"/>
-      <c r="I33" s="265"/>
+      <c r="I33" s="259"/>
       <c r="J33" s="197">
         <v>45134</v>
       </c>
@@ -7074,7 +7083,7 @@
         <v>109</v>
       </c>
       <c r="M33" s="187"/>
-      <c r="P33" s="265"/>
+      <c r="P33" s="259"/>
       <c r="Q33" s="197"/>
       <c r="R33" s="37"/>
       <c r="S33" s="3"/>
@@ -7089,12 +7098,12 @@
       <c r="AG33" s="118"/>
     </row>
     <row r="34" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="265"/>
+      <c r="B34" s="259"/>
       <c r="C34" s="225"/>
       <c r="D34" s="37"/>
       <c r="E34" s="168"/>
       <c r="F34" s="187"/>
-      <c r="I34" s="265"/>
+      <c r="I34" s="259"/>
       <c r="J34" s="197">
         <v>45134</v>
       </c>
@@ -7105,7 +7114,7 @@
         <v>110</v>
       </c>
       <c r="M34" s="187"/>
-      <c r="P34" s="265"/>
+      <c r="P34" s="259"/>
       <c r="Q34" s="197"/>
       <c r="R34" s="37"/>
       <c r="S34" s="3"/>
@@ -7120,12 +7129,12 @@
       <c r="AG34" s="118"/>
     </row>
     <row r="35" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="265"/>
+      <c r="B35" s="259"/>
       <c r="C35" s="225"/>
       <c r="D35" s="37"/>
       <c r="E35" s="168"/>
       <c r="F35" s="187"/>
-      <c r="I35" s="265"/>
+      <c r="I35" s="259"/>
       <c r="J35" s="197">
         <v>45136</v>
       </c>
@@ -7134,7 +7143,7 @@
       </c>
       <c r="L35" s="168"/>
       <c r="M35" s="187"/>
-      <c r="P35" s="265"/>
+      <c r="P35" s="259"/>
       <c r="Q35" s="197"/>
       <c r="R35" s="37"/>
       <c r="S35" s="3"/>
@@ -7149,12 +7158,12 @@
       <c r="AG35" s="118"/>
     </row>
     <row r="36" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="265"/>
+      <c r="B36" s="259"/>
       <c r="C36" s="225"/>
       <c r="D36" s="37"/>
       <c r="E36" s="168"/>
       <c r="F36" s="187"/>
-      <c r="I36" s="265"/>
+      <c r="I36" s="259"/>
       <c r="J36" s="197">
         <v>45138</v>
       </c>
@@ -7165,7 +7174,7 @@
         <v>111</v>
       </c>
       <c r="M36" s="187"/>
-      <c r="P36" s="265"/>
+      <c r="P36" s="259"/>
       <c r="Q36" s="197"/>
       <c r="R36" s="37"/>
       <c r="S36" s="3"/>
@@ -7180,12 +7189,12 @@
       <c r="AG36" s="118"/>
     </row>
     <row r="37" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="265"/>
+      <c r="B37" s="259"/>
       <c r="C37" s="225"/>
       <c r="D37" s="37"/>
       <c r="E37" s="169"/>
       <c r="F37" s="187"/>
-      <c r="I37" s="265"/>
+      <c r="I37" s="259"/>
       <c r="J37" s="197">
         <v>45138</v>
       </c>
@@ -7196,7 +7205,7 @@
         <v>112</v>
       </c>
       <c r="M37" s="187"/>
-      <c r="P37" s="265"/>
+      <c r="P37" s="259"/>
       <c r="Q37" s="197"/>
       <c r="R37" s="37"/>
       <c r="S37" s="3"/>
@@ -7211,12 +7220,12 @@
       <c r="AG37" s="118"/>
     </row>
     <row r="38" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="265"/>
+      <c r="B38" s="259"/>
       <c r="C38" s="225"/>
       <c r="D38" s="37"/>
       <c r="E38" s="168"/>
       <c r="F38" s="187"/>
-      <c r="I38" s="265"/>
+      <c r="I38" s="259"/>
       <c r="J38" s="197">
         <v>45138</v>
       </c>
@@ -7227,7 +7236,7 @@
         <v>113</v>
       </c>
       <c r="M38" s="187"/>
-      <c r="P38" s="265"/>
+      <c r="P38" s="259"/>
       <c r="Q38" s="197"/>
       <c r="R38" s="37"/>
       <c r="S38" s="3"/>
@@ -7242,12 +7251,12 @@
       <c r="AG38" s="118"/>
     </row>
     <row r="39" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="265"/>
+      <c r="B39" s="259"/>
       <c r="C39" s="225"/>
       <c r="D39" s="72"/>
       <c r="E39" s="168"/>
       <c r="F39" s="187"/>
-      <c r="I39" s="265"/>
+      <c r="I39" s="259"/>
       <c r="J39" s="197">
         <v>45138</v>
       </c>
@@ -7258,7 +7267,7 @@
         <v>114</v>
       </c>
       <c r="M39" s="187"/>
-      <c r="P39" s="265"/>
+      <c r="P39" s="259"/>
       <c r="Q39" s="197"/>
       <c r="R39" s="37"/>
       <c r="S39" s="3"/>
@@ -7273,12 +7282,12 @@
       <c r="AG39" s="118"/>
     </row>
     <row r="40" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="265"/>
+      <c r="B40" s="259"/>
       <c r="C40" s="225"/>
       <c r="D40" s="72"/>
       <c r="E40" s="168"/>
       <c r="F40" s="187"/>
-      <c r="I40" s="265"/>
+      <c r="I40" s="259"/>
       <c r="J40" s="197">
         <v>45139</v>
       </c>
@@ -7289,7 +7298,7 @@
         <v>115</v>
       </c>
       <c r="M40" s="187"/>
-      <c r="P40" s="265"/>
+      <c r="P40" s="259"/>
       <c r="Q40" s="197"/>
       <c r="R40" s="37"/>
       <c r="S40" s="3"/>
@@ -7304,12 +7313,12 @@
       <c r="AG40" s="118"/>
     </row>
     <row r="41" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="265"/>
+      <c r="B41" s="259"/>
       <c r="C41" s="225"/>
       <c r="D41" s="37"/>
       <c r="E41" s="168"/>
       <c r="F41" s="187"/>
-      <c r="I41" s="265"/>
+      <c r="I41" s="259"/>
       <c r="J41" s="197">
         <v>45139</v>
       </c>
@@ -7320,7 +7329,7 @@
         <v>116</v>
       </c>
       <c r="M41" s="187"/>
-      <c r="P41" s="265"/>
+      <c r="P41" s="259"/>
       <c r="Q41" s="197"/>
       <c r="R41" s="37"/>
       <c r="S41" s="3"/>
@@ -7335,12 +7344,12 @@
       <c r="AG41" s="118"/>
     </row>
     <row r="42" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="265"/>
+      <c r="B42" s="259"/>
       <c r="C42" s="225"/>
       <c r="D42" s="37"/>
       <c r="E42" s="168"/>
       <c r="F42" s="187"/>
-      <c r="I42" s="265"/>
+      <c r="I42" s="259"/>
       <c r="J42" s="197">
         <v>45143</v>
       </c>
@@ -7349,7 +7358,7 @@
       </c>
       <c r="L42" s="168"/>
       <c r="M42" s="187"/>
-      <c r="P42" s="265"/>
+      <c r="P42" s="259"/>
       <c r="Q42" s="197"/>
       <c r="R42" s="37"/>
       <c r="S42" s="3"/>
@@ -7364,12 +7373,12 @@
       <c r="AG42" s="118"/>
     </row>
     <row r="43" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="265"/>
+      <c r="B43" s="259"/>
       <c r="C43" s="225"/>
       <c r="D43" s="37"/>
       <c r="E43" s="168"/>
       <c r="F43" s="187"/>
-      <c r="I43" s="265"/>
+      <c r="I43" s="259"/>
       <c r="J43" s="197">
         <v>45150</v>
       </c>
@@ -7378,7 +7387,7 @@
       </c>
       <c r="L43" s="168"/>
       <c r="M43" s="187"/>
-      <c r="P43" s="265"/>
+      <c r="P43" s="259"/>
       <c r="Q43" s="197"/>
       <c r="R43" s="37"/>
       <c r="S43" s="3"/>
@@ -7393,17 +7402,17 @@
       <c r="AG43" s="118"/>
     </row>
     <row r="44" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="265"/>
+      <c r="B44" s="259"/>
       <c r="C44" s="225"/>
       <c r="D44" s="37"/>
       <c r="E44" s="168"/>
       <c r="F44" s="187"/>
-      <c r="I44" s="265"/>
+      <c r="I44" s="259"/>
       <c r="J44" s="197"/>
       <c r="K44" s="37"/>
       <c r="L44" s="168"/>
       <c r="M44" s="187"/>
-      <c r="P44" s="265"/>
+      <c r="P44" s="259"/>
       <c r="Q44" s="197"/>
       <c r="R44" s="37"/>
       <c r="S44" s="3"/>
@@ -7418,17 +7427,17 @@
       <c r="AG44" s="118"/>
     </row>
     <row r="45" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="265"/>
+      <c r="B45" s="259"/>
       <c r="C45" s="225"/>
       <c r="D45" s="37"/>
       <c r="E45" s="168"/>
       <c r="F45" s="187"/>
-      <c r="I45" s="265"/>
+      <c r="I45" s="259"/>
       <c r="J45" s="197"/>
       <c r="K45" s="37"/>
       <c r="L45" s="168"/>
       <c r="M45" s="187"/>
-      <c r="P45" s="265"/>
+      <c r="P45" s="259"/>
       <c r="Q45" s="197"/>
       <c r="R45" s="37"/>
       <c r="S45" s="3"/>
@@ -7443,17 +7452,17 @@
       <c r="AG45" s="118"/>
     </row>
     <row r="46" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="265"/>
+      <c r="B46" s="259"/>
       <c r="C46" s="225"/>
       <c r="D46" s="37"/>
       <c r="E46" s="168"/>
       <c r="F46" s="187"/>
-      <c r="I46" s="265"/>
+      <c r="I46" s="259"/>
       <c r="J46" s="197"/>
       <c r="K46" s="37"/>
       <c r="L46" s="168"/>
       <c r="M46" s="187"/>
-      <c r="P46" s="265"/>
+      <c r="P46" s="259"/>
       <c r="Q46" s="197"/>
       <c r="R46" s="37"/>
       <c r="S46" s="3"/>
@@ -7468,17 +7477,17 @@
       <c r="AG46" s="118"/>
     </row>
     <row r="47" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="265"/>
+      <c r="B47" s="259"/>
       <c r="C47" s="225"/>
       <c r="D47" s="37"/>
       <c r="E47" s="168"/>
       <c r="F47" s="187"/>
-      <c r="I47" s="265"/>
+      <c r="I47" s="259"/>
       <c r="J47" s="197"/>
       <c r="K47" s="37"/>
       <c r="L47" s="168"/>
       <c r="M47" s="187"/>
-      <c r="P47" s="265"/>
+      <c r="P47" s="259"/>
       <c r="Q47" s="197"/>
       <c r="R47" s="37"/>
       <c r="S47" s="3"/>
@@ -7493,7 +7502,7 @@
       <c r="AG47" s="118"/>
     </row>
     <row r="48" spans="2:33" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="266"/>
+      <c r="B48" s="260"/>
       <c r="C48" s="158" t="s">
         <v>3</v>
       </c>
@@ -7501,7 +7510,7 @@
         <f>SUM(D5:D47)</f>
         <v>2334303.66</v>
       </c>
-      <c r="I48" s="266"/>
+      <c r="I48" s="260"/>
       <c r="J48" s="158" t="s">
         <v>3</v>
       </c>
@@ -7509,7 +7518,7 @@
         <f>SUM(K5:K47)</f>
         <v>3545962.9600000004</v>
       </c>
-      <c r="P48" s="266"/>
+      <c r="P48" s="260"/>
       <c r="Q48" s="158" t="s">
         <v>3</v>
       </c>
@@ -7906,21 +7915,21 @@
       <c r="K66" s="171">
         <v>29450</v>
       </c>
-      <c r="L66" s="270" t="s">
+      <c r="L66" s="256" t="s">
         <v>100</v>
       </c>
-      <c r="M66" s="270"/>
-      <c r="N66" s="270"/>
-      <c r="O66" s="270"/>
-      <c r="P66" s="270"/>
-      <c r="Q66" s="270"/>
-      <c r="R66" s="270"/>
-      <c r="S66" s="270"/>
-      <c r="T66" s="270"/>
-      <c r="U66" s="270"/>
-      <c r="V66" s="270"/>
-      <c r="W66" s="270"/>
-      <c r="X66" s="270"/>
+      <c r="M66" s="256"/>
+      <c r="N66" s="256"/>
+      <c r="O66" s="256"/>
+      <c r="P66" s="256"/>
+      <c r="Q66" s="256"/>
+      <c r="R66" s="256"/>
+      <c r="S66" s="256"/>
+      <c r="T66" s="256"/>
+      <c r="U66" s="256"/>
+      <c r="V66" s="256"/>
+      <c r="W66" s="256"/>
+      <c r="X66" s="256"/>
     </row>
     <row r="67" spans="2:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="120"/>
@@ -7932,19 +7941,19 @@
       </c>
       <c r="J67" s="172"/>
       <c r="K67" s="173"/>
-      <c r="L67" s="270"/>
-      <c r="M67" s="270"/>
-      <c r="N67" s="270"/>
-      <c r="O67" s="270"/>
-      <c r="P67" s="270"/>
-      <c r="Q67" s="270"/>
-      <c r="R67" s="270"/>
-      <c r="S67" s="270"/>
-      <c r="T67" s="270"/>
-      <c r="U67" s="270"/>
-      <c r="V67" s="270"/>
-      <c r="W67" s="270"/>
-      <c r="X67" s="270"/>
+      <c r="L67" s="256"/>
+      <c r="M67" s="256"/>
+      <c r="N67" s="256"/>
+      <c r="O67" s="256"/>
+      <c r="P67" s="256"/>
+      <c r="Q67" s="256"/>
+      <c r="R67" s="256"/>
+      <c r="S67" s="256"/>
+      <c r="T67" s="256"/>
+      <c r="U67" s="256"/>
+      <c r="V67" s="256"/>
+      <c r="W67" s="256"/>
+      <c r="X67" s="256"/>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" s="120"/>
@@ -7954,19 +7963,19 @@
       <c r="I68" s="172"/>
       <c r="J68" s="172"/>
       <c r="K68" s="173"/>
-      <c r="L68" s="270"/>
-      <c r="M68" s="270"/>
-      <c r="N68" s="270"/>
-      <c r="O68" s="270"/>
-      <c r="P68" s="270"/>
-      <c r="Q68" s="270"/>
-      <c r="R68" s="270"/>
-      <c r="S68" s="270"/>
-      <c r="T68" s="270"/>
-      <c r="U68" s="270"/>
-      <c r="V68" s="270"/>
-      <c r="W68" s="270"/>
-      <c r="X68" s="270"/>
+      <c r="L68" s="256"/>
+      <c r="M68" s="256"/>
+      <c r="N68" s="256"/>
+      <c r="O68" s="256"/>
+      <c r="P68" s="256"/>
+      <c r="Q68" s="256"/>
+      <c r="R68" s="256"/>
+      <c r="S68" s="256"/>
+      <c r="T68" s="256"/>
+      <c r="U68" s="256"/>
+      <c r="V68" s="256"/>
+      <c r="W68" s="256"/>
+      <c r="X68" s="256"/>
     </row>
     <row r="69" spans="2:33" ht="21" x14ac:dyDescent="0.35">
       <c r="B69" s="120"/>
@@ -7976,21 +7985,21 @@
       <c r="I69" s="172"/>
       <c r="J69" s="172"/>
       <c r="K69" s="173"/>
-      <c r="L69" s="271" t="s">
+      <c r="L69" s="257" t="s">
         <v>102</v>
       </c>
-      <c r="M69" s="271"/>
-      <c r="N69" s="271"/>
-      <c r="O69" s="271"/>
-      <c r="P69" s="271"/>
-      <c r="Q69" s="271"/>
-      <c r="R69" s="271"/>
-      <c r="S69" s="271"/>
-      <c r="T69" s="271"/>
-      <c r="U69" s="271"/>
-      <c r="V69" s="271"/>
-      <c r="W69" s="271"/>
-      <c r="X69" s="271"/>
+      <c r="M69" s="257"/>
+      <c r="N69" s="257"/>
+      <c r="O69" s="257"/>
+      <c r="P69" s="257"/>
+      <c r="Q69" s="257"/>
+      <c r="R69" s="257"/>
+      <c r="S69" s="257"/>
+      <c r="T69" s="257"/>
+      <c r="U69" s="257"/>
+      <c r="V69" s="257"/>
+      <c r="W69" s="257"/>
+      <c r="X69" s="257"/>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B70" s="120"/>
@@ -8256,13 +8265,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="L66:X68"/>
-    <mergeCell ref="L69:X69"/>
-    <mergeCell ref="B2:B48"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="I2:I48"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="AD2:AD19"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="J3:L3"/>
@@ -8274,6 +8276,13 @@
     <mergeCell ref="P2:P48"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="X2:X22"/>
+    <mergeCell ref="L66:X68"/>
+    <mergeCell ref="L69:X69"/>
+    <mergeCell ref="B2:B48"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="I2:I48"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8458,8 +8467,8 @@
   </sheetPr>
   <dimension ref="B1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8490,80 +8499,80 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="264" t="s">
+      <c r="B2" s="258" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="259" t="s">
+      <c r="C2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="259"/>
+      <c r="D2" s="261"/>
       <c r="E2" s="17"/>
-      <c r="I2" s="264" t="s">
+      <c r="I2" s="258" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="259" t="s">
+      <c r="J2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="259"/>
+      <c r="K2" s="261"/>
       <c r="L2" s="17"/>
       <c r="M2" s="166"/>
-      <c r="Q2" s="267" t="s">
+      <c r="Q2" s="269" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="259" t="s">
+      <c r="R2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="259"/>
+      <c r="S2" s="261"/>
       <c r="T2" s="17"/>
-      <c r="W2" s="256" t="s">
+      <c r="W2" s="262" t="s">
         <v>94</v>
       </c>
-      <c r="X2" s="259" t="s">
+      <c r="X2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="Y2" s="259"/>
+      <c r="Y2" s="261"/>
       <c r="Z2" s="17"/>
     </row>
     <row r="3" spans="2:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="265"/>
+      <c r="B3" s="259"/>
       <c r="C3" s="232"/>
       <c r="D3" s="232"/>
       <c r="E3" s="233"/>
-      <c r="I3" s="265"/>
+      <c r="I3" s="259"/>
       <c r="J3" s="232"/>
       <c r="K3" s="232"/>
       <c r="L3" s="233"/>
       <c r="M3" s="166"/>
-      <c r="Q3" s="268"/>
+      <c r="Q3" s="270"/>
       <c r="R3" s="232"/>
       <c r="S3" s="232"/>
       <c r="T3" s="233"/>
-      <c r="W3" s="257"/>
+      <c r="W3" s="263"/>
       <c r="X3" s="232"/>
       <c r="Y3" s="232"/>
       <c r="Z3" s="233"/>
     </row>
     <row r="4" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="265"/>
+      <c r="B4" s="259"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="265"/>
+      <c r="I4" s="259"/>
       <c r="J4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="23"/>
       <c r="M4" s="166"/>
-      <c r="Q4" s="268"/>
+      <c r="Q4" s="270"/>
       <c r="R4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="23"/>
-      <c r="W4" s="257"/>
+      <c r="W4" s="263"/>
       <c r="X4" s="21" t="s">
         <v>2</v>
       </c>
@@ -8571,7 +8580,7 @@
       <c r="Z4" s="23"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="265"/>
+      <c r="B5" s="259"/>
       <c r="C5" s="203" t="s">
         <v>80</v>
       </c>
@@ -8579,7 +8588,7 @@
         <v>563480</v>
       </c>
       <c r="E5" s="28"/>
-      <c r="I5" s="265"/>
+      <c r="I5" s="259"/>
       <c r="J5" s="155">
         <v>45010</v>
       </c>
@@ -8588,7 +8597,7 @@
       </c>
       <c r="L5" s="28"/>
       <c r="M5" s="166"/>
-      <c r="Q5" s="268"/>
+      <c r="Q5" s="270"/>
       <c r="R5" s="155">
         <v>44947</v>
       </c>
@@ -8596,7 +8605,7 @@
         <v>50000</v>
       </c>
       <c r="T5" s="28"/>
-      <c r="W5" s="257"/>
+      <c r="W5" s="263"/>
       <c r="X5" s="155">
         <v>44873</v>
       </c>
@@ -8606,7 +8615,7 @@
       <c r="Z5" s="28"/>
     </row>
     <row r="6" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="265"/>
+      <c r="B6" s="259"/>
       <c r="C6" s="155">
         <v>45010</v>
       </c>
@@ -8614,7 +8623,7 @@
         <v>50000</v>
       </c>
       <c r="E6" s="27"/>
-      <c r="I6" s="265"/>
+      <c r="I6" s="259"/>
       <c r="J6" s="154">
         <v>45017</v>
       </c>
@@ -8623,7 +8632,7 @@
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="166"/>
-      <c r="Q6" s="268"/>
+      <c r="Q6" s="270"/>
       <c r="R6" s="176">
         <v>44954</v>
       </c>
@@ -8631,13 +8640,13 @@
         <v>50000</v>
       </c>
       <c r="T6" s="27"/>
-      <c r="W6" s="257"/>
+      <c r="W6" s="263"/>
       <c r="X6" s="176"/>
       <c r="Y6" s="37"/>
       <c r="Z6" s="27"/>
     </row>
     <row r="7" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="265"/>
+      <c r="B7" s="259"/>
       <c r="C7" s="165">
         <v>45017</v>
       </c>
@@ -8645,7 +8654,7 @@
         <v>100000</v>
       </c>
       <c r="E7" s="41"/>
-      <c r="I7" s="265"/>
+      <c r="I7" s="259"/>
       <c r="J7" s="154">
         <v>45021</v>
       </c>
@@ -8654,7 +8663,7 @@
       </c>
       <c r="L7" s="41"/>
       <c r="M7" s="166"/>
-      <c r="Q7" s="268"/>
+      <c r="Q7" s="270"/>
       <c r="R7" s="176">
         <v>44961</v>
       </c>
@@ -8662,13 +8671,13 @@
         <v>50000</v>
       </c>
       <c r="T7" s="41"/>
-      <c r="W7" s="257"/>
+      <c r="W7" s="263"/>
       <c r="X7" s="176"/>
       <c r="Y7" s="37"/>
       <c r="Z7" s="41"/>
     </row>
     <row r="8" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="265"/>
+      <c r="B8" s="259"/>
       <c r="C8" s="165">
         <v>45021</v>
       </c>
@@ -8676,7 +8685,7 @@
         <v>50000</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="I8" s="265"/>
+      <c r="I8" s="259"/>
       <c r="J8" s="154">
         <v>45031</v>
       </c>
@@ -8685,7 +8694,7 @@
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="166"/>
-      <c r="Q8" s="268"/>
+      <c r="Q8" s="270"/>
       <c r="R8" s="176">
         <v>44968</v>
       </c>
@@ -8693,13 +8702,13 @@
         <v>50000</v>
       </c>
       <c r="T8" s="27"/>
-      <c r="W8" s="257"/>
+      <c r="W8" s="263"/>
       <c r="X8" s="176"/>
       <c r="Y8" s="37"/>
       <c r="Z8" s="27"/>
     </row>
     <row r="9" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="265"/>
+      <c r="B9" s="259"/>
       <c r="C9" s="165">
         <v>45031</v>
       </c>
@@ -8707,7 +8716,7 @@
         <v>100000</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="I9" s="265"/>
+      <c r="I9" s="259"/>
       <c r="J9" s="156">
         <v>45038</v>
       </c>
@@ -8716,7 +8725,7 @@
       </c>
       <c r="L9" s="27"/>
       <c r="M9" s="166"/>
-      <c r="Q9" s="268"/>
+      <c r="Q9" s="270"/>
       <c r="R9" s="156">
         <v>44975</v>
       </c>
@@ -8724,15 +8733,15 @@
         <v>50000</v>
       </c>
       <c r="T9" s="27"/>
-      <c r="W9" s="257"/>
-      <c r="X9" s="260" t="s">
+      <c r="W9" s="263"/>
+      <c r="X9" s="265" t="s">
         <v>95</v>
       </c>
-      <c r="Y9" s="260"/>
-      <c r="Z9" s="261"/>
+      <c r="Y9" s="265"/>
+      <c r="Z9" s="266"/>
     </row>
     <row r="10" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="265"/>
+      <c r="B10" s="259"/>
       <c r="C10" s="156">
         <v>45038</v>
       </c>
@@ -8740,7 +8749,7 @@
         <v>50000</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="I10" s="265"/>
+      <c r="I10" s="259"/>
       <c r="J10" s="156">
         <v>45045</v>
       </c>
@@ -8749,7 +8758,7 @@
       </c>
       <c r="L10" s="27"/>
       <c r="M10" s="166"/>
-      <c r="Q10" s="268"/>
+      <c r="Q10" s="270"/>
       <c r="R10" s="156">
         <v>44982</v>
       </c>
@@ -8757,13 +8766,13 @@
         <v>50000</v>
       </c>
       <c r="T10" s="27"/>
-      <c r="W10" s="257"/>
-      <c r="X10" s="262"/>
-      <c r="Y10" s="262"/>
-      <c r="Z10" s="263"/>
+      <c r="W10" s="263"/>
+      <c r="X10" s="267"/>
+      <c r="Y10" s="267"/>
+      <c r="Z10" s="268"/>
     </row>
     <row r="11" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="265"/>
+      <c r="B11" s="259"/>
       <c r="C11" s="156">
         <v>45045</v>
       </c>
@@ -8771,7 +8780,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="I11" s="265"/>
+      <c r="I11" s="259"/>
       <c r="J11" s="156">
         <v>45052</v>
       </c>
@@ -8780,7 +8789,7 @@
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="166"/>
-      <c r="Q11" s="268"/>
+      <c r="Q11" s="270"/>
       <c r="R11" s="156">
         <v>44989</v>
       </c>
@@ -8788,13 +8797,13 @@
         <v>50000</v>
       </c>
       <c r="T11" s="27"/>
-      <c r="W11" s="257"/>
+      <c r="W11" s="263"/>
       <c r="X11" s="156"/>
       <c r="Y11" s="77"/>
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="265"/>
+      <c r="B12" s="259"/>
       <c r="C12" s="156">
         <v>45052</v>
       </c>
@@ -8802,7 +8811,7 @@
         <v>100000</v>
       </c>
       <c r="E12" s="146"/>
-      <c r="I12" s="265"/>
+      <c r="I12" s="259"/>
       <c r="J12" s="157">
         <v>45059</v>
       </c>
@@ -8811,7 +8820,7 @@
       </c>
       <c r="L12" s="146"/>
       <c r="M12" s="166"/>
-      <c r="Q12" s="268"/>
+      <c r="Q12" s="270"/>
       <c r="R12" s="157">
         <v>44989</v>
       </c>
@@ -8819,7 +8828,7 @@
         <v>50000</v>
       </c>
       <c r="T12" s="146"/>
-      <c r="W12" s="257"/>
+      <c r="W12" s="263"/>
       <c r="X12" s="176"/>
       <c r="Y12" s="37">
         <v>0</v>
@@ -8827,7 +8836,7 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="265"/>
+      <c r="B13" s="259"/>
       <c r="C13" s="157">
         <v>45059</v>
       </c>
@@ -8835,12 +8844,12 @@
         <v>100000</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="I13" s="265"/>
+      <c r="I13" s="259"/>
       <c r="J13" s="154"/>
       <c r="K13" s="37"/>
       <c r="L13" s="3"/>
       <c r="M13" s="166"/>
-      <c r="Q13" s="268"/>
+      <c r="Q13" s="270"/>
       <c r="R13" s="176">
         <v>44996</v>
       </c>
@@ -8848,13 +8857,13 @@
         <v>50000</v>
       </c>
       <c r="T13" s="3"/>
-      <c r="W13" s="257"/>
+      <c r="W13" s="263"/>
       <c r="X13" s="176"/>
       <c r="Y13" s="37"/>
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="265"/>
+      <c r="B14" s="259"/>
       <c r="C14" s="165">
         <v>45066</v>
       </c>
@@ -8862,12 +8871,12 @@
         <v>100000</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="I14" s="265"/>
+      <c r="I14" s="259"/>
       <c r="J14" s="154"/>
       <c r="K14" s="37"/>
       <c r="L14" s="3"/>
       <c r="M14" s="166"/>
-      <c r="Q14" s="268"/>
+      <c r="Q14" s="270"/>
       <c r="R14" s="176">
         <v>45003</v>
       </c>
@@ -8875,13 +8884,13 @@
         <v>113480</v>
       </c>
       <c r="T14" s="3"/>
-      <c r="W14" s="257"/>
+      <c r="W14" s="263"/>
       <c r="X14" s="176"/>
       <c r="Y14" s="37"/>
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="265"/>
+      <c r="B15" s="259"/>
       <c r="C15" s="165">
         <v>45073</v>
       </c>
@@ -8889,18 +8898,18 @@
         <v>100000</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="I15" s="265"/>
+      <c r="I15" s="259"/>
       <c r="J15" s="154"/>
       <c r="K15" s="37"/>
       <c r="L15" s="3"/>
       <c r="M15" s="166"/>
-      <c r="Q15" s="268"/>
+      <c r="Q15" s="270"/>
       <c r="R15" s="176"/>
       <c r="S15" s="37">
         <v>0</v>
       </c>
       <c r="T15" s="3"/>
-      <c r="W15" s="257"/>
+      <c r="W15" s="263"/>
       <c r="X15" s="158" t="s">
         <v>3</v>
       </c>
@@ -8910,7 +8919,7 @@
       </c>
     </row>
     <row r="16" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="265"/>
+      <c r="B16" s="259"/>
       <c r="C16" s="165">
         <v>45079</v>
       </c>
@@ -8918,18 +8927,18 @@
         <v>100000</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="I16" s="265"/>
+      <c r="I16" s="259"/>
       <c r="J16" s="154"/>
       <c r="K16" s="37"/>
       <c r="L16" s="3"/>
       <c r="M16" s="166"/>
-      <c r="Q16" s="268"/>
+      <c r="Q16" s="270"/>
       <c r="R16" s="176"/>
       <c r="S16" s="37">
         <v>0</v>
       </c>
       <c r="T16" s="3"/>
-      <c r="W16" s="257"/>
+      <c r="W16" s="263"/>
       <c r="X16" s="121"/>
       <c r="Y16" s="49">
         <v>67769</v>
@@ -8939,7 +8948,7 @@
       </c>
     </row>
     <row r="17" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="265"/>
+      <c r="B17" s="259"/>
       <c r="C17" s="165">
         <v>45092</v>
       </c>
@@ -8947,12 +8956,12 @@
         <v>100000</v>
       </c>
       <c r="E17" s="168"/>
-      <c r="I17" s="265"/>
+      <c r="I17" s="259"/>
       <c r="J17" s="154"/>
       <c r="K17" s="37"/>
       <c r="L17" s="3"/>
       <c r="M17" s="166"/>
-      <c r="Q17" s="268"/>
+      <c r="Q17" s="270"/>
       <c r="R17" s="184" t="s">
         <v>3</v>
       </c>
@@ -8960,7 +8969,7 @@
         <f>SUM(S5:S16)</f>
         <v>563480</v>
       </c>
-      <c r="W17" s="257"/>
+      <c r="W17" s="263"/>
       <c r="X17" s="65"/>
       <c r="Y17" s="49">
         <v>0</v>
@@ -8968,7 +8977,7 @@
       <c r="Z17" s="124"/>
     </row>
     <row r="18" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="265"/>
+      <c r="B18" s="259"/>
       <c r="C18" s="167">
         <v>45101</v>
       </c>
@@ -8976,12 +8985,12 @@
         <v>100000</v>
       </c>
       <c r="E18" s="168"/>
-      <c r="I18" s="265"/>
+      <c r="I18" s="259"/>
       <c r="J18" s="154"/>
       <c r="K18" s="37"/>
       <c r="L18" s="3"/>
       <c r="M18" s="166"/>
-      <c r="Q18" s="268"/>
+      <c r="Q18" s="270"/>
       <c r="R18" s="160"/>
       <c r="S18" s="161">
         <v>-563480</v>
@@ -8989,14 +8998,14 @@
       <c r="T18" s="152">
         <v>44947</v>
       </c>
-      <c r="W18" s="257"/>
+      <c r="W18" s="263"/>
       <c r="X18" s="84"/>
       <c r="Y18" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="265"/>
+      <c r="B19" s="259"/>
       <c r="C19" s="167">
         <v>45108</v>
       </c>
@@ -9004,18 +9013,18 @@
         <v>100000</v>
       </c>
       <c r="E19" s="168"/>
-      <c r="I19" s="265"/>
+      <c r="I19" s="259"/>
       <c r="J19" s="154"/>
       <c r="K19" s="37"/>
       <c r="L19" s="3"/>
       <c r="M19" s="166"/>
-      <c r="Q19" s="268"/>
+      <c r="Q19" s="270"/>
       <c r="R19" s="162"/>
       <c r="S19" s="161">
         <v>0</v>
       </c>
       <c r="T19" s="124"/>
-      <c r="W19" s="258"/>
+      <c r="W19" s="264"/>
       <c r="X19" s="185" t="s">
         <v>4</v>
       </c>
@@ -9025,7 +9034,7 @@
       </c>
     </row>
     <row r="20" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="265"/>
+      <c r="B20" s="259"/>
       <c r="C20" s="199">
         <v>45115</v>
       </c>
@@ -9033,12 +9042,12 @@
         <v>100000</v>
       </c>
       <c r="E20" s="168"/>
-      <c r="I20" s="265"/>
+      <c r="I20" s="259"/>
       <c r="J20" s="154"/>
       <c r="K20" s="37"/>
       <c r="L20" s="3"/>
       <c r="M20" s="166"/>
-      <c r="Q20" s="268"/>
+      <c r="Q20" s="270"/>
       <c r="R20" s="163"/>
       <c r="S20" s="164">
         <v>0</v>
@@ -9049,7 +9058,7 @@
       <c r="Z20" s="118"/>
     </row>
     <row r="21" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="265"/>
+      <c r="B21" s="259"/>
       <c r="C21" s="199">
         <v>45122</v>
       </c>
@@ -9058,12 +9067,12 @@
       </c>
       <c r="E21" s="168"/>
       <c r="F21" s="187"/>
-      <c r="I21" s="265"/>
+      <c r="I21" s="259"/>
       <c r="J21" s="154"/>
       <c r="K21" s="37"/>
       <c r="L21" s="3"/>
       <c r="M21" s="166"/>
-      <c r="Q21" s="268"/>
+      <c r="Q21" s="270"/>
       <c r="R21" s="33" t="s">
         <v>4</v>
       </c>
@@ -9077,7 +9086,7 @@
       <c r="Z21" s="118"/>
     </row>
     <row r="22" spans="2:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="265"/>
+      <c r="B22" s="259"/>
       <c r="C22" s="199">
         <v>45134</v>
       </c>
@@ -9088,12 +9097,12 @@
         <v>109</v>
       </c>
       <c r="F22" s="187"/>
-      <c r="I22" s="265"/>
+      <c r="I22" s="259"/>
       <c r="J22" s="154"/>
       <c r="K22" s="37"/>
       <c r="L22" s="3"/>
       <c r="M22" s="166"/>
-      <c r="Q22" s="269"/>
+      <c r="Q22" s="271"/>
       <c r="R22" s="182"/>
       <c r="S22" s="183"/>
       <c r="T22" s="118"/>
@@ -9103,7 +9112,7 @@
       <c r="Z22" s="118"/>
     </row>
     <row r="23" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="265"/>
+      <c r="B23" s="259"/>
       <c r="C23" s="199">
         <v>45138</v>
       </c>
@@ -9114,7 +9123,7 @@
         <v>111</v>
       </c>
       <c r="F23" s="187"/>
-      <c r="I23" s="265"/>
+      <c r="I23" s="259"/>
       <c r="J23" s="154"/>
       <c r="K23" s="37"/>
       <c r="L23" s="3"/>
@@ -9129,7 +9138,7 @@
       <c r="Z23" s="118"/>
     </row>
     <row r="24" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="265"/>
+      <c r="B24" s="259"/>
       <c r="C24" s="199">
         <v>45138</v>
       </c>
@@ -9140,7 +9149,7 @@
         <v>112</v>
       </c>
       <c r="F24" s="187"/>
-      <c r="I24" s="265"/>
+      <c r="I24" s="259"/>
       <c r="J24" s="154"/>
       <c r="K24" s="37"/>
       <c r="L24" s="3"/>
@@ -9155,7 +9164,7 @@
       <c r="Z24" s="118"/>
     </row>
     <row r="25" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="265"/>
+      <c r="B25" s="259"/>
       <c r="C25" s="199">
         <v>45138</v>
       </c>
@@ -9166,7 +9175,7 @@
         <v>113</v>
       </c>
       <c r="F25" s="187"/>
-      <c r="I25" s="265"/>
+      <c r="I25" s="259"/>
       <c r="J25" s="154"/>
       <c r="K25" s="37"/>
       <c r="L25" s="3"/>
@@ -9181,7 +9190,7 @@
       <c r="Z25" s="118"/>
     </row>
     <row r="26" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="265"/>
+      <c r="B26" s="259"/>
       <c r="C26" s="199">
         <v>45138</v>
       </c>
@@ -9192,7 +9201,7 @@
         <v>114</v>
       </c>
       <c r="F26" s="187"/>
-      <c r="I26" s="265"/>
+      <c r="I26" s="259"/>
       <c r="J26" s="176"/>
       <c r="K26" s="37"/>
       <c r="L26" s="3"/>
@@ -9207,7 +9216,7 @@
       <c r="Z26" s="118"/>
     </row>
     <row r="27" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="265"/>
+      <c r="B27" s="259"/>
       <c r="C27" s="199">
         <v>45139</v>
       </c>
@@ -9218,7 +9227,7 @@
         <v>115</v>
       </c>
       <c r="F27" s="187"/>
-      <c r="I27" s="265"/>
+      <c r="I27" s="259"/>
       <c r="J27" s="176"/>
       <c r="K27" s="37"/>
       <c r="L27" s="3"/>
@@ -9233,7 +9242,7 @@
       <c r="Z27" s="118"/>
     </row>
     <row r="28" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="265"/>
+      <c r="B28" s="259"/>
       <c r="C28" s="207">
         <v>45150</v>
       </c>
@@ -9244,7 +9253,7 @@
         <v>129</v>
       </c>
       <c r="F28" s="187"/>
-      <c r="I28" s="265"/>
+      <c r="I28" s="259"/>
       <c r="J28" s="176"/>
       <c r="K28" s="37"/>
       <c r="L28" s="3"/>
@@ -9259,7 +9268,7 @@
       <c r="Z28" s="118"/>
     </row>
     <row r="29" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="265"/>
+      <c r="B29" s="259"/>
       <c r="C29" s="199">
         <v>45157</v>
       </c>
@@ -9270,7 +9279,7 @@
         <v>136</v>
       </c>
       <c r="F29" s="187"/>
-      <c r="I29" s="265"/>
+      <c r="I29" s="259"/>
       <c r="J29" s="176"/>
       <c r="K29" s="37"/>
       <c r="L29" s="3"/>
@@ -9285,7 +9294,7 @@
       <c r="Z29" s="118"/>
     </row>
     <row r="30" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="265"/>
+      <c r="B30" s="259"/>
       <c r="C30" s="199">
         <v>45164</v>
       </c>
@@ -9294,7 +9303,7 @@
       </c>
       <c r="E30" s="168"/>
       <c r="F30" s="187"/>
-      <c r="I30" s="265"/>
+      <c r="I30" s="259"/>
       <c r="J30" s="176"/>
       <c r="K30" s="37"/>
       <c r="L30" s="3"/>
@@ -9309,12 +9318,18 @@
       <c r="Z30" s="118"/>
     </row>
     <row r="31" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="265"/>
-      <c r="C31" s="199"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="168"/>
+      <c r="B31" s="259"/>
+      <c r="C31" s="199">
+        <v>45161</v>
+      </c>
+      <c r="D31" s="37">
+        <v>10964.31</v>
+      </c>
+      <c r="E31" s="168" t="s">
+        <v>137</v>
+      </c>
       <c r="F31" s="187"/>
-      <c r="I31" s="265"/>
+      <c r="I31" s="259"/>
       <c r="J31" s="176"/>
       <c r="K31" s="37"/>
       <c r="L31" s="3"/>
@@ -9329,12 +9344,18 @@
       <c r="Z31" s="118"/>
     </row>
     <row r="32" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="265"/>
-      <c r="C32" s="199"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="168"/>
+      <c r="B32" s="259"/>
+      <c r="C32" s="199">
+        <v>45161</v>
+      </c>
+      <c r="D32" s="37">
+        <v>28618.33</v>
+      </c>
+      <c r="E32" s="168" t="s">
+        <v>112</v>
+      </c>
       <c r="F32" s="187"/>
-      <c r="I32" s="265"/>
+      <c r="I32" s="259"/>
       <c r="J32" s="176"/>
       <c r="K32" s="37"/>
       <c r="L32" s="3"/>
@@ -9349,12 +9370,18 @@
       <c r="Z32" s="118"/>
     </row>
     <row r="33" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="265"/>
-      <c r="C33" s="199"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="168"/>
+      <c r="B33" s="259"/>
+      <c r="C33" s="199">
+        <v>45166</v>
+      </c>
+      <c r="D33" s="37">
+        <v>29004.14</v>
+      </c>
+      <c r="E33" s="168" t="s">
+        <v>138</v>
+      </c>
       <c r="F33" s="187"/>
-      <c r="I33" s="265"/>
+      <c r="I33" s="259"/>
       <c r="J33" s="176"/>
       <c r="K33" s="37"/>
       <c r="L33" s="3"/>
@@ -9369,12 +9396,12 @@
       <c r="Z33" s="118"/>
     </row>
     <row r="34" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="265"/>
+      <c r="B34" s="259"/>
       <c r="C34" s="176"/>
       <c r="D34" s="37"/>
       <c r="E34" s="168"/>
       <c r="F34" s="187"/>
-      <c r="I34" s="265"/>
+      <c r="I34" s="259"/>
       <c r="J34" s="176"/>
       <c r="K34" s="37"/>
       <c r="L34" s="3"/>
@@ -9389,12 +9416,12 @@
       <c r="Z34" s="118"/>
     </row>
     <row r="35" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="265"/>
+      <c r="B35" s="259"/>
       <c r="C35" s="189"/>
       <c r="D35" s="37"/>
       <c r="E35" s="168"/>
       <c r="F35" s="187"/>
-      <c r="I35" s="265"/>
+      <c r="I35" s="259"/>
       <c r="J35" s="189"/>
       <c r="K35" s="37"/>
       <c r="L35" s="3"/>
@@ -9409,12 +9436,12 @@
       <c r="Z35" s="118"/>
     </row>
     <row r="36" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="265"/>
+      <c r="B36" s="259"/>
       <c r="C36" s="190"/>
       <c r="D36" s="37"/>
       <c r="E36" s="168"/>
       <c r="F36" s="187"/>
-      <c r="I36" s="265"/>
+      <c r="I36" s="259"/>
       <c r="J36" s="189"/>
       <c r="K36" s="37"/>
       <c r="L36" s="3"/>
@@ -9429,12 +9456,12 @@
       <c r="Z36" s="118"/>
     </row>
     <row r="37" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="265"/>
+      <c r="B37" s="259"/>
       <c r="C37" s="190"/>
       <c r="D37" s="37"/>
       <c r="E37" s="169"/>
       <c r="F37" s="187"/>
-      <c r="I37" s="265"/>
+      <c r="I37" s="259"/>
       <c r="J37" s="189"/>
       <c r="K37" s="37"/>
       <c r="L37" s="3"/>
@@ -9449,12 +9476,12 @@
       <c r="Z37" s="118"/>
     </row>
     <row r="38" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="265"/>
+      <c r="B38" s="259"/>
       <c r="C38" s="190"/>
       <c r="D38" s="37"/>
       <c r="E38" s="168"/>
       <c r="F38" s="187"/>
-      <c r="I38" s="265"/>
+      <c r="I38" s="259"/>
       <c r="J38" s="189"/>
       <c r="K38" s="37"/>
       <c r="L38" s="3"/>
@@ -9469,12 +9496,12 @@
       <c r="Z38" s="118"/>
     </row>
     <row r="39" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="265"/>
+      <c r="B39" s="259"/>
       <c r="C39" s="190"/>
       <c r="D39" s="72"/>
       <c r="E39" s="168"/>
       <c r="F39" s="187"/>
-      <c r="I39" s="265"/>
+      <c r="I39" s="259"/>
       <c r="J39" s="189"/>
       <c r="K39" s="37"/>
       <c r="L39" s="3"/>
@@ -9489,12 +9516,12 @@
       <c r="Z39" s="118"/>
     </row>
     <row r="40" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="265"/>
+      <c r="B40" s="259"/>
       <c r="C40" s="190"/>
       <c r="D40" s="72"/>
       <c r="E40" s="168"/>
       <c r="F40" s="187"/>
-      <c r="I40" s="265"/>
+      <c r="I40" s="259"/>
       <c r="J40" s="189"/>
       <c r="K40" s="37"/>
       <c r="L40" s="3"/>
@@ -9509,12 +9536,12 @@
       <c r="Z40" s="118"/>
     </row>
     <row r="41" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="265"/>
+      <c r="B41" s="259"/>
       <c r="C41" s="190"/>
       <c r="D41" s="37"/>
       <c r="E41" s="168"/>
       <c r="F41" s="187"/>
-      <c r="I41" s="265"/>
+      <c r="I41" s="259"/>
       <c r="J41" s="189"/>
       <c r="K41" s="37"/>
       <c r="L41" s="3"/>
@@ -9529,12 +9556,12 @@
       <c r="Z41" s="118"/>
     </row>
     <row r="42" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="265"/>
+      <c r="B42" s="259"/>
       <c r="C42" s="190"/>
       <c r="D42" s="37"/>
       <c r="E42" s="168"/>
       <c r="F42" s="187"/>
-      <c r="I42" s="265"/>
+      <c r="I42" s="259"/>
       <c r="J42" s="189"/>
       <c r="K42" s="37"/>
       <c r="L42" s="3"/>
@@ -9549,12 +9576,12 @@
       <c r="Z42" s="118"/>
     </row>
     <row r="43" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="265"/>
+      <c r="B43" s="259"/>
       <c r="C43" s="189"/>
       <c r="D43" s="37"/>
       <c r="E43" s="168"/>
       <c r="F43" s="187"/>
-      <c r="I43" s="265"/>
+      <c r="I43" s="259"/>
       <c r="J43" s="189"/>
       <c r="K43" s="37"/>
       <c r="L43" s="3"/>
@@ -9569,12 +9596,12 @@
       <c r="Z43" s="118"/>
     </row>
     <row r="44" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="265"/>
+      <c r="B44" s="259"/>
       <c r="C44" s="189"/>
       <c r="D44" s="37"/>
       <c r="E44" s="168"/>
       <c r="F44" s="187"/>
-      <c r="I44" s="265"/>
+      <c r="I44" s="259"/>
       <c r="J44" s="189"/>
       <c r="K44" s="37"/>
       <c r="L44" s="3"/>
@@ -9589,12 +9616,12 @@
       <c r="Z44" s="118"/>
     </row>
     <row r="45" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="265"/>
+      <c r="B45" s="259"/>
       <c r="C45" s="176"/>
       <c r="D45" s="37"/>
       <c r="E45" s="168"/>
       <c r="F45" s="187"/>
-      <c r="I45" s="265"/>
+      <c r="I45" s="259"/>
       <c r="J45" s="176"/>
       <c r="K45" s="37"/>
       <c r="L45" s="3"/>
@@ -9609,12 +9636,12 @@
       <c r="Z45" s="118"/>
     </row>
     <row r="46" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="265"/>
+      <c r="B46" s="259"/>
       <c r="C46" s="176"/>
       <c r="D46" s="37"/>
       <c r="E46" s="168"/>
       <c r="F46" s="187"/>
-      <c r="I46" s="265"/>
+      <c r="I46" s="259"/>
       <c r="J46" s="176"/>
       <c r="K46" s="37"/>
       <c r="L46" s="3"/>
@@ -9629,12 +9656,12 @@
       <c r="Z46" s="118"/>
     </row>
     <row r="47" spans="2:26" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="265"/>
+      <c r="B47" s="259"/>
       <c r="C47" s="165"/>
       <c r="D47" s="37"/>
       <c r="E47" s="168"/>
       <c r="F47" s="187"/>
-      <c r="I47" s="265"/>
+      <c r="I47" s="259"/>
       <c r="J47" s="154"/>
       <c r="K47" s="37"/>
       <c r="L47" s="3"/>
@@ -9649,15 +9676,15 @@
       <c r="Z47" s="118"/>
     </row>
     <row r="48" spans="2:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="266"/>
+      <c r="B48" s="260"/>
       <c r="C48" s="158" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="153">
         <f>SUM(D5:D47)</f>
-        <v>2534303.66</v>
-      </c>
-      <c r="I48" s="266"/>
+        <v>2602890.4400000004</v>
+      </c>
+      <c r="I48" s="260"/>
       <c r="J48" s="158" t="s">
         <v>3</v>
       </c>
@@ -9795,7 +9822,10 @@
       <c r="Z53" s="54"/>
     </row>
     <row r="54" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B54" s="64"/>
+      <c r="B54" s="295">
+        <f>D49+D50+D51+D52</f>
+        <v>-2796313.15</v>
+      </c>
       <c r="C54" s="121"/>
       <c r="D54" s="49"/>
       <c r="E54" s="191"/>
@@ -9836,7 +9866,7 @@
       </c>
       <c r="D56" s="192">
         <f>SUM(D48:D55)</f>
-        <v>-262009.48999999979</v>
+        <v>-193422.70999999953</v>
       </c>
       <c r="E56" s="202" t="s">
         <v>124</v>
@@ -10261,85 +10291,85 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="258" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="259" t="s">
+      <c r="B2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="259"/>
+      <c r="C2" s="261"/>
       <c r="D2" s="200" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="272" t="s">
+      <c r="F2" s="278" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="259" t="s">
+      <c r="G2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="259"/>
+      <c r="H2" s="261"/>
       <c r="I2" s="200" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="275" t="s">
+      <c r="K2" s="272" t="s">
         <v>121</v>
       </c>
-      <c r="L2" s="259" t="s">
+      <c r="L2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="259"/>
+      <c r="M2" s="261"/>
       <c r="N2" s="200" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="278" t="s">
+      <c r="P2" s="275" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" s="259" t="s">
+      <c r="Q2" s="261" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="259"/>
+      <c r="R2" s="261"/>
       <c r="S2" s="200" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="265"/>
+      <c r="A3" s="259"/>
       <c r="B3" s="232"/>
       <c r="C3" s="232"/>
       <c r="D3" s="233"/>
-      <c r="F3" s="273"/>
+      <c r="F3" s="279"/>
       <c r="G3" s="232"/>
       <c r="H3" s="232"/>
       <c r="I3" s="233"/>
-      <c r="K3" s="276"/>
+      <c r="K3" s="273"/>
       <c r="L3" s="232"/>
       <c r="M3" s="232"/>
       <c r="N3" s="233"/>
-      <c r="P3" s="279"/>
+      <c r="P3" s="276"/>
       <c r="Q3" s="232"/>
       <c r="R3" s="232"/>
       <c r="S3" s="233"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="265"/>
+      <c r="A4" s="259"/>
       <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="23"/>
-      <c r="F4" s="273"/>
+      <c r="F4" s="279"/>
       <c r="G4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="23"/>
-      <c r="K4" s="276"/>
+      <c r="K4" s="273"/>
       <c r="L4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="23"/>
-      <c r="P4" s="279"/>
+      <c r="P4" s="276"/>
       <c r="Q4" s="21" t="s">
         <v>2</v>
       </c>
@@ -10347,11 +10377,11 @@
       <c r="S4" s="23"/>
     </row>
     <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="265"/>
+      <c r="A5" s="259"/>
       <c r="B5" s="155"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
-      <c r="F5" s="273"/>
+      <c r="F5" s="279"/>
       <c r="G5" s="198">
         <v>45111</v>
       </c>
@@ -10361,7 +10391,7 @@
       <c r="I5" s="168" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="276"/>
+      <c r="K5" s="273"/>
       <c r="L5" s="198">
         <v>45106</v>
       </c>
@@ -10371,7 +10401,7 @@
       <c r="N5" s="201" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="279"/>
+      <c r="P5" s="276"/>
       <c r="Q5" s="198">
         <v>45091</v>
       </c>
@@ -10383,7 +10413,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="265"/>
+      <c r="A6" s="259"/>
       <c r="B6" s="197">
         <v>45086</v>
       </c>
@@ -10393,7 +10423,7 @@
       <c r="D6" s="168" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="273"/>
+      <c r="F6" s="279"/>
       <c r="G6" s="198">
         <v>45111</v>
       </c>
@@ -10403,7 +10433,7 @@
       <c r="I6" s="168" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="276"/>
+      <c r="K6" s="273"/>
       <c r="L6" s="198">
         <v>45111</v>
       </c>
@@ -10413,7 +10443,7 @@
       <c r="N6" s="223" t="s">
         <v>106</v>
       </c>
-      <c r="P6" s="279"/>
+      <c r="P6" s="276"/>
       <c r="Q6" s="198">
         <v>45134</v>
       </c>
@@ -10425,7 +10455,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="265"/>
+      <c r="A7" s="259"/>
       <c r="B7" s="197">
         <v>45090</v>
       </c>
@@ -10435,7 +10465,7 @@
       <c r="D7" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="273"/>
+      <c r="F7" s="279"/>
       <c r="G7" s="199">
         <v>45111</v>
       </c>
@@ -10445,7 +10475,7 @@
       <c r="I7" s="168" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="276"/>
+      <c r="K7" s="273"/>
       <c r="L7" s="199">
         <v>45139</v>
       </c>
@@ -10455,7 +10485,7 @@
       <c r="N7" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="P7" s="279"/>
+      <c r="P7" s="276"/>
       <c r="Q7" s="207">
         <v>45150</v>
       </c>
@@ -10467,7 +10497,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="265"/>
+      <c r="A8" s="259"/>
       <c r="B8" s="198">
         <v>45091</v>
       </c>
@@ -10477,7 +10507,7 @@
       <c r="D8" s="201" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="273"/>
+      <c r="F8" s="279"/>
       <c r="G8" s="199">
         <v>45120</v>
       </c>
@@ -10487,7 +10517,7 @@
       <c r="I8" s="168" t="s">
         <v>108</v>
       </c>
-      <c r="K8" s="276"/>
+      <c r="K8" s="273"/>
       <c r="L8" s="207">
         <v>45150</v>
       </c>
@@ -10497,13 +10527,13 @@
       <c r="N8" s="206" t="s">
         <v>128</v>
       </c>
-      <c r="P8" s="279"/>
+      <c r="P8" s="276"/>
       <c r="Q8" s="198"/>
       <c r="R8" s="37"/>
       <c r="S8" s="27"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="265"/>
+      <c r="A9" s="259"/>
       <c r="B9" s="199">
         <v>45129</v>
       </c>
@@ -10511,7 +10541,7 @@
         <v>100000</v>
       </c>
       <c r="D9" s="168"/>
-      <c r="F9" s="273"/>
+      <c r="F9" s="279"/>
       <c r="G9" s="212">
         <v>45136</v>
       </c>
@@ -10521,17 +10551,17 @@
       <c r="I9" s="204" t="s">
         <v>127</v>
       </c>
-      <c r="K9" s="276"/>
+      <c r="K9" s="273"/>
       <c r="L9" s="156"/>
       <c r="M9" s="77"/>
       <c r="N9" s="27"/>
-      <c r="P9" s="279"/>
+      <c r="P9" s="276"/>
       <c r="Q9" s="156"/>
       <c r="R9" s="77"/>
       <c r="S9" s="27"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="265"/>
+      <c r="A10" s="259"/>
       <c r="B10" s="205">
         <v>45136</v>
       </c>
@@ -10541,7 +10571,7 @@
       <c r="D10" s="204" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="273"/>
+      <c r="F10" s="279"/>
       <c r="G10" s="157">
         <v>45143</v>
       </c>
@@ -10549,21 +10579,21 @@
         <v>100000</v>
       </c>
       <c r="I10" s="27"/>
-      <c r="K10" s="276"/>
+      <c r="K10" s="273"/>
       <c r="L10" s="156"/>
       <c r="M10" s="77"/>
       <c r="N10" s="27"/>
-      <c r="P10" s="279"/>
+      <c r="P10" s="276"/>
       <c r="Q10" s="156"/>
       <c r="R10" s="77"/>
       <c r="S10" s="27"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="265"/>
+      <c r="A11" s="259"/>
       <c r="B11" s="199"/>
       <c r="C11" s="37"/>
       <c r="D11" s="168"/>
-      <c r="F11" s="273"/>
+      <c r="F11" s="279"/>
       <c r="G11" s="209">
         <v>45150</v>
       </c>
@@ -10573,107 +10603,107 @@
       <c r="I11" s="206" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="276"/>
+      <c r="K11" s="273"/>
       <c r="L11" s="156"/>
       <c r="M11" s="77"/>
       <c r="N11" s="27"/>
-      <c r="P11" s="279"/>
+      <c r="P11" s="276"/>
       <c r="Q11" s="156"/>
       <c r="R11" s="77"/>
       <c r="S11" s="27"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="265"/>
+      <c r="A12" s="259"/>
       <c r="B12" s="215"/>
       <c r="C12" s="97"/>
       <c r="D12" s="95"/>
-      <c r="F12" s="273"/>
+      <c r="F12" s="279"/>
       <c r="G12" s="157"/>
       <c r="H12" s="39"/>
       <c r="I12" s="146"/>
-      <c r="K12" s="276"/>
+      <c r="K12" s="273"/>
       <c r="L12" s="157"/>
       <c r="M12" s="39"/>
       <c r="N12" s="146"/>
-      <c r="P12" s="279"/>
+      <c r="P12" s="276"/>
       <c r="Q12" s="157"/>
       <c r="R12" s="39"/>
       <c r="S12" s="146"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="265"/>
+      <c r="A13" s="259"/>
       <c r="B13" s="155"/>
       <c r="C13" s="28"/>
       <c r="D13" s="10"/>
-      <c r="F13" s="273"/>
+      <c r="F13" s="279"/>
       <c r="G13" s="198"/>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
-      <c r="K13" s="276"/>
+      <c r="K13" s="273"/>
       <c r="L13" s="198"/>
       <c r="M13" s="37"/>
       <c r="N13" s="3"/>
-      <c r="P13" s="279"/>
+      <c r="P13" s="276"/>
       <c r="Q13" s="198"/>
       <c r="R13" s="37"/>
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="265"/>
+      <c r="A14" s="259"/>
       <c r="B14" s="197"/>
       <c r="C14" s="37"/>
       <c r="D14" s="3"/>
-      <c r="F14" s="273"/>
+      <c r="F14" s="279"/>
       <c r="G14" s="198"/>
       <c r="H14" s="37"/>
       <c r="I14" s="3"/>
-      <c r="K14" s="276"/>
+      <c r="K14" s="273"/>
       <c r="L14" s="198"/>
       <c r="M14" s="37"/>
       <c r="N14" s="3"/>
-      <c r="P14" s="279"/>
+      <c r="P14" s="276"/>
       <c r="Q14" s="198"/>
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="265"/>
+      <c r="A15" s="259"/>
       <c r="B15" s="197"/>
       <c r="C15" s="37"/>
       <c r="D15" s="3"/>
-      <c r="F15" s="273"/>
+      <c r="F15" s="279"/>
       <c r="G15" s="198"/>
       <c r="H15" s="37"/>
       <c r="I15" s="3"/>
-      <c r="K15" s="276"/>
+      <c r="K15" s="273"/>
       <c r="L15" s="198"/>
       <c r="M15" s="37"/>
       <c r="N15" s="3"/>
-      <c r="P15" s="279"/>
+      <c r="P15" s="276"/>
       <c r="Q15" s="198"/>
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="265"/>
+      <c r="A16" s="259"/>
       <c r="B16" s="197"/>
       <c r="C16" s="37">
         <v>0</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="F16" s="273"/>
+      <c r="F16" s="279"/>
       <c r="G16" s="198"/>
       <c r="H16" s="37">
         <v>0</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="K16" s="276"/>
+      <c r="K16" s="273"/>
       <c r="L16" s="198"/>
       <c r="M16" s="37">
         <v>0</v>
       </c>
       <c r="N16" s="3"/>
-      <c r="P16" s="279"/>
+      <c r="P16" s="276"/>
       <c r="Q16" s="198"/>
       <c r="R16" s="37">
         <v>0</v>
@@ -10681,7 +10711,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="265"/>
+      <c r="A17" s="259"/>
       <c r="B17" s="213" t="s">
         <v>3</v>
       </c>
@@ -10689,7 +10719,7 @@
         <f>SUM(C5:C16)</f>
         <v>495494.40000000002</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="279"/>
       <c r="G17" s="217" t="s">
         <v>3</v>
       </c>
@@ -10698,7 +10728,7 @@
         <v>219604.95</v>
       </c>
       <c r="I17" s="219"/>
-      <c r="K17" s="276"/>
+      <c r="K17" s="273"/>
       <c r="L17" s="217" t="s">
         <v>3</v>
       </c>
@@ -10707,7 +10737,7 @@
         <v>142859.95000000001</v>
       </c>
       <c r="N17" s="219"/>
-      <c r="P17" s="279"/>
+      <c r="P17" s="276"/>
       <c r="Q17" s="217" t="s">
         <v>3</v>
       </c>
@@ -10718,7 +10748,7 @@
       <c r="S17" s="219"/>
     </row>
     <row r="18" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="265"/>
+      <c r="A18" s="259"/>
       <c r="B18" s="220" t="s">
         <v>130</v>
       </c>
@@ -10728,7 +10758,7 @@
       <c r="D18" s="152">
         <v>45042</v>
       </c>
-      <c r="F18" s="273"/>
+      <c r="F18" s="279"/>
       <c r="G18" s="177"/>
       <c r="H18" s="55">
         <v>-219604.95</v>
@@ -10736,7 +10766,7 @@
       <c r="I18" s="221" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="276"/>
+      <c r="K18" s="273"/>
       <c r="L18" s="220" t="s">
         <v>130</v>
       </c>
@@ -10746,7 +10776,7 @@
       <c r="N18" s="216">
         <v>45120</v>
       </c>
-      <c r="P18" s="279"/>
+      <c r="P18" s="276"/>
       <c r="Q18" s="177" t="s">
         <v>131</v>
       </c>
@@ -10758,25 +10788,25 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="265"/>
+      <c r="A19" s="259"/>
       <c r="B19" s="162"/>
       <c r="C19" s="161">
         <v>0</v>
       </c>
       <c r="D19" s="124"/>
-      <c r="F19" s="273"/>
+      <c r="F19" s="279"/>
       <c r="G19" s="162"/>
       <c r="H19" s="161">
         <v>0</v>
       </c>
       <c r="I19" s="124"/>
-      <c r="K19" s="276"/>
+      <c r="K19" s="273"/>
       <c r="L19" s="162"/>
       <c r="M19" s="161">
         <v>0</v>
       </c>
       <c r="N19" s="124"/>
-      <c r="P19" s="279"/>
+      <c r="P19" s="276"/>
       <c r="Q19" s="162"/>
       <c r="R19" s="161">
         <v>0</v>
@@ -10784,29 +10814,29 @@
       <c r="S19" s="124"/>
     </row>
     <row r="20" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="265"/>
+      <c r="A20" s="259"/>
       <c r="B20" s="163"/>
       <c r="C20" s="164">
         <v>0</v>
       </c>
-      <c r="F20" s="273"/>
+      <c r="F20" s="279"/>
       <c r="G20" s="163"/>
       <c r="H20" s="164">
         <v>0</v>
       </c>
-      <c r="K20" s="276"/>
+      <c r="K20" s="273"/>
       <c r="L20" s="163"/>
       <c r="M20" s="164">
         <v>0</v>
       </c>
-      <c r="P20" s="279"/>
+      <c r="P20" s="276"/>
       <c r="Q20" s="163"/>
       <c r="R20" s="164">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="265"/>
+      <c r="A21" s="259"/>
       <c r="B21" s="33" t="s">
         <v>4</v>
       </c>
@@ -10814,7 +10844,7 @@
         <f>C20+C17+C18+C19</f>
         <v>0</v>
       </c>
-      <c r="F21" s="273"/>
+      <c r="F21" s="279"/>
       <c r="G21" s="33" t="s">
         <v>4</v>
       </c>
@@ -10822,7 +10852,7 @@
         <f>H20+H17+H18+H19</f>
         <v>0</v>
       </c>
-      <c r="K21" s="276"/>
+      <c r="K21" s="273"/>
       <c r="L21" s="33" t="s">
         <v>4</v>
       </c>
@@ -10830,7 +10860,7 @@
         <f>M20+M17+M18+M19</f>
         <v>0</v>
       </c>
-      <c r="P21" s="279"/>
+      <c r="P21" s="276"/>
       <c r="Q21" s="33" t="s">
         <v>4</v>
       </c>
@@ -10840,19 +10870,19 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="266"/>
+      <c r="A22" s="260"/>
       <c r="B22" s="182"/>
       <c r="C22" s="183"/>
       <c r="D22" s="118"/>
-      <c r="F22" s="274"/>
+      <c r="F22" s="280"/>
       <c r="G22" s="182"/>
       <c r="H22" s="183"/>
       <c r="I22" s="118"/>
-      <c r="K22" s="277"/>
+      <c r="K22" s="274"/>
       <c r="L22" s="182"/>
       <c r="M22" s="183"/>
       <c r="N22" s="118"/>
-      <c r="P22" s="280"/>
+      <c r="P22" s="277"/>
       <c r="Q22" s="182"/>
       <c r="R22" s="183"/>
       <c r="S22" s="118"/>
@@ -11006,18 +11036,18 @@
     <sortCondition ref="G5:G11"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F2:F22"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="K2:K22"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="P2:P22"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="A2:A22"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F2:F22"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12381,7 +12411,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="267" t="s">
+      <c r="B2" s="269" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="290" t="s">
@@ -12391,13 +12421,13 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="268"/>
+      <c r="B3" s="270"/>
       <c r="C3" s="232"/>
       <c r="D3" s="232"/>
       <c r="E3" s="233"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="269"/>
+      <c r="B4" s="271"/>
       <c r="C4" s="21" t="s">
         <v>2</v>
       </c>

</xml_diff>